<commit_message>
Top PSC / project.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/Platform/Aircraft/DoD_Aircraft_Contracts.xlsx
+++ b/Output/AcqTrends/Platform/Aircraft/DoD_Aircraft_Contracts.xlsx
@@ -11,12 +11,14 @@
     <sheet name="Price" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Veh" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="FYQ" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Proj" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="PSC" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t xml:space="preserve">SimpleArea</t>
   </si>
@@ -237,15 +239,93 @@
   <si>
     <t xml:space="preserve">Unlbd. IDV</t>
   </si>
+  <si>
+    <t xml:space="preserve">TopProject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLACK HAWK UPGRADE (UH-60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-17A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C130-J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-2C ADVANCED HAWKEYE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-16 FALCON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-18 HORNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F/A-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSF (F-35)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Labeled Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TopPStext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIRCRAFT, FIXED
+WING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIRCRAFT, ROTARY
+WING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIRFRAME STRUCTURAL
+COMPONENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEFENSE AIRCRAFT
+(OPERATIONAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAS TURBINES &amp; JET
+ENGINES AIRCRAFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAINT-REP OF
+AIRCRAFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAINT-REP OF
+AIRCRAFT COMPONENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISCELLANEOUS
+AIRCRAFT
+ACCESSORIES AND
+COMPONENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Labeled PSC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="167" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="168" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="173" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -281,11 +361,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8276,4 +8358,3606 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" xSplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="M2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="4" t="n">
+        <v>-3234412</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4" t="n">
+        <v>73612809</v>
+      </c>
+      <c r="S2" s="4" t="n">
+        <v>90611055</v>
+      </c>
+      <c r="T2" s="4" t="n">
+        <v>74947755.2194</v>
+      </c>
+      <c r="U2" s="4" t="n">
+        <v>23453739.4455</v>
+      </c>
+      <c r="V2" s="4" t="n">
+        <v>6267909.8805</v>
+      </c>
+      <c r="W2" s="4" t="n">
+        <v>5510614.2203</v>
+      </c>
+      <c r="X2" s="4" t="n">
+        <v>1035548.4999</v>
+      </c>
+      <c r="Y2" s="4" t="n">
+        <v>11809344.1849</v>
+      </c>
+      <c r="Z2" s="4" t="n">
+        <v>28246438.9313</v>
+      </c>
+      <c r="AA2" s="4" t="n">
+        <v>86620820.61</v>
+      </c>
+      <c r="AB2" s="4" t="n">
+        <v>19913017.3088</v>
+      </c>
+      <c r="AC2" s="4" t="n">
+        <v>232573623.6527</v>
+      </c>
+      <c r="AD2" s="4" t="n">
+        <v>439569602.0377</v>
+      </c>
+      <c r="AE2" s="4" t="n">
+        <v>733587271.8843</v>
+      </c>
+      <c r="AF2" s="4" t="n">
+        <v>1034906369.0508</v>
+      </c>
+      <c r="AG2" s="4" t="n">
+        <v>1029685688.0731</v>
+      </c>
+      <c r="AH2" s="4" t="n">
+        <v>1001596419.4928</v>
+      </c>
+      <c r="AI2" s="4" t="n">
+        <v>374208744.9589</v>
+      </c>
+      <c r="AJ2" s="4" t="n">
+        <v>565892101.5908</v>
+      </c>
+      <c r="AK2" s="4" t="n">
+        <v>259434051.2607</v>
+      </c>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" s="4" t="n">
+        <v>-4746228</v>
+      </c>
+      <c r="O3" s="4" t="n">
+        <v>-682672</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <v>23465356</v>
+      </c>
+      <c r="Q3" s="4" t="n">
+        <v>410914152</v>
+      </c>
+      <c r="R3" s="4" t="n">
+        <v>1260351400</v>
+      </c>
+      <c r="S3" s="4" t="n">
+        <v>1498226510</v>
+      </c>
+      <c r="T3" s="4" t="n">
+        <v>1951248339.18</v>
+      </c>
+      <c r="U3" s="4" t="n">
+        <v>3382381505.9866</v>
+      </c>
+      <c r="V3" s="4" t="n">
+        <v>2302232938.43</v>
+      </c>
+      <c r="W3" s="4" t="n">
+        <v>3937748293.865</v>
+      </c>
+      <c r="X3" s="4" t="n">
+        <v>3573248169.1858</v>
+      </c>
+      <c r="Y3" s="4" t="n">
+        <v>3527392217.612</v>
+      </c>
+      <c r="Z3" s="4" t="n">
+        <v>5502691461.6038</v>
+      </c>
+      <c r="AA3" s="4" t="n">
+        <v>1961143068.6485</v>
+      </c>
+      <c r="AB3" s="4" t="n">
+        <v>1617412327.4719</v>
+      </c>
+      <c r="AC3" s="4" t="n">
+        <v>875152105.078</v>
+      </c>
+      <c r="AD3" s="4" t="n">
+        <v>909691071.9537</v>
+      </c>
+      <c r="AE3" s="4" t="n">
+        <v>442827955.5559</v>
+      </c>
+      <c r="AF3" s="4" t="n">
+        <v>-16157042.1038</v>
+      </c>
+      <c r="AG3" s="4" t="n">
+        <v>-20086034.8218</v>
+      </c>
+      <c r="AH3" s="4" t="n">
+        <v>-47143500.1464</v>
+      </c>
+      <c r="AI3" s="4" t="n">
+        <v>-19881262.1299</v>
+      </c>
+      <c r="AJ3" s="4" t="n">
+        <v>27525142.1679</v>
+      </c>
+      <c r="AK3" s="4" t="n">
+        <v>426761.7573</v>
+      </c>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="M4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4" t="n">
+        <v>1899047</v>
+      </c>
+      <c r="R4" s="4" t="n">
+        <v>272575241</v>
+      </c>
+      <c r="S4" s="4" t="n">
+        <v>71582203</v>
+      </c>
+      <c r="T4" s="4" t="n">
+        <v>328393706</v>
+      </c>
+      <c r="U4" s="4" t="n">
+        <v>885464060.4574</v>
+      </c>
+      <c r="V4" s="4" t="n">
+        <v>1147089320.3728</v>
+      </c>
+      <c r="W4" s="4" t="n">
+        <v>801967764.4411</v>
+      </c>
+      <c r="X4" s="4" t="n">
+        <v>2923438276.2024</v>
+      </c>
+      <c r="Y4" s="4" t="n">
+        <v>3187537219.3051</v>
+      </c>
+      <c r="Z4" s="4" t="n">
+        <v>835521755.2762</v>
+      </c>
+      <c r="AA4" s="4" t="n">
+        <v>1208448663.1719</v>
+      </c>
+      <c r="AB4" s="4" t="n">
+        <v>2337976019.9025</v>
+      </c>
+      <c r="AC4" s="4" t="n">
+        <v>1463451495.9049</v>
+      </c>
+      <c r="AD4" s="4" t="n">
+        <v>5565212122.7758</v>
+      </c>
+      <c r="AE4" s="4" t="n">
+        <v>1659661667.8094</v>
+      </c>
+      <c r="AF4" s="4" t="n">
+        <v>1879935442.4908</v>
+      </c>
+      <c r="AG4" s="4" t="n">
+        <v>1889634750.5089</v>
+      </c>
+      <c r="AH4" s="4" t="n">
+        <v>3317526634.0356</v>
+      </c>
+      <c r="AI4" s="4" t="n">
+        <v>2462269136.3324</v>
+      </c>
+      <c r="AJ4" s="4" t="n">
+        <v>1283396519.7133</v>
+      </c>
+      <c r="AK4" s="4" t="n">
+        <v>1889699500.0695</v>
+      </c>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="M5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4" t="n">
+        <v>31922676</v>
+      </c>
+      <c r="S5" s="4" t="n">
+        <v>9021325</v>
+      </c>
+      <c r="T5" s="4" t="n">
+        <v>8609902</v>
+      </c>
+      <c r="U5" s="4" t="n">
+        <v>16126338</v>
+      </c>
+      <c r="V5" s="4" t="n">
+        <v>78672314.4727</v>
+      </c>
+      <c r="W5" s="4" t="n">
+        <v>467055106.2578</v>
+      </c>
+      <c r="X5" s="4" t="n">
+        <v>592060550.8711</v>
+      </c>
+      <c r="Y5" s="4" t="n">
+        <v>980124725.6754</v>
+      </c>
+      <c r="Z5" s="4" t="n">
+        <v>929401740.8428</v>
+      </c>
+      <c r="AA5" s="4" t="n">
+        <v>911944892.8</v>
+      </c>
+      <c r="AB5" s="4" t="n">
+        <v>955386251.5873</v>
+      </c>
+      <c r="AC5" s="4" t="n">
+        <v>987593268.9567</v>
+      </c>
+      <c r="AD5" s="4" t="n">
+        <v>1555534675.9832</v>
+      </c>
+      <c r="AE5" s="4" t="n">
+        <v>1067444154.4554</v>
+      </c>
+      <c r="AF5" s="4" t="n">
+        <v>1148246182.1916</v>
+      </c>
+      <c r="AG5" s="4" t="n">
+        <v>2764551250.0166</v>
+      </c>
+      <c r="AH5" s="4" t="n">
+        <v>1355906322.1603</v>
+      </c>
+      <c r="AI5" s="4" t="n">
+        <v>1087992070.5099</v>
+      </c>
+      <c r="AJ5" s="4" t="n">
+        <v>1287275822.408</v>
+      </c>
+      <c r="AK5" s="4" t="n">
+        <v>815038578.7023</v>
+      </c>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="M6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="4" t="n">
+        <v>649457506</v>
+      </c>
+      <c r="O6" s="4" t="n">
+        <v>642274963</v>
+      </c>
+      <c r="P6" s="4" t="n">
+        <v>784026790</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>768163207.5</v>
+      </c>
+      <c r="R6" s="4" t="n">
+        <v>155275786</v>
+      </c>
+      <c r="S6" s="4" t="n">
+        <v>116116565.5039</v>
+      </c>
+      <c r="T6" s="4" t="n">
+        <v>57910655</v>
+      </c>
+      <c r="U6" s="4" t="n">
+        <v>62605640.8496</v>
+      </c>
+      <c r="V6" s="4" t="n">
+        <v>3292285.4073</v>
+      </c>
+      <c r="W6" s="4" t="n">
+        <v>-1609620.8091</v>
+      </c>
+      <c r="X6" s="4" t="n">
+        <v>-2137806.4023</v>
+      </c>
+      <c r="Y6" s="4" t="n">
+        <v>-1691420.8099</v>
+      </c>
+      <c r="Z6" s="4" t="n">
+        <v>-2715816.0779</v>
+      </c>
+      <c r="AA6" s="4" t="n">
+        <v>-3190666.52</v>
+      </c>
+      <c r="AB6" s="4" t="n">
+        <v>-1031433.31</v>
+      </c>
+      <c r="AC6" s="4" t="n">
+        <v>-177369.95</v>
+      </c>
+      <c r="AD6" s="4" t="n">
+        <v>-826608.68</v>
+      </c>
+      <c r="AE6" s="4" t="n">
+        <v>-9135232.1963</v>
+      </c>
+      <c r="AF6" s="4" t="n">
+        <v>-128368.3477</v>
+      </c>
+      <c r="AG6" s="4" t="n">
+        <v>5493</v>
+      </c>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="M7" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <v>940923016</v>
+      </c>
+      <c r="O7" s="4" t="n">
+        <v>725487899</v>
+      </c>
+      <c r="P7" s="4" t="n">
+        <v>953275644</v>
+      </c>
+      <c r="Q7" s="4" t="n">
+        <v>1123830103</v>
+      </c>
+      <c r="R7" s="4" t="n">
+        <v>10557</v>
+      </c>
+      <c r="S7" s="4" t="n">
+        <v>239000</v>
+      </c>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4" t="n">
+        <v>-103704</v>
+      </c>
+      <c r="W7" s="4" t="n">
+        <v>-1643756.0938</v>
+      </c>
+      <c r="X7" s="4" t="n">
+        <v>-4330797.0375</v>
+      </c>
+      <c r="Y7" s="4" t="n">
+        <v>-477952.8633</v>
+      </c>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="4" t="n">
+        <v>-92500</v>
+      </c>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="M8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4" t="n">
+        <v>278982781</v>
+      </c>
+      <c r="R8" s="4" t="n">
+        <v>4247084514</v>
+      </c>
+      <c r="S8" s="4" t="n">
+        <v>2172292783</v>
+      </c>
+      <c r="T8" s="4" t="n">
+        <v>4940293889</v>
+      </c>
+      <c r="U8" s="4" t="n">
+        <v>6408106023.9843</v>
+      </c>
+      <c r="V8" s="4" t="n">
+        <v>4584560934.3672</v>
+      </c>
+      <c r="W8" s="4" t="n">
+        <v>4441826618.0391</v>
+      </c>
+      <c r="X8" s="4" t="n">
+        <v>2352786706.3597</v>
+      </c>
+      <c r="Y8" s="4" t="n">
+        <v>2195560560.3017</v>
+      </c>
+      <c r="Z8" s="4" t="n">
+        <v>1663615021.229</v>
+      </c>
+      <c r="AA8" s="4" t="n">
+        <v>1469701276.01</v>
+      </c>
+      <c r="AB8" s="4" t="n">
+        <v>1438385977.71</v>
+      </c>
+      <c r="AC8" s="4" t="n">
+        <v>1447816626.26</v>
+      </c>
+      <c r="AD8" s="4" t="n">
+        <v>1446423801.8031</v>
+      </c>
+      <c r="AE8" s="4" t="n">
+        <v>1806072185.7753</v>
+      </c>
+      <c r="AF8" s="4" t="n">
+        <v>42357732.0332</v>
+      </c>
+      <c r="AG8" s="4" t="n">
+        <v>-11584522.9001</v>
+      </c>
+      <c r="AH8" s="4" t="n">
+        <v>-17170445.5487</v>
+      </c>
+      <c r="AI8" s="4" t="n">
+        <v>2722228.418</v>
+      </c>
+      <c r="AJ8" s="4" t="n">
+        <v>-24005672.7453</v>
+      </c>
+      <c r="AK8" s="4" t="n">
+        <v>71078802</v>
+      </c>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="M9" t="s">
+        <v>81</v>
+      </c>
+      <c r="N9" s="4" t="n">
+        <v>178031456</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <v>268635741</v>
+      </c>
+      <c r="P9" s="4" t="n">
+        <v>6554622</v>
+      </c>
+      <c r="Q9" s="4" t="n">
+        <v>239927692</v>
+      </c>
+      <c r="R9" s="4" t="n">
+        <v>196592861.0938</v>
+      </c>
+      <c r="S9" s="4" t="n">
+        <v>298929304</v>
+      </c>
+      <c r="T9" s="4" t="n">
+        <v>634208169</v>
+      </c>
+      <c r="U9" s="4" t="n">
+        <v>1065880921.7227</v>
+      </c>
+      <c r="V9" s="4" t="n">
+        <v>2731035654.3702</v>
+      </c>
+      <c r="W9" s="4" t="n">
+        <v>3691756626.1371</v>
+      </c>
+      <c r="X9" s="4" t="n">
+        <v>1874970548.0441</v>
+      </c>
+      <c r="Y9" s="4" t="n">
+        <v>4876760172.575</v>
+      </c>
+      <c r="Z9" s="4" t="n">
+        <v>4703656860.9744</v>
+      </c>
+      <c r="AA9" s="4" t="n">
+        <v>12188274857.38</v>
+      </c>
+      <c r="AB9" s="4" t="n">
+        <v>3808932854.26</v>
+      </c>
+      <c r="AC9" s="4" t="n">
+        <v>11390479946.9339</v>
+      </c>
+      <c r="AD9" s="4" t="n">
+        <v>10166002384.5202</v>
+      </c>
+      <c r="AE9" s="4" t="n">
+        <v>24142780609.3471</v>
+      </c>
+      <c r="AF9" s="4" t="n">
+        <v>15994084688.9169</v>
+      </c>
+      <c r="AG9" s="4" t="n">
+        <v>17159190678.1875</v>
+      </c>
+      <c r="AH9" s="4" t="n">
+        <v>35953318555.1719</v>
+      </c>
+      <c r="AI9" s="4" t="n">
+        <v>9805187787.8331</v>
+      </c>
+      <c r="AJ9" s="4" t="n">
+        <v>20754154100.2067</v>
+      </c>
+      <c r="AK9" s="4" t="n">
+        <v>26856373541.1332</v>
+      </c>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="M10" t="s">
+        <v>82</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4" t="n">
+        <v>44877606</v>
+      </c>
+      <c r="S10" s="4" t="n">
+        <v>434557003</v>
+      </c>
+      <c r="T10" s="4" t="n">
+        <v>871521962</v>
+      </c>
+      <c r="U10" s="4" t="n">
+        <v>1073009382</v>
+      </c>
+      <c r="V10" s="4" t="n">
+        <v>783627139</v>
+      </c>
+      <c r="W10" s="4" t="n">
+        <v>1088710802.375</v>
+      </c>
+      <c r="X10" s="4" t="n">
+        <v>1281857793</v>
+      </c>
+      <c r="Y10" s="4" t="n">
+        <v>3027110789.6402</v>
+      </c>
+      <c r="Z10" s="4" t="n">
+        <v>3765412842.0601</v>
+      </c>
+      <c r="AA10" s="4" t="n">
+        <v>751308114.3</v>
+      </c>
+      <c r="AB10" s="4" t="n">
+        <v>850821379.74</v>
+      </c>
+      <c r="AC10" s="4" t="n">
+        <v>1758872527.909</v>
+      </c>
+      <c r="AD10" s="4" t="n">
+        <v>3492411209.718</v>
+      </c>
+      <c r="AE10" s="4" t="n">
+        <v>2821282548.3477</v>
+      </c>
+      <c r="AF10" s="4" t="n">
+        <v>2755575563.4591</v>
+      </c>
+      <c r="AG10" s="4" t="n">
+        <v>3882372006.5527</v>
+      </c>
+      <c r="AH10" s="4" t="n">
+        <v>2790636103.0426</v>
+      </c>
+      <c r="AI10" s="4" t="n">
+        <v>2635487049.2397</v>
+      </c>
+      <c r="AJ10" s="4" t="n">
+        <v>589031561.3532</v>
+      </c>
+      <c r="AK10" s="4" t="n">
+        <v>460936960.1566</v>
+      </c>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="M11" t="s">
+        <v>83</v>
+      </c>
+      <c r="N11" s="4" t="n">
+        <v>15808115106</v>
+      </c>
+      <c r="O11" s="4" t="n">
+        <v>15558061149</v>
+      </c>
+      <c r="P11" s="4" t="n">
+        <v>13884028147</v>
+      </c>
+      <c r="Q11" s="4" t="n">
+        <v>18954837569</v>
+      </c>
+      <c r="R11" s="4" t="n">
+        <v>4680864206.7391</v>
+      </c>
+      <c r="S11" s="4" t="n">
+        <v>7351632031.0235</v>
+      </c>
+      <c r="T11" s="4" t="n">
+        <v>8113420304.2091</v>
+      </c>
+      <c r="U11" s="4" t="n">
+        <v>11981029562.1725</v>
+      </c>
+      <c r="V11" s="4" t="n">
+        <v>16502909261.2491</v>
+      </c>
+      <c r="W11" s="4" t="n">
+        <v>16080070092.0397</v>
+      </c>
+      <c r="X11" s="4" t="n">
+        <v>17369956178.8314</v>
+      </c>
+      <c r="Y11" s="4" t="n">
+        <v>18906739434.9168</v>
+      </c>
+      <c r="Z11" s="4" t="n">
+        <v>21680351228.2259</v>
+      </c>
+      <c r="AA11" s="4" t="n">
+        <v>23652612320.2784</v>
+      </c>
+      <c r="AB11" s="4" t="n">
+        <v>19441537010.9345</v>
+      </c>
+      <c r="AC11" s="4" t="n">
+        <v>10679170634.9752</v>
+      </c>
+      <c r="AD11" s="4" t="n">
+        <v>14476597584.7523</v>
+      </c>
+      <c r="AE11" s="4" t="n">
+        <v>12843586933.5628</v>
+      </c>
+      <c r="AF11" s="4" t="n">
+        <v>13121867089.1534</v>
+      </c>
+      <c r="AG11" s="4" t="n">
+        <v>12528605899.2539</v>
+      </c>
+      <c r="AH11" s="4" t="n">
+        <v>8442705529.0752</v>
+      </c>
+      <c r="AI11" s="4" t="n">
+        <v>12504596812.7733</v>
+      </c>
+      <c r="AJ11" s="4" t="n">
+        <v>11917196075.6053</v>
+      </c>
+      <c r="AK11" s="4" t="n">
+        <v>8083669105.2669</v>
+      </c>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="M12" t="s">
+        <v>84</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4" t="n">
+        <v>217356961</v>
+      </c>
+      <c r="S12" s="4" t="n">
+        <v>1283300356</v>
+      </c>
+      <c r="T12" s="4" t="n">
+        <v>1206031696</v>
+      </c>
+      <c r="U12" s="4" t="n">
+        <v>1982775910.3563</v>
+      </c>
+      <c r="V12" s="4" t="n">
+        <v>2892461437.0703</v>
+      </c>
+      <c r="W12" s="4" t="n">
+        <v>2905749060.6262</v>
+      </c>
+      <c r="X12" s="4" t="n">
+        <v>3009617963.4144</v>
+      </c>
+      <c r="Y12" s="4" t="n">
+        <v>2933479559.2798</v>
+      </c>
+      <c r="Z12" s="4" t="n">
+        <v>3026050188.1968</v>
+      </c>
+      <c r="AA12" s="4" t="n">
+        <v>2126739059.26</v>
+      </c>
+      <c r="AB12" s="4" t="n">
+        <v>2171014786.2606</v>
+      </c>
+      <c r="AC12" s="4" t="n">
+        <v>2116717995.2878</v>
+      </c>
+      <c r="AD12" s="4" t="n">
+        <v>2240521439.5375</v>
+      </c>
+      <c r="AE12" s="4" t="n">
+        <v>2394172267.8088</v>
+      </c>
+      <c r="AF12" s="4" t="n">
+        <v>2496146679.9583</v>
+      </c>
+      <c r="AG12" s="4" t="n">
+        <v>1848018802.377</v>
+      </c>
+      <c r="AH12" s="4" t="n">
+        <v>1970407916.9383</v>
+      </c>
+      <c r="AI12" s="4" t="n">
+        <v>2102295787.8397</v>
+      </c>
+      <c r="AJ12" s="4" t="n">
+        <v>1590750685.0735</v>
+      </c>
+      <c r="AK12" s="4" t="n">
+        <v>843475451.2461</v>
+      </c>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="M13"/>
+      <c r="N13" s="4" t="n">
+        <v>17851791620.53</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <v>18928068967.9394</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>23374539002.1662</v>
+      </c>
+      <c r="Q13" s="4" t="n">
+        <v>27466465634.9567</v>
+      </c>
+      <c r="R13" s="4" t="n">
+        <v>36621601947.1452</v>
+      </c>
+      <c r="S13" s="4" t="n">
+        <v>33956090591.5561</v>
+      </c>
+      <c r="T13" s="4" t="n">
+        <v>35786391603.6723</v>
+      </c>
+      <c r="U13" s="4" t="n">
+        <v>33601097757.7611</v>
+      </c>
+      <c r="V13" s="4" t="n">
+        <v>35694689979.2755</v>
+      </c>
+      <c r="W13" s="4" t="n">
+        <v>32432508215.492</v>
+      </c>
+      <c r="X13" s="4" t="n">
+        <v>30630087808.0251</v>
+      </c>
+      <c r="Y13" s="4" t="n">
+        <v>30658449243.4073</v>
+      </c>
+      <c r="Z13" s="4" t="n">
+        <v>36031876920.4268</v>
+      </c>
+      <c r="AA13" s="4" t="n">
+        <v>28905105883.431</v>
+      </c>
+      <c r="AB13" s="4" t="n">
+        <v>25582095085.2758</v>
+      </c>
+      <c r="AC13" s="4" t="n">
+        <v>30741509217.2039</v>
+      </c>
+      <c r="AD13" s="4" t="n">
+        <v>35055003338.3831</v>
+      </c>
+      <c r="AE13" s="4" t="n">
+        <v>37920266007.3768</v>
+      </c>
+      <c r="AF13" s="4" t="n">
+        <v>44881946837.6313</v>
+      </c>
+      <c r="AG13" s="4" t="n">
+        <v>49017389369.1594</v>
+      </c>
+      <c r="AH13" s="4" t="n">
+        <v>50542746879.7162</v>
+      </c>
+      <c r="AI13" s="4" t="n">
+        <v>41539920169.8764</v>
+      </c>
+      <c r="AJ13" s="4" t="n">
+        <v>37139289470.8574</v>
+      </c>
+      <c r="AK13" s="4" t="n">
+        <v>25008178517.9099</v>
+      </c>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="4"/>
+    </row>
+    <row r="17">
+      <c r="M17" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S17" t="s">
+        <v>16</v>
+      </c>
+      <c r="T17" t="s">
+        <v>17</v>
+      </c>
+      <c r="U17" t="s">
+        <v>18</v>
+      </c>
+      <c r="V17" t="s">
+        <v>19</v>
+      </c>
+      <c r="W17" t="s">
+        <v>20</v>
+      </c>
+      <c r="X17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="M18" t="s">
+        <v>74</v>
+      </c>
+      <c r="N18" s="4" t="n">
+        <v>-5225936.661734</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4" t="n">
+        <v>109497531.713989</v>
+      </c>
+      <c r="S18" s="4" t="n">
+        <v>130811075.978186</v>
+      </c>
+      <c r="T18" s="4" t="n">
+        <v>104787063.505414</v>
+      </c>
+      <c r="U18" s="4" t="n">
+        <v>31916246.0356545</v>
+      </c>
+      <c r="V18" s="4" t="n">
+        <v>8355222.72600043</v>
+      </c>
+      <c r="W18" s="4" t="n">
+        <v>7271839.5597748</v>
+      </c>
+      <c r="X18" s="4" t="n">
+        <v>1354733.24892151</v>
+      </c>
+      <c r="Y18" s="4" t="n">
+        <v>15144100.9421999</v>
+      </c>
+      <c r="Z18" s="4" t="n">
+        <v>35570740.5393992</v>
+      </c>
+      <c r="AA18" s="4" t="n">
+        <v>107121279.923087</v>
+      </c>
+      <c r="AB18" s="4" t="n">
+        <v>24158441.9096011</v>
+      </c>
+      <c r="AC18" s="4" t="n">
+        <v>278959867.056182</v>
+      </c>
+      <c r="AD18" s="4" t="n">
+        <v>522907613.971075</v>
+      </c>
+      <c r="AE18" s="4" t="n">
+        <v>857360976.282733</v>
+      </c>
+      <c r="AF18" s="4" t="n">
+        <v>1181771482.05595</v>
+      </c>
+      <c r="AG18" s="4" t="n">
+        <v>1153222329.43531</v>
+      </c>
+      <c r="AH18" s="4" t="n">
+        <v>1106995235.87468</v>
+      </c>
+      <c r="AI18" s="4" t="n">
+        <v>400136768.896741</v>
+      </c>
+      <c r="AJ18" s="4" t="n">
+        <v>565892101.5908</v>
+      </c>
+      <c r="AK18" s="4" t="n">
+        <v>247447777.662795</v>
+      </c>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="4"/>
+    </row>
+    <row r="19">
+      <c r="M19" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19" s="4" t="n">
+        <v>-7668623.20265583</v>
+      </c>
+      <c r="O19" s="4" t="n">
+        <v>-1076899.47398204</v>
+      </c>
+      <c r="P19" s="4" t="n">
+        <v>36440896.3012542</v>
+      </c>
+      <c r="Q19" s="4" t="n">
+        <v>626166737.488577</v>
+      </c>
+      <c r="R19" s="4" t="n">
+        <v>1874746654.38009</v>
+      </c>
+      <c r="S19" s="4" t="n">
+        <v>2162921752.01075</v>
+      </c>
+      <c r="T19" s="4" t="n">
+        <v>2728108173.93985</v>
+      </c>
+      <c r="U19" s="4" t="n">
+        <v>4602802064.13858</v>
+      </c>
+      <c r="V19" s="4" t="n">
+        <v>3068912816.94411</v>
+      </c>
+      <c r="W19" s="4" t="n">
+        <v>5196276254.33818</v>
+      </c>
+      <c r="X19" s="4" t="n">
+        <v>4674622291.38604</v>
+      </c>
+      <c r="Y19" s="4" t="n">
+        <v>4523467431.37108</v>
+      </c>
+      <c r="Z19" s="4" t="n">
+        <v>6929539356.27551</v>
+      </c>
+      <c r="AA19" s="4" t="n">
+        <v>2425284754.24838</v>
+      </c>
+      <c r="AB19" s="4" t="n">
+        <v>1962242142.97423</v>
+      </c>
+      <c r="AC19" s="4" t="n">
+        <v>1049699063.25688</v>
+      </c>
+      <c r="AD19" s="4" t="n">
+        <v>1082159425.22181</v>
+      </c>
+      <c r="AE19" s="4" t="n">
+        <v>517543614.579743</v>
+      </c>
+      <c r="AF19" s="4" t="n">
+        <v>-18449912.1501792</v>
+      </c>
+      <c r="AG19" s="4" t="n">
+        <v>-22495858.8184927</v>
+      </c>
+      <c r="AH19" s="4" t="n">
+        <v>-52104449.5056697</v>
+      </c>
+      <c r="AI19" s="4" t="n">
+        <v>-21258786.9669402</v>
+      </c>
+      <c r="AJ19" s="4" t="n">
+        <v>27525142.1679</v>
+      </c>
+      <c r="AK19" s="4" t="n">
+        <v>407044.672517709</v>
+      </c>
+      <c r="AL19" s="4"/>
+      <c r="AM19" s="4"/>
+    </row>
+    <row r="20">
+      <c r="M20" t="s">
+        <v>76</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4" t="n">
+        <v>2893840.61984672</v>
+      </c>
+      <c r="R20" s="4" t="n">
+        <v>405450036.499024</v>
+      </c>
+      <c r="S20" s="4" t="n">
+        <v>103339984.236128</v>
+      </c>
+      <c r="T20" s="4" t="n">
+        <v>459138662.988174</v>
+      </c>
+      <c r="U20" s="4" t="n">
+        <v>1204954496.70011</v>
+      </c>
+      <c r="V20" s="4" t="n">
+        <v>1529088155.55061</v>
+      </c>
+      <c r="W20" s="4" t="n">
+        <v>1058281469.53997</v>
+      </c>
+      <c r="X20" s="4" t="n">
+        <v>3824522979.19762</v>
+      </c>
+      <c r="Y20" s="4" t="n">
+        <v>4087643195.96164</v>
+      </c>
+      <c r="Z20" s="4" t="n">
+        <v>1052172546.21856</v>
+      </c>
+      <c r="AA20" s="4" t="n">
+        <v>1494450948.49832</v>
+      </c>
+      <c r="AB20" s="4" t="n">
+        <v>2836428904.11662</v>
+      </c>
+      <c r="AC20" s="4" t="n">
+        <v>1755333336.29625</v>
+      </c>
+      <c r="AD20" s="4" t="n">
+        <v>6620320829.45083</v>
+      </c>
+      <c r="AE20" s="4" t="n">
+        <v>1939686254.58447</v>
+      </c>
+      <c r="AF20" s="4" t="n">
+        <v>2146719897.06618</v>
+      </c>
+      <c r="AG20" s="4" t="n">
+        <v>2116343864.93394</v>
+      </c>
+      <c r="AH20" s="4" t="n">
+        <v>3666632694.85777</v>
+      </c>
+      <c r="AI20" s="4" t="n">
+        <v>2632873842.84519</v>
+      </c>
+      <c r="AJ20" s="4" t="n">
+        <v>1283396519.7133</v>
+      </c>
+      <c r="AK20" s="4" t="n">
+        <v>1802392320.78602</v>
+      </c>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="4"/>
+    </row>
+    <row r="21">
+      <c r="M21" t="s">
+        <v>77</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4" t="n">
+        <v>47484320.6663312</v>
+      </c>
+      <c r="S21" s="4" t="n">
+        <v>13023678.2917814</v>
+      </c>
+      <c r="T21" s="4" t="n">
+        <v>12037803.4673393</v>
+      </c>
+      <c r="U21" s="4" t="n">
+        <v>21944993.993735</v>
+      </c>
+      <c r="V21" s="4" t="n">
+        <v>104871435.984482</v>
+      </c>
+      <c r="W21" s="4" t="n">
+        <v>616328718.08896</v>
+      </c>
+      <c r="X21" s="4" t="n">
+        <v>774550022.251318</v>
+      </c>
+      <c r="Y21" s="4" t="n">
+        <v>1256895179.71314</v>
+      </c>
+      <c r="Z21" s="4" t="n">
+        <v>1170395612.02003</v>
+      </c>
+      <c r="AA21" s="4" t="n">
+        <v>1127773939.89246</v>
+      </c>
+      <c r="AB21" s="4" t="n">
+        <v>1159073128.00875</v>
+      </c>
+      <c r="AC21" s="4" t="n">
+        <v>1184566343.71033</v>
+      </c>
+      <c r="AD21" s="4" t="n">
+        <v>1850448534.42319</v>
+      </c>
+      <c r="AE21" s="4" t="n">
+        <v>1247547493.62053</v>
+      </c>
+      <c r="AF21" s="4" t="n">
+        <v>1311195517.84984</v>
+      </c>
+      <c r="AG21" s="4" t="n">
+        <v>3096228557.23436</v>
+      </c>
+      <c r="AH21" s="4" t="n">
+        <v>1498589461.49578</v>
+      </c>
+      <c r="AI21" s="4" t="n">
+        <v>1163376424.37224</v>
+      </c>
+      <c r="AJ21" s="4" t="n">
+        <v>1287275822.408</v>
+      </c>
+      <c r="AK21" s="4" t="n">
+        <v>777382475.54352</v>
+      </c>
+      <c r="AL21" s="4"/>
+      <c r="AM21" s="4"/>
+    </row>
+    <row r="22">
+      <c r="M22" t="s">
+        <v>78</v>
+      </c>
+      <c r="N22" s="4" t="n">
+        <v>1049348008.49234</v>
+      </c>
+      <c r="O22" s="4" t="n">
+        <v>1013174071.59886</v>
+      </c>
+      <c r="P22" s="4" t="n">
+        <v>1217566822.8428</v>
+      </c>
+      <c r="Q22" s="4" t="n">
+        <v>1170556543.64281</v>
+      </c>
+      <c r="R22" s="4" t="n">
+        <v>230969521.920425</v>
+      </c>
+      <c r="S22" s="4" t="n">
+        <v>167632226.249398</v>
+      </c>
+      <c r="T22" s="4" t="n">
+        <v>80966901.0814398</v>
+      </c>
+      <c r="U22" s="4" t="n">
+        <v>85194816.8529275</v>
+      </c>
+      <c r="V22" s="4" t="n">
+        <v>4388668.37271091</v>
+      </c>
+      <c r="W22" s="4" t="n">
+        <v>-2124065.26893709</v>
+      </c>
+      <c r="X22" s="4" t="n">
+        <v>-2796737.58711712</v>
+      </c>
+      <c r="Y22" s="4" t="n">
+        <v>-2169049.10889258</v>
+      </c>
+      <c r="Z22" s="4" t="n">
+        <v>-3420027.18624693</v>
+      </c>
+      <c r="AA22" s="4" t="n">
+        <v>-3945798.23907467</v>
+      </c>
+      <c r="AB22" s="4" t="n">
+        <v>-1251333.30207325</v>
+      </c>
+      <c r="AC22" s="4" t="n">
+        <v>-212745.954999817</v>
+      </c>
+      <c r="AD22" s="4" t="n">
+        <v>-983325.440482822</v>
+      </c>
+      <c r="AE22" s="4" t="n">
+        <v>-10676564.1861143</v>
+      </c>
+      <c r="AF22" s="4" t="n">
+        <v>-146585.292203431</v>
+      </c>
+      <c r="AG22" s="4" t="n">
+        <v>6152.02321345506</v>
+      </c>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="4"/>
+      <c r="AL22" s="4"/>
+      <c r="AM22" s="4"/>
+    </row>
+    <row r="23">
+      <c r="M23" t="s">
+        <v>79</v>
+      </c>
+      <c r="N23" s="4" t="n">
+        <v>1520277591.47064</v>
+      </c>
+      <c r="O23" s="4" t="n">
+        <v>1144440575.87456</v>
+      </c>
+      <c r="P23" s="4" t="n">
+        <v>1480404511.63474</v>
+      </c>
+      <c r="Q23" s="4" t="n">
+        <v>1712535393.73587</v>
+      </c>
+      <c r="R23" s="4" t="n">
+        <v>15703.319272935</v>
+      </c>
+      <c r="S23" s="4" t="n">
+        <v>345033.474765153</v>
+      </c>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4" t="n">
+        <v>-138239.067583408</v>
+      </c>
+      <c r="W23" s="4" t="n">
+        <v>-2169110.39525917</v>
+      </c>
+      <c r="X23" s="4" t="n">
+        <v>-5665668.71720503</v>
+      </c>
+      <c r="Y23" s="4" t="n">
+        <v>-612918.574825158</v>
+      </c>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="4" t="n">
+        <v>-102233.85120552</v>
+      </c>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="4"/>
+      <c r="AL23" s="4"/>
+      <c r="AM23" s="4"/>
+    </row>
+    <row r="24">
+      <c r="M24" t="s">
+        <v>80</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4" t="n">
+        <v>425124656.680747</v>
+      </c>
+      <c r="R24" s="4" t="n">
+        <v>6317450421.75617</v>
+      </c>
+      <c r="S24" s="4" t="n">
+        <v>3136040699.27094</v>
+      </c>
+      <c r="T24" s="4" t="n">
+        <v>6907196726.12759</v>
+      </c>
+      <c r="U24" s="4" t="n">
+        <v>8720259255.85541</v>
+      </c>
+      <c r="V24" s="4" t="n">
+        <v>6111292031.61149</v>
+      </c>
+      <c r="W24" s="4" t="n">
+        <v>5861461032.73384</v>
+      </c>
+      <c r="X24" s="4" t="n">
+        <v>3077980779.30084</v>
+      </c>
+      <c r="Y24" s="4" t="n">
+        <v>2815549299.71783</v>
+      </c>
+      <c r="Z24" s="4" t="n">
+        <v>2094990395.83396</v>
+      </c>
+      <c r="AA24" s="4" t="n">
+        <v>1817533944.86556</v>
+      </c>
+      <c r="AB24" s="4" t="n">
+        <v>1745047651.35394</v>
+      </c>
+      <c r="AC24" s="4" t="n">
+        <v>1736580129.93913</v>
+      </c>
+      <c r="AD24" s="4" t="n">
+        <v>1720651326.85622</v>
+      </c>
+      <c r="AE24" s="4" t="n">
+        <v>2110799725.92221</v>
+      </c>
+      <c r="AF24" s="4" t="n">
+        <v>48368781.2331422</v>
+      </c>
+      <c r="AG24" s="4" t="n">
+        <v>-12974377.1706202</v>
+      </c>
+      <c r="AH24" s="4" t="n">
+        <v>-18977305.6795489</v>
+      </c>
+      <c r="AI24" s="4" t="n">
+        <v>2910845.07791779</v>
+      </c>
+      <c r="AJ24" s="4" t="n">
+        <v>-24005672.7453</v>
+      </c>
+      <c r="AK24" s="4" t="n">
+        <v>67794846.1598039</v>
+      </c>
+      <c r="AL24" s="4"/>
+      <c r="AM24" s="4"/>
+    </row>
+    <row r="25">
+      <c r="M25" t="s">
+        <v>81</v>
+      </c>
+      <c r="N25" s="4" t="n">
+        <v>287650773.263358</v>
+      </c>
+      <c r="O25" s="4" t="n">
+        <v>423766740.36093</v>
+      </c>
+      <c r="P25" s="4" t="n">
+        <v>10179104.0628542</v>
+      </c>
+      <c r="Q25" s="4" t="n">
+        <v>365611014.859387</v>
+      </c>
+      <c r="R25" s="4" t="n">
+        <v>292427817.044208</v>
+      </c>
+      <c r="S25" s="4" t="n">
+        <v>431550696.51987</v>
+      </c>
+      <c r="T25" s="4" t="n">
+        <v>886708500.956586</v>
+      </c>
+      <c r="U25" s="4" t="n">
+        <v>1450468818.47828</v>
+      </c>
+      <c r="V25" s="4" t="n">
+        <v>3640513600.21965</v>
+      </c>
+      <c r="W25" s="4" t="n">
+        <v>4871664174.94981</v>
+      </c>
+      <c r="X25" s="4" t="n">
+        <v>2452888437.79815</v>
+      </c>
+      <c r="Y25" s="4" t="n">
+        <v>6253873811.11388</v>
+      </c>
+      <c r="Z25" s="4" t="n">
+        <v>5923315083.89489</v>
+      </c>
+      <c r="AA25" s="4" t="n">
+        <v>15072861161.814</v>
+      </c>
+      <c r="AB25" s="4" t="n">
+        <v>4620991468.55793</v>
+      </c>
+      <c r="AC25" s="4" t="n">
+        <v>13662283460.173</v>
+      </c>
+      <c r="AD25" s="4" t="n">
+        <v>12093375032.921</v>
+      </c>
+      <c r="AE25" s="4" t="n">
+        <v>28216244674.2591</v>
+      </c>
+      <c r="AF25" s="4" t="n">
+        <v>18263829204.4582</v>
+      </c>
+      <c r="AG25" s="4" t="n">
+        <v>19217866261.8444</v>
+      </c>
+      <c r="AH25" s="4" t="n">
+        <v>39736715886.6388</v>
+      </c>
+      <c r="AI25" s="4" t="n">
+        <v>10484565667.4331</v>
+      </c>
+      <c r="AJ25" s="4" t="n">
+        <v>20754154100.2067</v>
+      </c>
+      <c r="AK25" s="4" t="n">
+        <v>25615565561.0424</v>
+      </c>
+      <c r="AL25" s="4"/>
+      <c r="AM25" s="4"/>
+    </row>
+    <row r="26">
+      <c r="M26" t="s">
+        <v>82</v>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4" t="n">
+        <v>66754511.2459015</v>
+      </c>
+      <c r="S26" s="4" t="n">
+        <v>627350262.46285</v>
+      </c>
+      <c r="T26" s="4" t="n">
+        <v>1218505169.51598</v>
+      </c>
+      <c r="U26" s="4" t="n">
+        <v>1460169348.00767</v>
+      </c>
+      <c r="V26" s="4" t="n">
+        <v>1044587335.3816</v>
+      </c>
+      <c r="W26" s="4" t="n">
+        <v>1436669301.34581</v>
+      </c>
+      <c r="X26" s="4" t="n">
+        <v>1676961892.88473</v>
+      </c>
+      <c r="Y26" s="4" t="n">
+        <v>3881915087.21971</v>
+      </c>
+      <c r="Z26" s="4" t="n">
+        <v>4741784391.10155</v>
+      </c>
+      <c r="AA26" s="4" t="n">
+        <v>929119422.485886</v>
+      </c>
+      <c r="AB26" s="4" t="n">
+        <v>1032215186.63633</v>
+      </c>
+      <c r="AC26" s="4" t="n">
+        <v>2109675374.39652</v>
+      </c>
+      <c r="AD26" s="4" t="n">
+        <v>4154537539.02402</v>
+      </c>
+      <c r="AE26" s="4" t="n">
+        <v>3297300338.66007</v>
+      </c>
+      <c r="AF26" s="4" t="n">
+        <v>3146623419.21135</v>
+      </c>
+      <c r="AG26" s="4" t="n">
+        <v>4348159968.61102</v>
+      </c>
+      <c r="AH26" s="4" t="n">
+        <v>3084297039.21306</v>
+      </c>
+      <c r="AI26" s="4" t="n">
+        <v>2818093608.33565</v>
+      </c>
+      <c r="AJ26" s="4" t="n">
+        <v>589031561.3532</v>
+      </c>
+      <c r="AK26" s="4" t="n">
+        <v>439640925.619207</v>
+      </c>
+      <c r="AL26" s="4"/>
+      <c r="AM26" s="4"/>
+    </row>
+    <row r="27">
+      <c r="M27" t="s">
+        <v>83</v>
+      </c>
+      <c r="N27" s="4" t="n">
+        <v>25541646606.9742</v>
+      </c>
+      <c r="O27" s="4" t="n">
+        <v>24542485802.1694</v>
+      </c>
+      <c r="P27" s="4" t="n">
+        <v>21561421439.697</v>
+      </c>
+      <c r="Q27" s="4" t="n">
+        <v>28884108134.1162</v>
+      </c>
+      <c r="R27" s="4" t="n">
+        <v>6962688747.90922</v>
+      </c>
+      <c r="S27" s="4" t="n">
+        <v>10613218179.3257</v>
+      </c>
+      <c r="T27" s="4" t="n">
+        <v>11343655139.163</v>
+      </c>
+      <c r="U27" s="4" t="n">
+        <v>16303988033.7766</v>
+      </c>
+      <c r="V27" s="4" t="n">
+        <v>21998638323.3883</v>
+      </c>
+      <c r="W27" s="4" t="n">
+        <v>21219356889.1999</v>
+      </c>
+      <c r="X27" s="4" t="n">
+        <v>22723858100.3641</v>
+      </c>
+      <c r="Y27" s="4" t="n">
+        <v>24245679184.824</v>
+      </c>
+      <c r="Z27" s="4" t="n">
+        <v>27302066296.4956</v>
+      </c>
+      <c r="AA27" s="4" t="n">
+        <v>29250451420.6863</v>
+      </c>
+      <c r="AB27" s="4" t="n">
+        <v>23586442738.8641</v>
+      </c>
+      <c r="AC27" s="4" t="n">
+        <v>12809105236.506</v>
+      </c>
+      <c r="AD27" s="4" t="n">
+        <v>17221216085.8499</v>
+      </c>
+      <c r="AE27" s="4" t="n">
+        <v>15010606991.6495</v>
+      </c>
+      <c r="AF27" s="4" t="n">
+        <v>14984010902.8538</v>
+      </c>
+      <c r="AG27" s="4" t="n">
+        <v>14031726620.142</v>
+      </c>
+      <c r="AH27" s="4" t="n">
+        <v>9331138387.36748</v>
+      </c>
+      <c r="AI27" s="4" t="n">
+        <v>13371010251.4284</v>
+      </c>
+      <c r="AJ27" s="4" t="n">
+        <v>11917196075.6053</v>
+      </c>
+      <c r="AK27" s="4" t="n">
+        <v>7710190492.49493</v>
+      </c>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+    </row>
+    <row r="28">
+      <c r="M28" t="s">
+        <v>84</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4" t="n">
+        <v>323313986.433445</v>
+      </c>
+      <c r="S28" s="4" t="n">
+        <v>1852642598.31815</v>
+      </c>
+      <c r="T28" s="4" t="n">
+        <v>1686194863.98683</v>
+      </c>
+      <c r="U28" s="4" t="n">
+        <v>2698195054.80361</v>
+      </c>
+      <c r="V28" s="4" t="n">
+        <v>3855696714.51016</v>
+      </c>
+      <c r="W28" s="4" t="n">
+        <v>3834443879.59528</v>
+      </c>
+      <c r="X28" s="4" t="n">
+        <v>3937265634.57207</v>
+      </c>
+      <c r="Y28" s="4" t="n">
+        <v>3761843999.29822</v>
+      </c>
+      <c r="Z28" s="4" t="n">
+        <v>3810705001.26915</v>
+      </c>
+      <c r="AA28" s="4" t="n">
+        <v>2630072175.327</v>
+      </c>
+      <c r="AB28" s="4" t="n">
+        <v>2633871792.77867</v>
+      </c>
+      <c r="AC28" s="4" t="n">
+        <v>2538892249.63305</v>
+      </c>
+      <c r="AD28" s="4" t="n">
+        <v>2665301955.7506</v>
+      </c>
+      <c r="AE28" s="4" t="n">
+        <v>2798126346.50147</v>
+      </c>
+      <c r="AF28" s="4" t="n">
+        <v>2850378594.25771</v>
+      </c>
+      <c r="AG28" s="4" t="n">
+        <v>2069735039.34548</v>
+      </c>
+      <c r="AH28" s="4" t="n">
+        <v>2177755565.34538</v>
+      </c>
+      <c r="AI28" s="4" t="n">
+        <v>2247958806.79859</v>
+      </c>
+      <c r="AJ28" s="4" t="n">
+        <v>1590750685.0735</v>
+      </c>
+      <c r="AK28" s="4" t="n">
+        <v>804505518.492005</v>
+      </c>
+      <c r="AL28" s="4"/>
+      <c r="AM28" s="4"/>
+    </row>
+    <row r="29">
+      <c r="M29"/>
+      <c r="N29" s="4" t="n">
+        <v>28843676163.5078</v>
+      </c>
+      <c r="O29" s="4" t="n">
+        <v>29858596097.496</v>
+      </c>
+      <c r="P29" s="4" t="n">
+        <v>36299860605.889</v>
+      </c>
+      <c r="Q29" s="4" t="n">
+        <v>41854453280.0198</v>
+      </c>
+      <c r="R29" s="4" t="n">
+        <v>54473875879.7346</v>
+      </c>
+      <c r="S29" s="4" t="n">
+        <v>49020869984.2884</v>
+      </c>
+      <c r="T29" s="4" t="n">
+        <v>50034198871.282</v>
+      </c>
+      <c r="U29" s="4" t="n">
+        <v>45724943162.9779</v>
+      </c>
+      <c r="V29" s="4" t="n">
+        <v>47581584706.6059</v>
+      </c>
+      <c r="W29" s="4" t="n">
+        <v>42798132265.4258</v>
+      </c>
+      <c r="X29" s="4" t="n">
+        <v>40071129816.6374</v>
+      </c>
+      <c r="Y29" s="4" t="n">
+        <v>39315870788.7558</v>
+      </c>
+      <c r="Z29" s="4" t="n">
+        <v>45374942597.2359</v>
+      </c>
+      <c r="AA29" s="4" t="n">
+        <v>35746047159.7981</v>
+      </c>
+      <c r="AB29" s="4" t="n">
+        <v>31036158330.9832</v>
+      </c>
+      <c r="AC29" s="4" t="n">
+        <v>36872828438.8067</v>
+      </c>
+      <c r="AD29" s="4" t="n">
+        <v>41701082305.1633</v>
+      </c>
+      <c r="AE29" s="4" t="n">
+        <v>44318321120.0986</v>
+      </c>
+      <c r="AF29" s="4" t="n">
+        <v>51251211141.4598</v>
+      </c>
+      <c r="AG29" s="4" t="n">
+        <v>54898255463.6872</v>
+      </c>
+      <c r="AH29" s="4" t="n">
+        <v>55861401773.1799</v>
+      </c>
+      <c r="AI29" s="4" t="n">
+        <v>44418121331.7944</v>
+      </c>
+      <c r="AJ29" s="4" t="n">
+        <v>37139289470.8574</v>
+      </c>
+      <c r="AK29" s="4" t="n">
+        <v>23852760143.0116</v>
+      </c>
+      <c r="AL29" s="4"/>
+      <c r="AM29" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" xSplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="M1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="M2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="5" t="n">
+        <v>11523165905</v>
+      </c>
+      <c r="O2" s="5" t="n">
+        <v>11635066230</v>
+      </c>
+      <c r="P2" s="5" t="n">
+        <v>13035567972</v>
+      </c>
+      <c r="Q2" s="5" t="n">
+        <v>13973522637</v>
+      </c>
+      <c r="R2" s="5" t="n">
+        <v>14174736024.5723</v>
+      </c>
+      <c r="S2" s="5" t="n">
+        <v>11924630566</v>
+      </c>
+      <c r="T2" s="5" t="n">
+        <v>17163459478.6448</v>
+      </c>
+      <c r="U2" s="5" t="n">
+        <v>20300409799.806</v>
+      </c>
+      <c r="V2" s="5" t="n">
+        <v>19850845472.7235</v>
+      </c>
+      <c r="W2" s="5" t="n">
+        <v>17516742394.2319</v>
+      </c>
+      <c r="X2" s="5" t="n">
+        <v>15377360972.433</v>
+      </c>
+      <c r="Y2" s="5" t="n">
+        <v>20828666552.2071</v>
+      </c>
+      <c r="Z2" s="5" t="n">
+        <v>25012321488.1929</v>
+      </c>
+      <c r="AA2" s="5" t="n">
+        <v>28424731458.0841</v>
+      </c>
+      <c r="AB2" s="5" t="n">
+        <v>18903233969.8585</v>
+      </c>
+      <c r="AC2" s="5" t="n">
+        <v>20896709228.0732</v>
+      </c>
+      <c r="AD2" s="5" t="n">
+        <v>28713124933.7282</v>
+      </c>
+      <c r="AE2" s="5" t="n">
+        <v>36472650890.3201</v>
+      </c>
+      <c r="AF2" s="5" t="n">
+        <v>31697764945.9667</v>
+      </c>
+      <c r="AG2" s="5" t="n">
+        <v>29469330002.0175</v>
+      </c>
+      <c r="AH2" s="5" t="n">
+        <v>49310683025.1053</v>
+      </c>
+      <c r="AI2" s="5" t="n">
+        <v>24076627044.1989</v>
+      </c>
+      <c r="AJ2" s="5" t="n">
+        <v>22473083092.4323</v>
+      </c>
+      <c r="AK2" s="5" t="n">
+        <v>30783189501.5461</v>
+      </c>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="M3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <v>1526310355</v>
+      </c>
+      <c r="O3" s="5" t="n">
+        <v>1527502959</v>
+      </c>
+      <c r="P3" s="5" t="n">
+        <v>1566657341</v>
+      </c>
+      <c r="Q3" s="5" t="n">
+        <v>1614627173</v>
+      </c>
+      <c r="R3" s="5" t="n">
+        <v>2543315614</v>
+      </c>
+      <c r="S3" s="5" t="n">
+        <v>2406935142.6504</v>
+      </c>
+      <c r="T3" s="5" t="n">
+        <v>2217531658.0625</v>
+      </c>
+      <c r="U3" s="5" t="n">
+        <v>3311788138.5867</v>
+      </c>
+      <c r="V3" s="5" t="n">
+        <v>7294328950.3001</v>
+      </c>
+      <c r="W3" s="5" t="n">
+        <v>7488304800.9775</v>
+      </c>
+      <c r="X3" s="5" t="n">
+        <v>7344378933.9791</v>
+      </c>
+      <c r="Y3" s="5" t="n">
+        <v>8728311625.3308</v>
+      </c>
+      <c r="Z3" s="5" t="n">
+        <v>10131143816.4921</v>
+      </c>
+      <c r="AA3" s="5" t="n">
+        <v>7007160788.3216</v>
+      </c>
+      <c r="AB3" s="5" t="n">
+        <v>6104120338.316</v>
+      </c>
+      <c r="AC3" s="5" t="n">
+        <v>5191054981.9223</v>
+      </c>
+      <c r="AD3" s="5" t="n">
+        <v>7294777184.7297</v>
+      </c>
+      <c r="AE3" s="5" t="n">
+        <v>4981803507.7</v>
+      </c>
+      <c r="AF3" s="5" t="n">
+        <v>4009280634.0914</v>
+      </c>
+      <c r="AG3" s="5" t="n">
+        <v>6272321628.1071</v>
+      </c>
+      <c r="AH3" s="5" t="n">
+        <v>5093640606.5798</v>
+      </c>
+      <c r="AI3" s="5" t="n">
+        <v>5751712310.2692</v>
+      </c>
+      <c r="AJ3" s="5" t="n">
+        <v>4504888484.4697</v>
+      </c>
+      <c r="AK3" s="5" t="n">
+        <v>3753102927.7395</v>
+      </c>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+    </row>
+    <row r="4">
+      <c r="M4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>1024707059</v>
+      </c>
+      <c r="O4" s="5" t="n">
+        <v>1505365287.25</v>
+      </c>
+      <c r="P4" s="5" t="n">
+        <v>1842407111</v>
+      </c>
+      <c r="Q4" s="5" t="n">
+        <v>2021251722</v>
+      </c>
+      <c r="R4" s="5" t="n">
+        <v>2156075566.0303</v>
+      </c>
+      <c r="S4" s="5" t="n">
+        <v>1881665918.5924</v>
+      </c>
+      <c r="T4" s="5" t="n">
+        <v>2078067023.3162</v>
+      </c>
+      <c r="U4" s="5" t="n">
+        <v>2328285596.009</v>
+      </c>
+      <c r="V4" s="5" t="n">
+        <v>3273817869.9623</v>
+      </c>
+      <c r="W4" s="5" t="n">
+        <v>3408596579.9311</v>
+      </c>
+      <c r="X4" s="5" t="n">
+        <v>3281318468.4949</v>
+      </c>
+      <c r="Y4" s="5" t="n">
+        <v>2778369808.9903</v>
+      </c>
+      <c r="Z4" s="5" t="n">
+        <v>2165992656.0871</v>
+      </c>
+      <c r="AA4" s="5" t="n">
+        <v>2997099335.7022</v>
+      </c>
+      <c r="AB4" s="5" t="n">
+        <v>1750965950.2267</v>
+      </c>
+      <c r="AC4" s="5" t="n">
+        <v>2299197942.8896</v>
+      </c>
+      <c r="AD4" s="5" t="n">
+        <v>2561559096.887</v>
+      </c>
+      <c r="AE4" s="5" t="n">
+        <v>2473645976.2595</v>
+      </c>
+      <c r="AF4" s="5" t="n">
+        <v>3263723149.8721</v>
+      </c>
+      <c r="AG4" s="5" t="n">
+        <v>3121038771.9798</v>
+      </c>
+      <c r="AH4" s="5" t="n">
+        <v>2893022681.5449</v>
+      </c>
+      <c r="AI4" s="5" t="n">
+        <v>2417184572.3753</v>
+      </c>
+      <c r="AJ4" s="5" t="n">
+        <v>2621443014.8911</v>
+      </c>
+      <c r="AK4" s="5" t="n">
+        <v>1328212616.3231</v>
+      </c>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="M5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <v>1631584413</v>
+      </c>
+      <c r="O5" s="5" t="n">
+        <v>1424361314</v>
+      </c>
+      <c r="P5" s="5" t="n">
+        <v>2882724041</v>
+      </c>
+      <c r="Q5" s="5" t="n">
+        <v>5157605831</v>
+      </c>
+      <c r="R5" s="5" t="n">
+        <v>5351273078.2813</v>
+      </c>
+      <c r="S5" s="5" t="n">
+        <v>6406269058</v>
+      </c>
+      <c r="T5" s="5" t="n">
+        <v>7535206808</v>
+      </c>
+      <c r="U5" s="5" t="n">
+        <v>7052497117.5649</v>
+      </c>
+      <c r="V5" s="5" t="n">
+        <v>5980976276.9147</v>
+      </c>
+      <c r="W5" s="5" t="n">
+        <v>5635584424.0052</v>
+      </c>
+      <c r="X5" s="5" t="n">
+        <v>5016553175.262</v>
+      </c>
+      <c r="Y5" s="5" t="n">
+        <v>3950598791.9931</v>
+      </c>
+      <c r="Z5" s="5" t="n">
+        <v>3901297069.2169</v>
+      </c>
+      <c r="AA5" s="5" t="n">
+        <v>3506508605.88</v>
+      </c>
+      <c r="AB5" s="5" t="n">
+        <v>1924748817.8513</v>
+      </c>
+      <c r="AC5" s="5" t="n">
+        <v>2029722696.6524</v>
+      </c>
+      <c r="AD5" s="5" t="n">
+        <v>1674887591.3212</v>
+      </c>
+      <c r="AE5" s="5" t="n">
+        <v>1791969018.6331</v>
+      </c>
+      <c r="AF5" s="5" t="n">
+        <v>1071516291.4968</v>
+      </c>
+      <c r="AG5" s="5" t="n">
+        <v>1358865606.2214</v>
+      </c>
+      <c r="AH5" s="5" t="n">
+        <v>1451977119.4719</v>
+      </c>
+      <c r="AI5" s="5" t="n">
+        <v>1081057404.8316</v>
+      </c>
+      <c r="AJ5" s="5" t="n">
+        <v>1197423909.9488</v>
+      </c>
+      <c r="AK5" s="5" t="n">
+        <v>900646301.9873</v>
+      </c>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="M6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <v>3081494684</v>
+      </c>
+      <c r="O6" s="5" t="n">
+        <v>3597072376</v>
+      </c>
+      <c r="P6" s="5" t="n">
+        <v>3581449904</v>
+      </c>
+      <c r="Q6" s="5" t="n">
+        <v>5090117133.75</v>
+      </c>
+      <c r="R6" s="5" t="n">
+        <v>4252312963</v>
+      </c>
+      <c r="S6" s="5" t="n">
+        <v>5029819058.1563</v>
+      </c>
+      <c r="T6" s="5" t="n">
+        <v>4042086114.9101</v>
+      </c>
+      <c r="U6" s="5" t="n">
+        <v>4897902934.7801</v>
+      </c>
+      <c r="V6" s="5" t="n">
+        <v>3894657966.8977</v>
+      </c>
+      <c r="W6" s="5" t="n">
+        <v>4314844046.2276</v>
+      </c>
+      <c r="X6" s="5" t="n">
+        <v>4233643934.6057</v>
+      </c>
+      <c r="Y6" s="5" t="n">
+        <v>4443449535.729</v>
+      </c>
+      <c r="Z6" s="5" t="n">
+        <v>4199880662.3778</v>
+      </c>
+      <c r="AA6" s="5" t="n">
+        <v>3683885727.6941</v>
+      </c>
+      <c r="AB6" s="5" t="n">
+        <v>3859477123.0163</v>
+      </c>
+      <c r="AC6" s="5" t="n">
+        <v>3894232466.3633</v>
+      </c>
+      <c r="AD6" s="5" t="n">
+        <v>4884931006.8703</v>
+      </c>
+      <c r="AE6" s="5" t="n">
+        <v>3265867785.9096</v>
+      </c>
+      <c r="AF6" s="5" t="n">
+        <v>7038647958.3636</v>
+      </c>
+      <c r="AG6" s="5" t="n">
+        <v>9563635622.0819</v>
+      </c>
+      <c r="AH6" s="5" t="n">
+        <v>8751503140.2144</v>
+      </c>
+      <c r="AI6" s="5" t="n">
+        <v>5014299385.473</v>
+      </c>
+      <c r="AJ6" s="5" t="n">
+        <v>9059356158.3807</v>
+      </c>
+      <c r="AK6" s="5" t="n">
+        <v>4358452869.9185</v>
+      </c>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="M7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>1692281014</v>
+      </c>
+      <c r="O7" s="5" t="n">
+        <v>1294033820.0703</v>
+      </c>
+      <c r="P7" s="5" t="n">
+        <v>1371509275.1877</v>
+      </c>
+      <c r="Q7" s="5" t="n">
+        <v>1758442747.4023</v>
+      </c>
+      <c r="R7" s="5" t="n">
+        <v>1766137378.7492</v>
+      </c>
+      <c r="S7" s="5" t="n">
+        <v>2141360307.3462</v>
+      </c>
+      <c r="T7" s="5" t="n">
+        <v>2965158237.8856</v>
+      </c>
+      <c r="U7" s="5" t="n">
+        <v>3262406448.1676</v>
+      </c>
+      <c r="V7" s="5" t="n">
+        <v>3543228996.7589</v>
+      </c>
+      <c r="W7" s="5" t="n">
+        <v>2753970286.2125</v>
+      </c>
+      <c r="X7" s="5" t="n">
+        <v>2903333302.4875</v>
+      </c>
+      <c r="Y7" s="5" t="n">
+        <v>3234688297.5393</v>
+      </c>
+      <c r="Z7" s="5" t="n">
+        <v>3765447953.0069</v>
+      </c>
+      <c r="AA7" s="5" t="n">
+        <v>4184208304.4962</v>
+      </c>
+      <c r="AB7" s="5" t="n">
+        <v>4747892302.6095</v>
+      </c>
+      <c r="AC7" s="5" t="n">
+        <v>4289479624.1908</v>
+      </c>
+      <c r="AD7" s="5" t="n">
+        <v>4437075747.4315</v>
+      </c>
+      <c r="AE7" s="5" t="n">
+        <v>5088520307.0746</v>
+      </c>
+      <c r="AF7" s="5" t="n">
+        <v>5147116522.526</v>
+      </c>
+      <c r="AG7" s="5" t="n">
+        <v>5387572438.4417</v>
+      </c>
+      <c r="AH7" s="5" t="n">
+        <v>6042592599.7574</v>
+      </c>
+      <c r="AI7" s="5" t="n">
+        <v>5978991439.1975</v>
+      </c>
+      <c r="AJ7" s="5" t="n">
+        <v>5973325868.1803</v>
+      </c>
+      <c r="AK7" s="5" t="n">
+        <v>4331229233.7263</v>
+      </c>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+    </row>
+    <row r="8">
+      <c r="M8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" s="5" t="n">
+        <v>129335396</v>
+      </c>
+      <c r="O8" s="5" t="n">
+        <v>195211562</v>
+      </c>
+      <c r="P8" s="5" t="n">
+        <v>154166576</v>
+      </c>
+      <c r="Q8" s="5" t="n">
+        <v>562088268</v>
+      </c>
+      <c r="R8" s="5" t="n">
+        <v>729270677.7193</v>
+      </c>
+      <c r="S8" s="5" t="n">
+        <v>809623548</v>
+      </c>
+      <c r="T8" s="5" t="n">
+        <v>872507237.7906</v>
+      </c>
+      <c r="U8" s="5" t="n">
+        <v>441535594.9308</v>
+      </c>
+      <c r="V8" s="5" t="n">
+        <v>1178713249.7479</v>
+      </c>
+      <c r="W8" s="5" t="n">
+        <v>1495141671.6773</v>
+      </c>
+      <c r="X8" s="5" t="n">
+        <v>1058516239.4655</v>
+      </c>
+      <c r="Y8" s="5" t="n">
+        <v>1340861687.1985</v>
+      </c>
+      <c r="Z8" s="5" t="n">
+        <v>3483311599.3926</v>
+      </c>
+      <c r="AA8" s="5" t="n">
+        <v>1729451136.6205</v>
+      </c>
+      <c r="AB8" s="5" t="n">
+        <v>1927679670.4557</v>
+      </c>
+      <c r="AC8" s="5" t="n">
+        <v>2321036824.1751</v>
+      </c>
+      <c r="AD8" s="5" t="n">
+        <v>2068277146.4878</v>
+      </c>
+      <c r="AE8" s="5" t="n">
+        <v>2775210033.8739</v>
+      </c>
+      <c r="AF8" s="5" t="n">
+        <v>2046718123.3618</v>
+      </c>
+      <c r="AG8" s="5" t="n">
+        <v>2815635491.5853</v>
+      </c>
+      <c r="AH8" s="5" t="n">
+        <v>2435485404.4599</v>
+      </c>
+      <c r="AI8" s="5" t="n">
+        <v>2128116189.6113</v>
+      </c>
+      <c r="AJ8" s="5" t="n">
+        <v>2158416643.1052</v>
+      </c>
+      <c r="AK8" s="5" t="n">
+        <v>1964336827.3326</v>
+      </c>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5"/>
+    </row>
+    <row r="9">
+      <c r="M9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N9" s="5" t="n">
+        <v>961194893</v>
+      </c>
+      <c r="O9" s="5" t="n">
+        <v>1062482642</v>
+      </c>
+      <c r="P9" s="5" t="n">
+        <v>1105709463.3809</v>
+      </c>
+      <c r="Q9" s="5" t="n">
+        <v>1565199186</v>
+      </c>
+      <c r="R9" s="5" t="n">
+        <v>1296303672.8721</v>
+      </c>
+      <c r="S9" s="5" t="n">
+        <v>1389110028.4114</v>
+      </c>
+      <c r="T9" s="5" t="n">
+        <v>2006236893.5796</v>
+      </c>
+      <c r="U9" s="5" t="n">
+        <v>2231091720.3776</v>
+      </c>
+      <c r="V9" s="5" t="n">
+        <v>3265277083.8173</v>
+      </c>
+      <c r="W9" s="5" t="n">
+        <v>3059132175.0728</v>
+      </c>
+      <c r="X9" s="5" t="n">
+        <v>3398880448.8511</v>
+      </c>
+      <c r="Y9" s="5" t="n">
+        <v>3943493230.406</v>
+      </c>
+      <c r="Z9" s="5" t="n">
+        <v>3631783055.3313</v>
+      </c>
+      <c r="AA9" s="5" t="n">
+        <v>3907687401.5249</v>
+      </c>
+      <c r="AB9" s="5" t="n">
+        <v>2671115201.1736</v>
+      </c>
+      <c r="AC9" s="5" t="n">
+        <v>2989225731.9579</v>
+      </c>
+      <c r="AD9" s="5" t="n">
+        <v>4227250449.0447</v>
+      </c>
+      <c r="AE9" s="5" t="n">
+        <v>5297665670.3874</v>
+      </c>
+      <c r="AF9" s="5" t="n">
+        <v>4612257034.4371</v>
+      </c>
+      <c r="AG9" s="5" t="n">
+        <v>6326657031.2252</v>
+      </c>
+      <c r="AH9" s="5" t="n">
+        <v>5144323542.7282</v>
+      </c>
+      <c r="AI9" s="5" t="n">
+        <v>4036484484.5643</v>
+      </c>
+      <c r="AJ9" s="5" t="n">
+        <v>4162714111.4593</v>
+      </c>
+      <c r="AK9" s="5" t="n">
+        <v>3299322853.726</v>
+      </c>
+      <c r="AL9" s="5"/>
+      <c r="AM9" s="5"/>
+    </row>
+    <row r="10">
+      <c r="M10" t="s">
+        <v>94</v>
+      </c>
+      <c r="N10" s="5" t="n">
+        <v>13850260539</v>
+      </c>
+      <c r="O10" s="5" t="n">
+        <v>13880749857.6191</v>
+      </c>
+      <c r="P10" s="5" t="n">
+        <v>13485688366.4775</v>
+      </c>
+      <c r="Q10" s="5" t="n">
+        <v>17502165488.3044</v>
+      </c>
+      <c r="R10" s="5" t="n">
+        <v>15532701589.7536</v>
+      </c>
+      <c r="S10" s="5" t="n">
+        <v>15293185099.9268</v>
+      </c>
+      <c r="T10" s="5" t="n">
+        <v>15092724529.0914</v>
+      </c>
+      <c r="U10" s="5" t="n">
+        <v>16656013492.5133</v>
+      </c>
+      <c r="V10" s="5" t="n">
+        <v>18444889602.7732</v>
+      </c>
+      <c r="W10" s="5" t="n">
+        <v>20177333438.2545</v>
+      </c>
+      <c r="X10" s="5" t="n">
+        <v>20988605463.4153</v>
+      </c>
+      <c r="Y10" s="5" t="n">
+        <v>21054354363.8309</v>
+      </c>
+      <c r="Z10" s="5" t="n">
+        <v>21872930341.5916</v>
+      </c>
+      <c r="AA10" s="5" t="n">
+        <v>17817975531.0462</v>
+      </c>
+      <c r="AB10" s="5" t="n">
+        <v>16333209903.6338</v>
+      </c>
+      <c r="AC10" s="5" t="n">
+        <v>17782500575.9875</v>
+      </c>
+      <c r="AD10" s="5" t="n">
+        <v>19484257466.2842</v>
+      </c>
+      <c r="AE10" s="5" t="n">
+        <v>23675213179.569</v>
+      </c>
+      <c r="AF10" s="5" t="n">
+        <v>24451756514.3184</v>
+      </c>
+      <c r="AG10" s="5" t="n">
+        <v>25772726787.7473</v>
+      </c>
+      <c r="AH10" s="5" t="n">
+        <v>24187209794.076</v>
+      </c>
+      <c r="AI10" s="5" t="n">
+        <v>22010325695.1304</v>
+      </c>
+      <c r="AJ10" s="5" t="n">
+        <v>22979854523.3634</v>
+      </c>
+      <c r="AK10" s="5" t="n">
+        <v>13569818137.2031</v>
+      </c>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5"/>
+    </row>
+    <row r="11">
+      <c r="M11"/>
+      <c r="N11" s="5" t="n">
+        <v>3806.53</v>
+      </c>
+      <c r="O11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5" t="n">
+        <v>9511.1201</v>
+      </c>
+      <c r="Q11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="5"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="5"/>
+      <c r="AM11" s="5"/>
+    </row>
+    <row r="15">
+      <c r="M15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R15" t="s">
+        <v>15</v>
+      </c>
+      <c r="S15" t="s">
+        <v>16</v>
+      </c>
+      <c r="T15" t="s">
+        <v>17</v>
+      </c>
+      <c r="U15" t="s">
+        <v>18</v>
+      </c>
+      <c r="V15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W15" t="s">
+        <v>20</v>
+      </c>
+      <c r="X15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="M16" t="s">
+        <v>86</v>
+      </c>
+      <c r="N16" s="5" t="n">
+        <v>18618325421.1841</v>
+      </c>
+      <c r="O16" s="5" t="n">
+        <v>18354050997.8925</v>
+      </c>
+      <c r="P16" s="5" t="n">
+        <v>20243791770.9666</v>
+      </c>
+      <c r="Q16" s="5" t="n">
+        <v>21293389478.6692</v>
+      </c>
+      <c r="R16" s="5" t="n">
+        <v>21084626826.1279</v>
+      </c>
+      <c r="S16" s="5" t="n">
+        <v>17215049035.4717</v>
+      </c>
+      <c r="T16" s="5" t="n">
+        <v>23996829699.5213</v>
+      </c>
+      <c r="U16" s="5" t="n">
+        <v>27625141624.0378</v>
+      </c>
+      <c r="V16" s="5" t="n">
+        <v>26461490095.7688</v>
+      </c>
+      <c r="W16" s="5" t="n">
+        <v>23115198271.6412</v>
+      </c>
+      <c r="X16" s="5" t="n">
+        <v>20117089824.4116</v>
+      </c>
+      <c r="Y16" s="5" t="n">
+        <v>26710325638.6899</v>
+      </c>
+      <c r="Z16" s="5" t="n">
+        <v>31498016444.0715</v>
+      </c>
+      <c r="AA16" s="5" t="n">
+        <v>35151983019.9863</v>
+      </c>
+      <c r="AB16" s="5" t="n">
+        <v>22933374319.0496</v>
+      </c>
+      <c r="AC16" s="5" t="n">
+        <v>25064507043.4982</v>
+      </c>
+      <c r="AD16" s="5" t="n">
+        <v>34156847013.8695</v>
+      </c>
+      <c r="AE16" s="5" t="n">
+        <v>42626458736.9722</v>
+      </c>
+      <c r="AF16" s="5" t="n">
+        <v>36196042249.1298</v>
+      </c>
+      <c r="AG16" s="5" t="n">
+        <v>33004915757.7607</v>
+      </c>
+      <c r="AH16" s="5" t="n">
+        <v>54499686824.1206</v>
+      </c>
+      <c r="AI16" s="5" t="n">
+        <v>25744838625.9807</v>
+      </c>
+      <c r="AJ16" s="5" t="n">
+        <v>22473083092.4323</v>
+      </c>
+      <c r="AK16" s="5" t="n">
+        <v>29360956260.425</v>
+      </c>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="5"/>
+    </row>
+    <row r="17">
+      <c r="M17" t="s">
+        <v>87</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <v>2466105505.84735</v>
+      </c>
+      <c r="O17" s="5" t="n">
+        <v>2409600998.80047</v>
+      </c>
+      <c r="P17" s="5" t="n">
+        <v>2432965334.21354</v>
+      </c>
+      <c r="Q17" s="5" t="n">
+        <v>2460430784.03835</v>
+      </c>
+      <c r="R17" s="5" t="n">
+        <v>3783129402.14859</v>
+      </c>
+      <c r="S17" s="5" t="n">
+        <v>3474783246.03777</v>
+      </c>
+      <c r="T17" s="5" t="n">
+        <v>3100408144.2924</v>
+      </c>
+      <c r="U17" s="5" t="n">
+        <v>4506737413.65263</v>
+      </c>
+      <c r="V17" s="5" t="n">
+        <v>9723455534.36843</v>
+      </c>
+      <c r="W17" s="5" t="n">
+        <v>9881611905.76596</v>
+      </c>
+      <c r="X17" s="5" t="n">
+        <v>9608120078.87705</v>
+      </c>
+      <c r="Y17" s="5" t="n">
+        <v>11193037499.7455</v>
+      </c>
+      <c r="Z17" s="5" t="n">
+        <v>12758149405.6742</v>
+      </c>
+      <c r="AA17" s="5" t="n">
+        <v>8665538227.25179</v>
+      </c>
+      <c r="AB17" s="5" t="n">
+        <v>7405509386.93018</v>
+      </c>
+      <c r="AC17" s="5" t="n">
+        <v>6226398268.62227</v>
+      </c>
+      <c r="AD17" s="5" t="n">
+        <v>8677794175.1088</v>
+      </c>
+      <c r="AE17" s="5" t="n">
+        <v>5822352817.05387</v>
+      </c>
+      <c r="AF17" s="5" t="n">
+        <v>4578243654.32604</v>
+      </c>
+      <c r="AG17" s="5" t="n">
+        <v>7024844030.28785</v>
+      </c>
+      <c r="AH17" s="5" t="n">
+        <v>5629648603.97267</v>
+      </c>
+      <c r="AI17" s="5" t="n">
+        <v>6150234622.94421</v>
+      </c>
+      <c r="AJ17" s="5" t="n">
+        <v>4504888484.4697</v>
+      </c>
+      <c r="AK17" s="5" t="n">
+        <v>3579703490.33189</v>
+      </c>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="5"/>
+    </row>
+    <row r="18">
+      <c r="M18" t="s">
+        <v>88</v>
+      </c>
+      <c r="N18" s="5" t="n">
+        <v>1655649987.43689</v>
+      </c>
+      <c r="O18" s="5" t="n">
+        <v>2374679327.68644</v>
+      </c>
+      <c r="P18" s="5" t="n">
+        <v>2861195307.52674</v>
+      </c>
+      <c r="Q18" s="5" t="n">
+        <v>3080060860.03071</v>
+      </c>
+      <c r="R18" s="5" t="n">
+        <v>3207117835.5544</v>
+      </c>
+      <c r="S18" s="5" t="n">
+        <v>2716475858.741</v>
+      </c>
+      <c r="T18" s="5" t="n">
+        <v>2905417787.40794</v>
+      </c>
+      <c r="U18" s="5" t="n">
+        <v>3168370489.32729</v>
+      </c>
+      <c r="V18" s="5" t="n">
+        <v>4364050854.17618</v>
+      </c>
+      <c r="W18" s="5" t="n">
+        <v>4498004480.50719</v>
+      </c>
+      <c r="X18" s="5" t="n">
+        <v>4292711765.79322</v>
+      </c>
+      <c r="Y18" s="5" t="n">
+        <v>3562933909.22674</v>
+      </c>
+      <c r="Z18" s="5" t="n">
+        <v>2727634551.29005</v>
+      </c>
+      <c r="AA18" s="5" t="n">
+        <v>3706419711.0595</v>
+      </c>
+      <c r="AB18" s="5" t="n">
+        <v>2124269192.27091</v>
+      </c>
+      <c r="AC18" s="5" t="n">
+        <v>2757767378.82411</v>
+      </c>
+      <c r="AD18" s="5" t="n">
+        <v>3047205150.65144</v>
+      </c>
+      <c r="AE18" s="5" t="n">
+        <v>2891009168.86981</v>
+      </c>
+      <c r="AF18" s="5" t="n">
+        <v>3726882990.76006</v>
+      </c>
+      <c r="AG18" s="5" t="n">
+        <v>3495485704.59003</v>
+      </c>
+      <c r="AH18" s="5" t="n">
+        <v>3197457841.72167</v>
+      </c>
+      <c r="AI18" s="5" t="n">
+        <v>2584665477.8833</v>
+      </c>
+      <c r="AJ18" s="5" t="n">
+        <v>2621443014.8911</v>
+      </c>
+      <c r="AK18" s="5" t="n">
+        <v>1266847040.99452</v>
+      </c>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+    </row>
+    <row r="19">
+      <c r="M19" t="s">
+        <v>89</v>
+      </c>
+      <c r="N19" s="5" t="n">
+        <v>2636199964.81909</v>
+      </c>
+      <c r="O19" s="5" t="n">
+        <v>2246897411.65153</v>
+      </c>
+      <c r="P19" s="5" t="n">
+        <v>4476771963.02555</v>
+      </c>
+      <c r="Q19" s="5" t="n">
+        <v>7859357485.57361</v>
+      </c>
+      <c r="R19" s="5" t="n">
+        <v>7959908086.09575</v>
+      </c>
+      <c r="S19" s="5" t="n">
+        <v>9248440474.31893</v>
+      </c>
+      <c r="T19" s="5" t="n">
+        <v>10535234737.917</v>
+      </c>
+      <c r="U19" s="5" t="n">
+        <v>9597157574.50919</v>
+      </c>
+      <c r="V19" s="5" t="n">
+        <v>7972735707.00426</v>
+      </c>
+      <c r="W19" s="5" t="n">
+        <v>7436750989.74732</v>
+      </c>
+      <c r="X19" s="5" t="n">
+        <v>6562793903.10206</v>
+      </c>
+      <c r="Y19" s="5" t="n">
+        <v>5066180301.91515</v>
+      </c>
+      <c r="Z19" s="5" t="n">
+        <v>4912903398.32746</v>
+      </c>
+      <c r="AA19" s="5" t="n">
+        <v>4336390342.16007</v>
+      </c>
+      <c r="AB19" s="5" t="n">
+        <v>2335102299.44334</v>
+      </c>
+      <c r="AC19" s="5" t="n">
+        <v>2434545950.3378</v>
+      </c>
+      <c r="AD19" s="5" t="n">
+        <v>1992429571.98941</v>
+      </c>
+      <c r="AE19" s="5" t="n">
+        <v>2094317017.43865</v>
+      </c>
+      <c r="AF19" s="5" t="n">
+        <v>1223576773.4338</v>
+      </c>
+      <c r="AG19" s="5" t="n">
+        <v>1521895640.53154</v>
+      </c>
+      <c r="AH19" s="5" t="n">
+        <v>1604769867.95577</v>
+      </c>
+      <c r="AI19" s="5" t="n">
+        <v>1155961272.38748</v>
+      </c>
+      <c r="AJ19" s="5" t="n">
+        <v>1197423909.9488</v>
+      </c>
+      <c r="AK19" s="5" t="n">
+        <v>859034983.2799</v>
+      </c>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="5"/>
+    </row>
+    <row r="20">
+      <c r="M20" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="5" t="n">
+        <v>4978863559.14276</v>
+      </c>
+      <c r="O20" s="5" t="n">
+        <v>5674299443.3487</v>
+      </c>
+      <c r="P20" s="5" t="n">
+        <v>5561869360.08134</v>
+      </c>
+      <c r="Q20" s="5" t="n">
+        <v>7756515621.47936</v>
+      </c>
+      <c r="R20" s="5" t="n">
+        <v>6325227631.56476</v>
+      </c>
+      <c r="S20" s="5" t="n">
+        <v>7261321954.29146</v>
+      </c>
+      <c r="T20" s="5" t="n">
+        <v>5651381194.50708</v>
+      </c>
+      <c r="U20" s="5" t="n">
+        <v>6665149303.31031</v>
+      </c>
+      <c r="V20" s="5" t="n">
+        <v>5191640495.06507</v>
+      </c>
+      <c r="W20" s="5" t="n">
+        <v>5693894069.74463</v>
+      </c>
+      <c r="X20" s="5" t="n">
+        <v>5538570335.29485</v>
+      </c>
+      <c r="Y20" s="5" t="n">
+        <v>5698203663.73048</v>
+      </c>
+      <c r="Z20" s="5" t="n">
+        <v>5288909717.12324</v>
+      </c>
+      <c r="AA20" s="5" t="n">
+        <v>4555747122.48138</v>
+      </c>
+      <c r="AB20" s="5" t="n">
+        <v>4682311697.51553</v>
+      </c>
+      <c r="AC20" s="5" t="n">
+        <v>4670927657.40619</v>
+      </c>
+      <c r="AD20" s="5" t="n">
+        <v>5811065199.6286</v>
+      </c>
+      <c r="AE20" s="5" t="n">
+        <v>3816897730.71662</v>
+      </c>
+      <c r="AF20" s="5" t="n">
+        <v>8037513033.23668</v>
+      </c>
+      <c r="AG20" s="5" t="n">
+        <v>10711033743.3231</v>
+      </c>
+      <c r="AH20" s="5" t="n">
+        <v>9672431025.52774</v>
+      </c>
+      <c r="AI20" s="5" t="n">
+        <v>5361728130.1228</v>
+      </c>
+      <c r="AJ20" s="5" t="n">
+        <v>9059356158.3807</v>
+      </c>
+      <c r="AK20" s="5" t="n">
+        <v>4157085284.17348</v>
+      </c>
+      <c r="AL20" s="5"/>
+      <c r="AM20" s="5"/>
+    </row>
+    <row r="21">
+      <c r="M21" t="s">
+        <v>91</v>
+      </c>
+      <c r="N21" s="5" t="n">
+        <v>2734269286.97364</v>
+      </c>
+      <c r="O21" s="5" t="n">
+        <v>2041308769.28991</v>
+      </c>
+      <c r="P21" s="5" t="n">
+        <v>2129907054.18334</v>
+      </c>
+      <c r="Q21" s="5" t="n">
+        <v>2679582469.57955</v>
+      </c>
+      <c r="R21" s="5" t="n">
+        <v>2627092842.50859</v>
+      </c>
+      <c r="S21" s="5" t="n">
+        <v>3091384885.22107</v>
+      </c>
+      <c r="T21" s="5" t="n">
+        <v>4145690870.49179</v>
+      </c>
+      <c r="U21" s="5" t="n">
+        <v>4439537972.61104</v>
+      </c>
+      <c r="V21" s="5" t="n">
+        <v>4723180135.25461</v>
+      </c>
+      <c r="W21" s="5" t="n">
+        <v>3634155699.00557</v>
+      </c>
+      <c r="X21" s="5" t="n">
+        <v>3798221095.35259</v>
+      </c>
+      <c r="Y21" s="5" t="n">
+        <v>4148108932.00356</v>
+      </c>
+      <c r="Z21" s="5" t="n">
+        <v>4741828606.31685</v>
+      </c>
+      <c r="AA21" s="5" t="n">
+        <v>5174480521.95775</v>
+      </c>
+      <c r="AB21" s="5" t="n">
+        <v>5760135624.19516</v>
+      </c>
+      <c r="AC21" s="5" t="n">
+        <v>5145005899.25592</v>
+      </c>
+      <c r="AD21" s="5" t="n">
+        <v>5278301050.26084</v>
+      </c>
+      <c r="AE21" s="5" t="n">
+        <v>5947075290.85383</v>
+      </c>
+      <c r="AF21" s="5" t="n">
+        <v>5877551538.03837</v>
+      </c>
+      <c r="AG21" s="5" t="n">
+        <v>6033946969.8642</v>
+      </c>
+      <c r="AH21" s="5" t="n">
+        <v>6678459597.18023</v>
+      </c>
+      <c r="AI21" s="5" t="n">
+        <v>6393261376.09245</v>
+      </c>
+      <c r="AJ21" s="5" t="n">
+        <v>5973325868.1803</v>
+      </c>
+      <c r="AK21" s="5" t="n">
+        <v>4131119424.09102</v>
+      </c>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+    </row>
+    <row r="22">
+      <c r="M22" t="s">
+        <v>92</v>
+      </c>
+      <c r="N22" s="5" t="n">
+        <v>208971085.815995</v>
+      </c>
+      <c r="O22" s="5" t="n">
+        <v>307941776.479793</v>
+      </c>
+      <c r="P22" s="5" t="n">
+        <v>239415426.262249</v>
+      </c>
+      <c r="Q22" s="5" t="n">
+        <v>856531650.811007</v>
+      </c>
+      <c r="R22" s="5" t="n">
+        <v>1084775058.12407</v>
+      </c>
+      <c r="S22" s="5" t="n">
+        <v>1168816845.26415</v>
+      </c>
+      <c r="T22" s="5" t="n">
+        <v>1219882717.87</v>
+      </c>
+      <c r="U22" s="5" t="n">
+        <v>600849118.924373</v>
+      </c>
+      <c r="V22" s="5" t="n">
+        <v>1571243352.16923</v>
+      </c>
+      <c r="W22" s="5" t="n">
+        <v>1972997912.92211</v>
+      </c>
+      <c r="X22" s="5" t="n">
+        <v>1384780282.39697</v>
+      </c>
+      <c r="Y22" s="5" t="n">
+        <v>1719498087.49134</v>
+      </c>
+      <c r="Z22" s="5" t="n">
+        <v>4386534296.27815</v>
+      </c>
+      <c r="AA22" s="5" t="n">
+        <v>2138758534.20208</v>
+      </c>
+      <c r="AB22" s="5" t="n">
+        <v>2338658005.30604</v>
+      </c>
+      <c r="AC22" s="5" t="n">
+        <v>2783961971.84965</v>
+      </c>
+      <c r="AD22" s="5" t="n">
+        <v>2460401862.83874</v>
+      </c>
+      <c r="AE22" s="5" t="n">
+        <v>3243454289.9308</v>
+      </c>
+      <c r="AF22" s="5" t="n">
+        <v>2337170958.00125</v>
+      </c>
+      <c r="AG22" s="5" t="n">
+        <v>3153441635.69283</v>
+      </c>
+      <c r="AH22" s="5" t="n">
+        <v>2691773540.02993</v>
+      </c>
+      <c r="AI22" s="5" t="n">
+        <v>2275568242.10892</v>
+      </c>
+      <c r="AJ22" s="5" t="n">
+        <v>2158416643.1052</v>
+      </c>
+      <c r="AK22" s="5" t="n">
+        <v>1873581282.57495</v>
+      </c>
+      <c r="AL22" s="5"/>
+      <c r="AM22" s="5"/>
+    </row>
+    <row r="23">
+      <c r="M23" t="s">
+        <v>93</v>
+      </c>
+      <c r="N23" s="5" t="n">
+        <v>1553031472.30476</v>
+      </c>
+      <c r="O23" s="5" t="n">
+        <v>1676042079.19008</v>
+      </c>
+      <c r="P23" s="5" t="n">
+        <v>1717129026.05777</v>
+      </c>
+      <c r="Q23" s="5" t="n">
+        <v>2385110522.59256</v>
+      </c>
+      <c r="R23" s="5" t="n">
+        <v>1928224917.0966</v>
+      </c>
+      <c r="S23" s="5" t="n">
+        <v>2005395229.84898</v>
+      </c>
+      <c r="T23" s="5" t="n">
+        <v>2804989584.53146</v>
+      </c>
+      <c r="U23" s="5" t="n">
+        <v>3036107416.52311</v>
+      </c>
+      <c r="V23" s="5" t="n">
+        <v>4352665851.54259</v>
+      </c>
+      <c r="W23" s="5" t="n">
+        <v>4036849156.91</v>
+      </c>
+      <c r="X23" s="5" t="n">
+        <v>4446509606.85328</v>
+      </c>
+      <c r="Y23" s="5" t="n">
+        <v>5057068251.30156</v>
+      </c>
+      <c r="Z23" s="5" t="n">
+        <v>4573504400.70608</v>
+      </c>
+      <c r="AA23" s="5" t="n">
+        <v>4832515705.14841</v>
+      </c>
+      <c r="AB23" s="5" t="n">
+        <v>3240592845.4091</v>
+      </c>
+      <c r="AC23" s="5" t="n">
+        <v>3585419531.63662</v>
+      </c>
+      <c r="AD23" s="5" t="n">
+        <v>5028694968.26248</v>
+      </c>
+      <c r="AE23" s="5" t="n">
+        <v>6191508475.21686</v>
+      </c>
+      <c r="AF23" s="5" t="n">
+        <v>5266789338.83552</v>
+      </c>
+      <c r="AG23" s="5" t="n">
+        <v>7085698328.7213</v>
+      </c>
+      <c r="AH23" s="5" t="n">
+        <v>5685664947.24677</v>
+      </c>
+      <c r="AI23" s="5" t="n">
+        <v>4316162786.44899</v>
+      </c>
+      <c r="AJ23" s="5" t="n">
+        <v>4162714111.4593</v>
+      </c>
+      <c r="AK23" s="5" t="n">
+        <v>3146888791.11777</v>
+      </c>
+      <c r="AL23" s="5"/>
+      <c r="AM23" s="5"/>
+    </row>
+    <row r="24">
+      <c r="M24" t="s">
+        <v>94</v>
+      </c>
+      <c r="N24" s="5" t="n">
+        <v>22378282149.9945</v>
+      </c>
+      <c r="O24" s="5" t="n">
+        <v>21896565583.6864</v>
+      </c>
+      <c r="P24" s="5" t="n">
+        <v>20942813367.6658</v>
+      </c>
+      <c r="Q24" s="5" t="n">
+        <v>26670470728.3889</v>
+      </c>
+      <c r="R24" s="5" t="n">
+        <v>23104572533.4021</v>
+      </c>
+      <c r="S24" s="5" t="n">
+        <v>22078078641.2318</v>
+      </c>
+      <c r="T24" s="5" t="n">
+        <v>21101663139.4752</v>
+      </c>
+      <c r="U24" s="5" t="n">
+        <v>22665785378.7248</v>
+      </c>
+      <c r="V24" s="5" t="n">
+        <v>24587328746.8782</v>
+      </c>
+      <c r="W24" s="5" t="n">
+        <v>26626130162.8692</v>
+      </c>
+      <c r="X24" s="5" t="n">
+        <v>27457875389.2552</v>
+      </c>
+      <c r="Y24" s="5" t="n">
+        <v>26999743827.1296</v>
+      </c>
+      <c r="Z24" s="5" t="n">
+        <v>27544581173.9108</v>
+      </c>
+      <c r="AA24" s="5" t="n">
+        <v>22034937225.0528</v>
+      </c>
+      <c r="AB24" s="5" t="n">
+        <v>19815425082.7614</v>
+      </c>
+      <c r="AC24" s="5" t="n">
+        <v>21329177052.3883</v>
+      </c>
+      <c r="AD24" s="5" t="n">
+        <v>23178278330.5816</v>
+      </c>
+      <c r="AE24" s="5" t="n">
+        <v>27669787444.9197</v>
+      </c>
+      <c r="AF24" s="5" t="n">
+        <v>27921741907.242</v>
+      </c>
+      <c r="AG24" s="5" t="n">
+        <v>28864812210.4964</v>
+      </c>
+      <c r="AH24" s="5" t="n">
+        <v>26732449807.1811</v>
+      </c>
+      <c r="AI24" s="5" t="n">
+        <v>23535368226.0464</v>
+      </c>
+      <c r="AJ24" s="5" t="n">
+        <v>22979854523.3634</v>
+      </c>
+      <c r="AK24" s="5" t="n">
+        <v>12942870548.4963</v>
+      </c>
+      <c r="AL24" s="5"/>
+      <c r="AM24" s="5"/>
+    </row>
+    <row r="25">
+      <c r="M25"/>
+      <c r="N25" s="5" t="n">
+        <v>6150.32490634784</v>
+      </c>
+      <c r="O25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="5" t="n">
+        <v>14770.4446194157</v>
+      </c>
+      <c r="Q25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="5"/>
+      <c r="AJ25" s="5"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="5"/>
+      <c r="AM25" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rerun with wider right margin.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/Platform/Aircraft/DoD_Aircraft_Contracts.xlsx
+++ b/Output/AcqTrends/Platform/Aircraft/DoD_Aircraft_Contracts.xlsx
@@ -1344,14 +1344,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
     <numFmt numFmtId="193" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="194" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="195" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="168" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="189" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="191" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="180" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="192" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="195" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="196" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1390,7 +1390,7 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="193" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -1398,7 +1398,7 @@
     <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="192" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="196" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2862,11 +2862,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" xSplit="2" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="str">
+        <f>M1</f>
+      </c>
+      <c r="B1" t="str">
+        <f>N1</f>
+      </c>
       <c r="M1" t="s">
         <v>39</v>
       </c>
@@ -2977,700 +2986,870 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <f>M2</f>
+      </c>
+      <c r="B2" t="str">
+        <f>N2</f>
+      </c>
       <c r="M2" t="s">
         <v>41</v>
       </c>
       <c r="N2" t="s">
         <v>41</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2" s="10" t="n">
         <v>16391574000</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2" s="10" t="n">
         <v>17838245000</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2" s="10" t="n">
         <v>17454681932</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2" s="10" t="n">
         <v>17653003009</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2" s="10" t="n">
         <v>19673358698</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T2" s="10" t="n">
         <v>15723011307</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U2" s="10" t="n">
         <v>18138145959</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2" s="10" t="n">
         <v>14850717460</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2" s="10" t="n">
         <v>13963015456</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2" s="10" t="n">
         <v>15528455039</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Y2" s="10" t="n">
         <v>17363817617</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="Z2" s="10" t="n">
         <v>18760776804</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AA2" s="10" t="n">
         <v>21403163432.8184</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AB2" s="10" t="n">
         <v>25629544247.232</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AC2" s="10" t="n">
         <v>22537651820.4586</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AD2" s="10" t="n">
         <v>20274951982.0621</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AE2" s="10" t="n">
         <v>24943309183.8877</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2" s="10" t="n">
         <v>29692705322.6938</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2" s="10" t="n">
         <v>26233268759.7976</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2" s="10" t="n">
         <v>26298821053.0011</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2" s="10" t="n">
         <v>26738380644.2979</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AJ2" s="10" t="n">
         <v>27511723187.9643</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AK2" s="10" t="n">
         <v>32198894439.3838</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AL2" s="10" t="n">
         <v>24165194566.5125</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="AM2" s="10" t="n">
         <v>22912994163.6177</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AN2" s="10" t="n">
         <v>21859111644.8921</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AO2" s="10" t="n">
         <v>29547016396.6323</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AP2" s="10" t="n">
         <v>25129507305.3762</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AQ2" s="10" t="n">
         <v>29103178713.6169</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AR2" s="10" t="n">
         <v>29875200240.767</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AS2" s="10" t="n">
         <v>30619881506.4275</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="AT2" s="10" t="n">
         <v>28662616164.5242</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AU2" s="10" t="n">
         <v>25168814866.1088</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AV2" s="10" t="n">
         <v>15135793787.3224</v>
       </c>
+      <c r="AW2" s="10"/>
     </row>
     <row r="3">
+      <c r="A3" t="str">
+        <f>M3</f>
+      </c>
+      <c r="B3" t="str">
+        <f>N3</f>
+      </c>
       <c r="M3" t="s">
         <v>42</v>
       </c>
       <c r="N3" t="s">
         <v>42</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3" s="10" t="n">
         <v>4614277000</v>
       </c>
-      <c r="P3" t="n">
+      <c r="P3" s="10" t="n">
         <v>3662072000</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q3" s="10" t="n">
         <v>3458743985</v>
       </c>
-      <c r="R3" t="n">
+      <c r="R3" s="10" t="n">
         <v>3343825705</v>
       </c>
-      <c r="S3" t="n">
+      <c r="S3" s="10" t="n">
         <v>2357211931</v>
       </c>
-      <c r="T3" t="n">
+      <c r="T3" s="10" t="n">
         <v>2690270705</v>
       </c>
-      <c r="U3" t="n">
+      <c r="U3" s="10" t="n">
         <v>2498599569</v>
       </c>
-      <c r="V3" t="n">
+      <c r="V3" s="10" t="n">
         <v>1621683927</v>
       </c>
-      <c r="W3" t="n">
+      <c r="W3" s="10" t="n">
         <v>2381316058</v>
       </c>
-      <c r="X3" t="n">
+      <c r="X3" s="10" t="n">
         <v>2797805602</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="Y3" s="10" t="n">
         <v>7826824197.53</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="Z3" s="10" t="n">
         <v>7740161769.25</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AA3" s="10" t="n">
         <v>6120423016.6201</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AB3" s="10" t="n">
         <v>7292829557</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AC3" s="10" t="n">
         <v>9158613871.1189</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AD3" s="10" t="n">
         <v>8202415157.6841</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AE3" s="10" t="n">
         <v>8289438845.8463</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AF3" s="10" t="n">
         <v>8863031258.9926</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AG3" s="10" t="n">
         <v>13426758395.7341</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AH3" s="10" t="n">
         <v>10720767225.5465</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AI3" s="10" t="n">
         <v>10814501824.1502</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AJ3" s="10" t="n">
         <v>12332377029.733</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="AK3" s="10" t="n">
         <v>14454946861.0917</v>
       </c>
-      <c r="AL3" t="n">
+      <c r="AL3" s="10" t="n">
         <v>12189508660.0373</v>
       </c>
-      <c r="AM3" t="n">
+      <c r="AM3" s="10" t="n">
         <v>9618295813.6203</v>
       </c>
-      <c r="AN3" t="n">
+      <c r="AN3" s="10" t="n">
         <v>9124715224.1509</v>
       </c>
-      <c r="AO3" t="n">
+      <c r="AO3" s="10" t="n">
         <v>11237165287.6543</v>
       </c>
-      <c r="AP3" t="n">
+      <c r="AP3" s="10" t="n">
         <v>11300540308.5238</v>
       </c>
-      <c r="AQ3" t="n">
+      <c r="AQ3" s="10" t="n">
         <v>9660629680.1112</v>
       </c>
-      <c r="AR3" t="n">
+      <c r="AR3" s="10" t="n">
         <v>9219671762.8742</v>
       </c>
-      <c r="AS3" t="n">
+      <c r="AS3" s="10" t="n">
         <v>9731411012.4712</v>
       </c>
-      <c r="AT3" t="n">
+      <c r="AT3" s="10" t="n">
         <v>6995611243.5556</v>
       </c>
-      <c r="AU3" t="n">
+      <c r="AU3" s="10" t="n">
         <v>5872197067.0852</v>
       </c>
-      <c r="AV3" t="n">
+      <c r="AV3" s="10" t="n">
         <v>6213962336.3561</v>
       </c>
+      <c r="AW3" s="10"/>
     </row>
     <row r="4">
+      <c r="A4" t="str">
+        <f>M4</f>
+      </c>
+      <c r="B4" t="str">
+        <f>N4</f>
+      </c>
       <c r="M4" t="s">
         <v>43</v>
       </c>
       <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O4" s="10" t="n">
         <v>133371000</v>
       </c>
-      <c r="P4" t="n">
+      <c r="P4" s="10" t="n">
         <v>281502000</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4" s="10" t="n">
         <v>172805706</v>
       </c>
-      <c r="R4" t="n">
+      <c r="R4" s="10" t="n">
         <v>135194064</v>
       </c>
-      <c r="S4" t="n">
+      <c r="S4" s="10" t="n">
         <v>191192468</v>
       </c>
-      <c r="T4" t="n">
+      <c r="T4" s="10" t="n">
         <v>303867690</v>
       </c>
-      <c r="U4" t="n">
+      <c r="U4" s="10" t="n">
         <v>422215119</v>
       </c>
-      <c r="V4" t="n">
+      <c r="V4" s="10" t="n">
         <v>630009186</v>
       </c>
-      <c r="W4" t="n">
+      <c r="W4" s="10" t="n">
         <v>770315247</v>
       </c>
-      <c r="X4" t="n">
+      <c r="X4" s="10" t="n">
         <v>1002509479</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="Y4" s="10" t="n">
         <v>1308847901</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="Z4" s="10" t="n">
         <v>1590494100</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AA4" s="10" t="n">
         <v>1829325311</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AB4" s="10" t="n">
         <v>1778040618</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AC4" s="10" t="n">
         <v>1591548738</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AD4" s="10" t="n">
         <v>1959610013</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AE4" s="10" t="n">
         <v>2254774860.129</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AF4" s="10" t="n">
         <v>1646689399.2673</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="AG4" s="10" t="n">
         <v>2811895990.9985</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AH4" s="10" t="n">
         <v>3466416632.9502</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AI4" s="10" t="n">
         <v>4573260762.5403</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AJ4" s="10" t="n">
         <v>4507333597.5953</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AK4" s="10" t="n">
         <v>4757126009.3412</v>
       </c>
-      <c r="AL4" t="n">
+      <c r="AL4" s="10" t="n">
         <v>3860264713.0309</v>
       </c>
-      <c r="AM4" t="n">
+      <c r="AM4" s="10" t="n">
         <v>4078470507.3136</v>
       </c>
-      <c r="AN4" t="n">
+      <c r="AN4" s="10" t="n">
         <v>4040399395.0495</v>
       </c>
-      <c r="AO4" t="n">
+      <c r="AO4" s="10" t="n">
         <v>4768761642.2886</v>
       </c>
-      <c r="AP4" t="n">
+      <c r="AP4" s="10" t="n">
         <v>6122532461.5931</v>
       </c>
-      <c r="AQ4" t="n">
+      <c r="AQ4" s="10" t="n">
         <v>8269284407.4819</v>
       </c>
-      <c r="AR4" t="n">
+      <c r="AR4" s="10" t="n">
         <v>8722529680.0504</v>
       </c>
-      <c r="AS4" t="n">
+      <c r="AS4" s="10" t="n">
         <v>7330502462.9696</v>
       </c>
-      <c r="AT4" t="n">
+      <c r="AT4" s="10" t="n">
         <v>5460413161.1389</v>
       </c>
-      <c r="AU4" t="n">
+      <c r="AU4" s="10" t="n">
         <v>6100214031.6176</v>
       </c>
-      <c r="AV4" t="n">
+      <c r="AV4" s="10" t="n">
         <v>2087688800.7209</v>
       </c>
+      <c r="AW4" s="10"/>
     </row>
     <row r="5">
+      <c r="A5" t="str">
+        <f>M5</f>
+      </c>
+      <c r="B5" t="str">
+        <f>N5</f>
+      </c>
       <c r="M5" t="s">
         <v>45</v>
       </c>
       <c r="N5" t="s">
         <v>46</v>
       </c>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5" t="n">
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10" t="n">
         <v>82828871</v>
       </c>
-      <c r="W5" t="n">
+      <c r="W5" s="10" t="n">
         <v>650715792</v>
       </c>
-      <c r="X5" t="n">
+      <c r="X5" s="10" t="n">
         <v>693041844</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="Y5" s="10" t="n">
         <v>178031456</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="Z5" s="10" t="n">
         <v>268635741</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AA5" s="10" t="n">
         <v>6554622</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AB5" s="10" t="n">
         <v>239927692</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AC5" s="10" t="n">
         <v>196180517.0938</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AD5" s="10" t="n">
         <v>297828366</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AE5" s="10" t="n">
         <v>634208169</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AF5" s="10" t="n">
         <v>1065862766.7227</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AG5" s="10" t="n">
         <v>2725377126.3311</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AH5" s="10" t="n">
         <v>3681464062.0067</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AI5" s="10" t="n">
         <v>1874856013.4357</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AJ5" s="10" t="n">
         <v>4877655064.5174</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="AK5" s="10" t="n">
         <v>4691798600.1306</v>
       </c>
-      <c r="AL5" t="n">
+      <c r="AL5" s="10" t="n">
         <v>12181364143.38</v>
       </c>
-      <c r="AM5" t="n">
+      <c r="AM5" s="10" t="n">
         <v>3796342018.2</v>
       </c>
-      <c r="AN5" t="n">
+      <c r="AN5" s="10" t="n">
         <v>11389818543.0914</v>
       </c>
-      <c r="AO5" t="n">
+      <c r="AO5" s="10" t="n">
         <v>10143588537.0827</v>
       </c>
-      <c r="AP5" t="n">
+      <c r="AP5" s="10" t="n">
         <v>24140285523.0243</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="AQ5" s="10" t="n">
         <v>15993414967.9989</v>
       </c>
-      <c r="AR5" t="n">
+      <c r="AR5" s="10" t="n">
         <v>17244736490.1055</v>
       </c>
-      <c r="AS5" t="n">
+      <c r="AS5" s="10" t="n">
         <v>35959136464.6929</v>
       </c>
-      <c r="AT5" t="n">
+      <c r="AT5" s="10" t="n">
         <v>9846932233.464</v>
       </c>
-      <c r="AU5" t="n">
+      <c r="AU5" s="10" t="n">
         <v>20737931632.3383</v>
       </c>
-      <c r="AV5" t="n">
+      <c r="AV5" s="10" t="n">
         <v>18232001549.4868</v>
       </c>
+      <c r="AW5" s="10"/>
     </row>
     <row r="6">
+      <c r="A6" t="str">
+        <f>M6</f>
+      </c>
+      <c r="B6" t="str">
+        <f>N6</f>
+      </c>
       <c r="M6" t="s">
         <v>47</v>
       </c>
       <c r="N6" t="s">
         <v>44</v>
       </c>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-      <c r="AF6"/>
-      <c r="AG6"/>
-      <c r="AH6"/>
-      <c r="AI6"/>
-      <c r="AJ6"/>
-      <c r="AK6"/>
-      <c r="AL6"/>
-      <c r="AM6"/>
-      <c r="AN6"/>
-      <c r="AO6"/>
-      <c r="AP6"/>
-      <c r="AQ6" t="n">
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10" t="n">
         <v>1015462.3203</v>
       </c>
-      <c r="AR6" t="n">
+      <c r="AR6" s="10" t="n">
         <v>301794.4688</v>
       </c>
-      <c r="AS6" t="n">
+      <c r="AS6" s="10" t="n">
         <v>-18449.4502</v>
       </c>
-      <c r="AT6"/>
-      <c r="AU6"/>
-      <c r="AV6"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
+      <c r="AW6" s="10"/>
     </row>
     <row r="7">
+      <c r="A7" t="str">
+        <f>M7</f>
+      </c>
+      <c r="B7" t="str">
+        <f>N7</f>
+      </c>
       <c r="M7" t="s">
         <v>46</v>
       </c>
       <c r="N7" t="s">
         <v>46</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O7" s="10" t="n">
         <v>9839685148</v>
       </c>
-      <c r="P7" t="n">
+      <c r="P7" s="10" t="n">
         <v>8725297255</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7" s="10" t="n">
         <v>9244808172</v>
       </c>
-      <c r="R7" t="n">
+      <c r="R7" s="10" t="n">
         <v>8776733718</v>
       </c>
-      <c r="S7" t="n">
+      <c r="S7" s="10" t="n">
         <v>8271683151</v>
       </c>
-      <c r="T7" t="n">
+      <c r="T7" s="10" t="n">
         <v>8065718595</v>
       </c>
-      <c r="U7" t="n">
+      <c r="U7" s="10" t="n">
         <v>7748869942</v>
       </c>
-      <c r="V7" t="n">
+      <c r="V7" s="10" t="n">
         <v>7669461587</v>
       </c>
-      <c r="W7" t="n">
+      <c r="W7" s="10" t="n">
         <v>8622122558</v>
       </c>
-      <c r="X7" t="n">
+      <c r="X7" s="10" t="n">
         <v>7365752543</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="Y7" s="10" t="n">
         <v>8583593857</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="Z7" s="10" t="n">
         <v>7604791151.6894</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AA7" s="10" t="n">
         <v>9422425825.7277</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AB7" s="10" t="n">
         <v>14006118686.9454</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AC7" s="10" t="n">
         <v>13871568112.8849</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AD7" s="10" t="n">
         <v>16110986465.9325</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AE7" s="10" t="n">
         <v>17411796629.8726</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AF7" s="10" t="n">
         <v>18665566187.1937</v>
       </c>
-      <c r="AG7" t="n">
+      <c r="AG7" s="10" t="n">
         <v>20745443146.4835</v>
       </c>
-      <c r="AH7" t="n">
+      <c r="AH7" s="10" t="n">
         <v>20805440988.6384</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AI7" s="10" t="n">
         <v>18902019133.4777</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AJ7" s="10" t="n">
         <v>20085402335.649</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="AK7" s="10" t="n">
         <v>21343379088.1912</v>
       </c>
-      <c r="AL7" t="n">
+      <c r="AL7" s="10" t="n">
         <v>20335319881.8431</v>
       </c>
-      <c r="AM7" t="n">
+      <c r="AM7" s="10" t="n">
         <v>17361208695.2696</v>
       </c>
-      <c r="AN7" t="n">
+      <c r="AN7" s="10" t="n">
         <v>14802780312.6182</v>
       </c>
-      <c r="AO7" t="n">
+      <c r="AO7" s="10" t="n">
         <v>19086196037.5947</v>
       </c>
-      <c r="AP7" t="n">
+      <c r="AP7" s="10" t="n">
         <v>18630360546.2453</v>
       </c>
-      <c r="AQ7" t="n">
+      <c r="AQ7" s="10" t="n">
         <v>19276599690.8854</v>
       </c>
-      <c r="AR7" t="n">
+      <c r="AR7" s="10" t="n">
         <v>24058676107.9643</v>
       </c>
-      <c r="AS7" t="n">
+      <c r="AS7" s="10" t="n">
         <v>20671618344.8429</v>
       </c>
-      <c r="AT7" t="n">
+      <c r="AT7" s="10" t="n">
         <v>19902451920.0744</v>
       </c>
-      <c r="AU7" t="n">
+      <c r="AU7" s="10" t="n">
         <v>16116608567.0774</v>
       </c>
-      <c r="AV7" t="n">
+      <c r="AV7" s="10" t="n">
         <v>7762302832.3832</v>
       </c>
+      <c r="AW7" s="10"/>
     </row>
     <row r="8">
+      <c r="A8" t="str">
+        <f>M8</f>
+      </c>
+      <c r="B8" t="str">
+        <f>N8</f>
+      </c>
       <c r="M8" t="s">
         <v>44</v>
       </c>
       <c r="N8" t="s">
         <v>44</v>
       </c>
-      <c r="O8" t="n">
+      <c r="O8" s="10" t="n">
         <v>1340000</v>
       </c>
-      <c r="P8" t="n">
+      <c r="P8" s="10" t="n">
         <v>5983000</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8" s="10" t="n">
         <v>6931772</v>
       </c>
-      <c r="R8" t="n">
+      <c r="R8" s="10" t="n">
         <v>9288369</v>
       </c>
-      <c r="S8" t="n">
+      <c r="S8" s="10" t="n">
         <v>53514157</v>
       </c>
-      <c r="T8" t="n">
+      <c r="T8" s="10" t="n">
         <v>32637021</v>
       </c>
-      <c r="U8" t="n">
+      <c r="U8" s="10" t="n">
         <v>48175601</v>
       </c>
-      <c r="V8" t="n">
+      <c r="V8" s="10" t="n">
         <v>76132888</v>
       </c>
-      <c r="W8" t="n">
+      <c r="W8" s="10" t="n">
         <v>142284958</v>
       </c>
-      <c r="X8" t="n">
+      <c r="X8" s="10" t="n">
         <v>157809624</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="Y8" s="10" t="n">
         <v>159223036</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="Z8" s="10" t="n">
         <v>156986482</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AA8" s="10" t="n">
         <v>243997353</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AB8" s="10" t="n">
         <v>298559385.2793</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AC8" s="10" t="n">
         <v>446563505.4219</v>
       </c>
-      <c r="AD8" t="n">
+      <c r="AD8" s="10" t="n">
         <v>436806742.4048</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AE8" s="10" t="n">
         <v>439450292.5452</v>
       </c>
-      <c r="AF8" t="n">
+      <c r="AF8" s="10" t="n">
         <v>548075907.8659</v>
       </c>
-      <c r="AG8" t="n">
+      <c r="AG8" s="10" t="n">
         <v>783992050.5508</v>
       </c>
-      <c r="AH8" t="n">
+      <c r="AH8" s="10" t="n">
         <v>876739854.4475</v>
       </c>
-      <c r="AI8" t="n">
+      <c r="AI8" s="10" t="n">
         <v>699572561.0923</v>
       </c>
-      <c r="AJ8" t="n">
+      <c r="AJ8" s="10" t="n">
         <v>988302677.766</v>
       </c>
-      <c r="AK8" t="n">
+      <c r="AK8" s="10" t="n">
         <v>717963643.5507</v>
       </c>
-      <c r="AL8" t="n">
+      <c r="AL8" s="10" t="n">
         <v>527056324.566</v>
       </c>
-      <c r="AM8" t="n">
+      <c r="AM8" s="10" t="n">
         <v>455132079.1202</v>
       </c>
-      <c r="AN8" t="n">
+      <c r="AN8" s="10" t="n">
         <v>476334952.41</v>
       </c>
-      <c r="AO8" t="n">
+      <c r="AO8" s="10" t="n">
         <v>563412721.532</v>
       </c>
-      <c r="AP8" t="n">
+      <c r="AP8" s="10" t="n">
         <v>499320224.9645</v>
       </c>
-      <c r="AQ8" t="n">
+      <c r="AQ8" s="10" t="n">
         <v>1034658252.0193</v>
       </c>
-      <c r="AR8" t="n">
+      <c r="AR8" s="10" t="n">
         <v>966667303.177</v>
       </c>
-      <c r="AS8" t="n">
+      <c r="AS8" s="10" t="n">
         <v>997906571.9839</v>
       </c>
-      <c r="AT8" t="n">
+      <c r="AT8" s="10" t="n">
         <v>1626773802.8944</v>
       </c>
-      <c r="AU8" t="n">
+      <c r="AU8" s="10" t="n">
         <v>1134739642.0035</v>
       </c>
-      <c r="AV8" t="n">
+      <c r="AV8" s="10" t="n">
         <v>817139802.2437</v>
       </c>
+      <c r="AW8" s="10"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <f>M9</f>
+      </c>
+      <c r="B9" t="str">
+        <f>N9</f>
+      </c>
+      <c r="M9" t="s">
+        <v>433</v>
+      </c>
+      <c r="N9" t="s">
+        <v>434</v>
+      </c>
+      <c r="O9" s="10" t="str">
+        <f>Sum(O2:O8)</f>
+      </c>
+      <c r="P9" s="10" t="str">
+        <f>Sum(P2:P8)</f>
+      </c>
+      <c r="Q9" s="10" t="str">
+        <f>Sum(Q2:Q8)</f>
+      </c>
+      <c r="R9" s="10" t="str">
+        <f>Sum(R2:R8)</f>
+      </c>
+      <c r="S9" s="10" t="str">
+        <f>Sum(S2:S8)</f>
+      </c>
+      <c r="T9" s="10" t="str">
+        <f>Sum(T2:T8)</f>
+      </c>
+      <c r="U9" s="10" t="str">
+        <f>Sum(U2:U8)</f>
+      </c>
+      <c r="V9" s="10" t="str">
+        <f>Sum(V2:V8)</f>
+      </c>
+      <c r="W9" s="10" t="str">
+        <f>Sum(W2:W8)</f>
+      </c>
+      <c r="X9" s="10" t="str">
+        <f>Sum(X2:X8)</f>
+      </c>
+      <c r="Y9" s="10" t="str">
+        <f>Sum(Y2:Y8)</f>
+      </c>
+      <c r="Z9" s="10" t="str">
+        <f>Sum(Z2:Z8)</f>
+      </c>
+      <c r="AA9" s="10" t="str">
+        <f>Sum(AA2:AA8)</f>
+      </c>
+      <c r="AB9" s="10" t="str">
+        <f>Sum(AB2:AB8)</f>
+      </c>
+      <c r="AC9" s="10" t="str">
+        <f>Sum(AC2:AC8)</f>
+      </c>
+      <c r="AD9" s="10" t="str">
+        <f>Sum(AD2:AD8)</f>
+      </c>
+      <c r="AE9" s="10" t="str">
+        <f>Sum(AE2:AE8)</f>
+      </c>
+      <c r="AF9" s="10" t="str">
+        <f>Sum(AF2:AF8)</f>
+      </c>
+      <c r="AG9" s="10" t="str">
+        <f>Sum(AG2:AG8)</f>
+      </c>
+      <c r="AH9" s="10" t="str">
+        <f>Sum(AH2:AH8)</f>
+      </c>
+      <c r="AI9" s="10" t="str">
+        <f>Sum(AI2:AI8)</f>
+      </c>
+      <c r="AJ9" s="10" t="str">
+        <f>Sum(AJ2:AJ8)</f>
+      </c>
+      <c r="AK9" s="10" t="str">
+        <f>Sum(AK2:AK8)</f>
+      </c>
+      <c r="AL9" s="10" t="str">
+        <f>Sum(AL2:AL8)</f>
+      </c>
+      <c r="AM9" s="10" t="str">
+        <f>Sum(AM2:AM8)</f>
+      </c>
+      <c r="AN9" s="10" t="str">
+        <f>Sum(AN2:AN8)</f>
+      </c>
+      <c r="AO9" s="10" t="str">
+        <f>Sum(AO2:AO8)</f>
+      </c>
+      <c r="AP9" s="10" t="str">
+        <f>Sum(AP2:AP8)</f>
+      </c>
+      <c r="AQ9" s="10" t="str">
+        <f>Sum(AQ2:AQ8)</f>
+      </c>
+      <c r="AR9" s="10" t="str">
+        <f>Sum(AR2:AR8)</f>
+      </c>
+      <c r="AS9" s="10" t="str">
+        <f>Sum(AS2:AS8)</f>
+      </c>
+      <c r="AT9" s="10" t="str">
+        <f>Sum(AT2:AT8)</f>
+      </c>
+      <c r="AU9" s="10" t="str">
+        <f>Sum(AU2:AU8)</f>
+      </c>
+      <c r="AV9" s="10"/>
+      <c r="AW9" s="10"/>
     </row>
     <row r="12">
+      <c r="A12" t="str">
+        <f>M12</f>
+      </c>
+      <c r="B12" t="str">
+        <f>N12</f>
+      </c>
       <c r="M12" t="s">
         <v>39</v>
       </c>
@@ -3781,698 +3960,790 @@
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="str">
+        <f>M13</f>
+      </c>
+      <c r="B13" t="str">
+        <f>N13</f>
+      </c>
       <c r="M13" t="s">
         <v>41</v>
       </c>
       <c r="N13" t="s">
         <v>41</v>
       </c>
-      <c r="O13" t="n">
+      <c r="O13" s="10" t="n">
         <v>32578770750.4035</v>
       </c>
-      <c r="P13" t="n">
+      <c r="P13" s="10" t="n">
         <v>34233011196.1922</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="Q13" s="10" t="n">
         <v>32680167910.4111</v>
       </c>
-      <c r="R13" t="n">
+      <c r="R13" s="10" t="n">
         <v>32292891786.3862</v>
       </c>
-      <c r="S13" t="n">
+      <c r="S13" s="10" t="n">
         <v>35221297408.3438</v>
       </c>
-      <c r="T13" t="n">
+      <c r="T13" s="10" t="n">
         <v>27565067708.4042</v>
       </c>
-      <c r="U13" t="n">
+      <c r="U13" s="10" t="n">
         <v>31212581603.6682</v>
       </c>
-      <c r="V13" t="n">
+      <c r="V13" s="10" t="n">
         <v>25109436745.9672</v>
       </c>
-      <c r="W13" t="n">
+      <c r="W13" s="10" t="n">
         <v>23317365549.6106</v>
       </c>
-      <c r="X13" t="n">
+      <c r="X13" s="10" t="n">
         <v>25612290032.7132</v>
       </c>
-      <c r="Y13" t="n">
+      <c r="Y13" s="10" t="n">
         <v>28055241902.4982</v>
       </c>
-      <c r="Z13" t="n">
+      <c r="Z13" s="10" t="n">
         <v>29594696533.2138</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AA13" s="10" t="n">
         <v>33238381688.0567</v>
       </c>
-      <c r="AB13" t="n">
+      <c r="AB13" s="10" t="n">
         <v>39055282049.7854</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AC13" s="10" t="n">
         <v>33524291200.0479</v>
       </c>
-      <c r="AD13" t="n">
+      <c r="AD13" s="10" t="n">
         <v>29270029845.4708</v>
       </c>
-      <c r="AE13" t="n">
+      <c r="AE13" s="10" t="n">
         <v>34874108181.5704</v>
       </c>
-      <c r="AF13" t="n">
+      <c r="AF13" s="10" t="n">
         <v>40406336513.8607</v>
       </c>
-      <c r="AG13" t="n">
+      <c r="AG13" s="10" t="n">
         <v>34969360998.7981</v>
       </c>
-      <c r="AH13" t="n">
+      <c r="AH13" s="10" t="n">
         <v>34704081915.9793</v>
       </c>
-      <c r="AI13" t="n">
+      <c r="AI13" s="10" t="n">
         <v>34979890642.155</v>
       </c>
-      <c r="AJ13" t="n">
+      <c r="AJ13" s="10" t="n">
         <v>35280563131.1119</v>
       </c>
-      <c r="AK13" t="n">
+      <c r="AK13" s="10" t="n">
         <v>40548067759.7794</v>
       </c>
-      <c r="AL13" t="n">
+      <c r="AL13" s="10" t="n">
         <v>29884345972.7787</v>
       </c>
-      <c r="AM13" t="n">
+      <c r="AM13" s="10" t="n">
         <v>27798009206.378</v>
       </c>
-      <c r="AN13" t="n">
+      <c r="AN13" s="10" t="n">
         <v>26218858280.8993</v>
       </c>
-      <c r="AO13" t="n">
+      <c r="AO13" s="10" t="n">
         <v>35148835980.2508</v>
       </c>
-      <c r="AP13" t="n">
+      <c r="AP13" s="10" t="n">
         <v>29369455745.1911</v>
       </c>
-      <c r="AQ13" t="n">
+      <c r="AQ13" s="10" t="n">
         <v>33233254398.1494</v>
       </c>
-      <c r="AR13" t="n">
+      <c r="AR13" s="10" t="n">
         <v>33459480318.1899</v>
       </c>
-      <c r="AS13" t="n">
+      <c r="AS13" s="10" t="n">
         <v>33842036863.3378</v>
       </c>
-      <c r="AT13" t="n">
+      <c r="AT13" s="10" t="n">
         <v>30648579902.8023</v>
       </c>
-      <c r="AU13" t="n">
+      <c r="AU13" s="10" t="n">
         <v>25168814866.1088</v>
       </c>
-      <c r="AV13" t="n">
+      <c r="AV13" s="10" t="n">
         <v>14436495585.8153</v>
       </c>
+      <c r="AW13" s="10"/>
     </row>
     <row r="14">
+      <c r="A14" t="str">
+        <f>M14</f>
+      </c>
+      <c r="B14" t="str">
+        <f>N14</f>
+      </c>
       <c r="M14" t="s">
         <v>42</v>
       </c>
       <c r="N14" t="s">
         <v>42</v>
       </c>
-      <c r="O14" t="n">
+      <c r="O14" s="10" t="n">
         <v>9171021194.29528</v>
       </c>
-      <c r="P14" t="n">
+      <c r="P14" s="10" t="n">
         <v>7027807487.63468</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Q14" s="10" t="n">
         <v>6475760178.80337</v>
       </c>
-      <c r="R14" t="n">
+      <c r="R14" s="10" t="n">
         <v>6116908357.69129</v>
       </c>
-      <c r="S14" t="n">
+      <c r="S14" s="10" t="n">
         <v>4220126504.61599</v>
       </c>
-      <c r="T14" t="n">
+      <c r="T14" s="10" t="n">
         <v>4716494359.08285</v>
       </c>
-      <c r="U14" t="n">
+      <c r="U14" s="10" t="n">
         <v>4299653510.26442</v>
       </c>
-      <c r="V14" t="n">
+      <c r="V14" s="10" t="n">
         <v>2741926112.09763</v>
       </c>
-      <c r="W14" t="n">
+      <c r="W14" s="10" t="n">
         <v>3976649398.44236</v>
       </c>
-      <c r="X14" t="n">
+      <c r="X14" s="10" t="n">
         <v>4614638632.98718</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="Y14" s="10" t="n">
         <v>12646035050.2097</v>
       </c>
-      <c r="Z14" t="n">
+      <c r="Z14" s="10" t="n">
         <v>12209928249.3515</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AA14" s="10" t="n">
         <v>9504807873.72084</v>
       </c>
-      <c r="AB14" t="n">
+      <c r="AB14" s="10" t="n">
         <v>11113093254.4931</v>
       </c>
-      <c r="AC14" t="n">
+      <c r="AC14" s="10" t="n">
         <v>13623248812.7035</v>
       </c>
-      <c r="AD14" t="n">
+      <c r="AD14" s="10" t="n">
         <v>11841455244.0256</v>
       </c>
-      <c r="AE14" t="n">
+      <c r="AE14" s="10" t="n">
         <v>11589752784.7385</v>
       </c>
-      <c r="AF14" t="n">
+      <c r="AF14" s="10" t="n">
         <v>12060963111.7045</v>
       </c>
-      <c r="AG14" t="n">
+      <c r="AG14" s="10" t="n">
         <v>17898080703.6756</v>
       </c>
-      <c r="AH14" t="n">
+      <c r="AH14" s="10" t="n">
         <v>14147188698.9799</v>
       </c>
-      <c r="AI14" t="n">
+      <c r="AI14" s="10" t="n">
         <v>14147831022.0269</v>
       </c>
-      <c r="AJ14" t="n">
+      <c r="AJ14" s="10" t="n">
         <v>15814829314.0908</v>
       </c>
-      <c r="AK14" t="n">
+      <c r="AK14" s="10" t="n">
         <v>18203114578.6996</v>
       </c>
-      <c r="AL14" t="n">
+      <c r="AL14" s="10" t="n">
         <v>15074386967.2599</v>
       </c>
-      <c r="AM14" t="n">
+      <c r="AM14" s="10" t="n">
         <v>11668901657.6116</v>
       </c>
-      <c r="AN14" t="n">
+      <c r="AN14" s="10" t="n">
         <v>10944617475.8653</v>
       </c>
-      <c r="AO14" t="n">
+      <c r="AO14" s="10" t="n">
         <v>13367619737.8679</v>
       </c>
-      <c r="AP14" t="n">
+      <c r="AP14" s="10" t="n">
         <v>13207211524.4748</v>
       </c>
-      <c r="AQ14" t="n">
+      <c r="AQ14" s="10" t="n">
         <v>11031584108.5507</v>
       </c>
-      <c r="AR14" t="n">
+      <c r="AR14" s="10" t="n">
         <v>10325802786.3896</v>
       </c>
-      <c r="AS14" t="n">
+      <c r="AS14" s="10" t="n">
         <v>10755455410.4728</v>
       </c>
-      <c r="AT14" t="n">
+      <c r="AT14" s="10" t="n">
         <v>7480320321.64693</v>
       </c>
-      <c r="AU14" t="n">
+      <c r="AU14" s="10" t="n">
         <v>5872197067.0852</v>
       </c>
-      <c r="AV14" t="n">
+      <c r="AV14" s="10" t="n">
         <v>5926867206.28856</v>
       </c>
+      <c r="AW14" s="10"/>
     </row>
     <row r="15">
+      <c r="A15" t="str">
+        <f>M15</f>
+      </c>
+      <c r="B15" t="str">
+        <f>N15</f>
+      </c>
       <c r="M15" t="s">
         <v>43</v>
       </c>
       <c r="N15" t="s">
         <v>44</v>
       </c>
-      <c r="O15" t="n">
+      <c r="O15" s="10" t="n">
         <v>265079072.562041</v>
       </c>
-      <c r="P15" t="n">
+      <c r="P15" s="10" t="n">
         <v>540224731.62301</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="Q15" s="10" t="n">
         <v>323541815.884012</v>
       </c>
-      <c r="R15" t="n">
+      <c r="R15" s="10" t="n">
         <v>247312441.78047</v>
       </c>
-      <c r="S15" t="n">
+      <c r="S15" s="10" t="n">
         <v>342292685.302781</v>
       </c>
-      <c r="T15" t="n">
+      <c r="T15" s="10" t="n">
         <v>532730867.242795</v>
       </c>
-      <c r="U15" t="n">
+      <c r="U15" s="10" t="n">
         <v>726558485.408536</v>
       </c>
-      <c r="V15" t="n">
+      <c r="V15" s="10" t="n">
         <v>1065212899.50158</v>
       </c>
-      <c r="W15" t="n">
+      <c r="W15" s="10" t="n">
         <v>1286378451.65597</v>
       </c>
-      <c r="X15" t="n">
+      <c r="X15" s="10" t="n">
         <v>1653516945.00226</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="Y15" s="10" t="n">
         <v>2114744884.22301</v>
       </c>
-      <c r="Z15" t="n">
+      <c r="Z15" s="10" t="n">
         <v>2508968083.73794</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AA15" s="10" t="n">
         <v>2840879718.99555</v>
       </c>
-      <c r="AB15" t="n">
+      <c r="AB15" s="10" t="n">
         <v>2709446456.09391</v>
       </c>
-      <c r="AC15" t="n">
+      <c r="AC15" s="10" t="n">
         <v>2367395848.37082</v>
       </c>
-      <c r="AD15" t="n">
+      <c r="AD15" s="10" t="n">
         <v>2829000217.4476</v>
       </c>
-      <c r="AE15" t="n">
+      <c r="AE15" s="10" t="n">
         <v>3152479160.5445</v>
       </c>
-      <c r="AF15" t="n">
+      <c r="AF15" s="10" t="n">
         <v>2240842835.8917</v>
       </c>
-      <c r="AG15" t="n">
+      <c r="AG15" s="10" t="n">
         <v>3748301704.24627</v>
       </c>
-      <c r="AH15" t="n">
+      <c r="AH15" s="10" t="n">
         <v>4574304169.08704</v>
       </c>
-      <c r="AI15" t="n">
+      <c r="AI15" s="10" t="n">
         <v>5982866482.44845</v>
       </c>
-      <c r="AJ15" t="n">
+      <c r="AJ15" s="10" t="n">
         <v>5780127491.70545</v>
       </c>
-      <c r="AK15" t="n">
+      <c r="AK15" s="10" t="n">
         <v>5990648782.42036</v>
       </c>
-      <c r="AL15" t="n">
+      <c r="AL15" s="10" t="n">
         <v>4773869538.40585</v>
       </c>
-      <c r="AM15" t="n">
+      <c r="AM15" s="10" t="n">
         <v>4947994133.83799</v>
       </c>
-      <c r="AN15" t="n">
+      <c r="AN15" s="10" t="n">
         <v>4846247224.40576</v>
       </c>
-      <c r="AO15" t="n">
+      <c r="AO15" s="10" t="n">
         <v>5672871282.28683</v>
       </c>
-      <c r="AP15" t="n">
+      <c r="AP15" s="10" t="n">
         <v>7155550007.17363</v>
       </c>
-      <c r="AQ15" t="n">
+      <c r="AQ15" s="10" t="n">
         <v>9442790944.20413</v>
       </c>
-      <c r="AR15" t="n">
+      <c r="AR15" s="10" t="n">
         <v>9769016033.44635</v>
       </c>
-      <c r="AS15" t="n">
+      <c r="AS15" s="10" t="n">
         <v>8101897276.33437</v>
       </c>
-      <c r="AT15" t="n">
+      <c r="AT15" s="10" t="n">
         <v>5838752056.36718</v>
       </c>
-      <c r="AU15" t="n">
+      <c r="AU15" s="10" t="n">
         <v>6100214031.6176</v>
       </c>
-      <c r="AV15" t="n">
+      <c r="AV15" s="10" t="n">
         <v>1991234194.89286</v>
       </c>
+      <c r="AW15" s="10"/>
     </row>
     <row r="16">
+      <c r="A16" t="str">
+        <f>M16</f>
+      </c>
+      <c r="B16" t="str">
+        <f>N16</f>
+      </c>
       <c r="M16" t="s">
         <v>45</v>
       </c>
       <c r="N16" t="s">
         <v>46</v>
       </c>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16" t="n">
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10" t="n">
         <v>140046183.136688</v>
       </c>
-      <c r="W16" t="n">
+      <c r="W16" s="10" t="n">
         <v>1086654815.98736</v>
       </c>
-      <c r="X16" t="n">
+      <c r="X16" s="10" t="n">
         <v>1143087877.62556</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="Y16" s="10" t="n">
         <v>287650773.263358</v>
       </c>
-      <c r="Z16" t="n">
+      <c r="Z16" s="10" t="n">
         <v>423766740.36093</v>
       </c>
-      <c r="AA16" t="n">
+      <c r="AA16" s="10" t="n">
         <v>10179104.0628542</v>
       </c>
-      <c r="AB16" t="n">
+      <c r="AB16" s="10" t="n">
         <v>365611014.859387</v>
       </c>
-      <c r="AC16" t="n">
+      <c r="AC16" s="10" t="n">
         <v>291814463.8679</v>
       </c>
-      <c r="AD16" t="n">
+      <c r="AD16" s="10" t="n">
         <v>429961322.195012</v>
       </c>
-      <c r="AE16" t="n">
+      <c r="AE16" s="10" t="n">
         <v>886708500.956586</v>
       </c>
-      <c r="AF16" t="n">
+      <c r="AF16" s="10" t="n">
         <v>1450444112.84666</v>
       </c>
-      <c r="AG16" t="n">
+      <c r="AG16" s="10" t="n">
         <v>3632970693.09919</v>
       </c>
-      <c r="AH16" t="n">
+      <c r="AH16" s="10" t="n">
         <v>4858082045.62215</v>
       </c>
-      <c r="AI16" t="n">
+      <c r="AI16" s="10" t="n">
         <v>2452738600.44899</v>
       </c>
-      <c r="AJ16" t="n">
+      <c r="AJ16" s="10" t="n">
         <v>6255021405.23053</v>
       </c>
-      <c r="AK16" t="n">
+      <c r="AK16" s="10" t="n">
         <v>5908381976.01715</v>
       </c>
-      <c r="AL16" t="n">
+      <c r="AL16" s="10" t="n">
         <v>15064314896.3359</v>
       </c>
-      <c r="AM16" t="n">
+      <c r="AM16" s="10" t="n">
         <v>4605716285.65461</v>
       </c>
-      <c r="AN16" t="n">
+      <c r="AN16" s="10" t="n">
         <v>13661490140.9433</v>
       </c>
-      <c r="AO16" t="n">
+      <c r="AO16" s="10" t="n">
         <v>12066711743.5826</v>
       </c>
-      <c r="AP16" t="n">
+      <c r="AP16" s="10" t="n">
         <v>28213328607.2449</v>
       </c>
-      <c r="AQ16" t="n">
+      <c r="AQ16" s="10" t="n">
         <v>18263064442.4415</v>
       </c>
-      <c r="AR16" t="n">
+      <c r="AR16" s="10" t="n">
         <v>19313675440.9329</v>
       </c>
-      <c r="AS16" t="n">
+      <c r="AS16" s="10" t="n">
         <v>39743146019.5718</v>
       </c>
-      <c r="AT16" t="n">
+      <c r="AT16" s="10" t="n">
         <v>10529202485.3032</v>
       </c>
-      <c r="AU16" t="n">
+      <c r="AU16" s="10" t="n">
         <v>20737931632.3383</v>
       </c>
-      <c r="AV16" t="n">
+      <c r="AV16" s="10" t="n">
         <v>17389653531.7627</v>
       </c>
+      <c r="AW16" s="10"/>
     </row>
     <row r="17">
+      <c r="A17" t="str">
+        <f>M17</f>
+      </c>
+      <c r="B17" t="str">
+        <f>N17</f>
+      </c>
       <c r="M17" t="s">
         <v>47</v>
       </c>
       <c r="N17" t="s">
         <v>44</v>
       </c>
-      <c r="O17"/>
-      <c r="P17"/>
-      <c r="Q17"/>
-      <c r="R17"/>
-      <c r="S17"/>
-      <c r="T17"/>
-      <c r="U17"/>
-      <c r="V17"/>
-      <c r="W17"/>
-      <c r="X17"/>
-      <c r="Y17"/>
-      <c r="Z17"/>
-      <c r="AA17"/>
-      <c r="AB17"/>
-      <c r="AC17"/>
-      <c r="AD17"/>
-      <c r="AE17"/>
-      <c r="AF17"/>
-      <c r="AG17"/>
-      <c r="AH17"/>
-      <c r="AI17"/>
-      <c r="AJ17"/>
-      <c r="AK17"/>
-      <c r="AL17"/>
-      <c r="AM17"/>
-      <c r="AN17"/>
-      <c r="AO17"/>
-      <c r="AP17"/>
-      <c r="AQ17" t="n">
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10"/>
+      <c r="AJ17" s="10"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="10"/>
+      <c r="AM17" s="10"/>
+      <c r="AN17" s="10"/>
+      <c r="AO17" s="10"/>
+      <c r="AP17" s="10"/>
+      <c r="AQ17" s="10" t="n">
         <v>1159568.09922193</v>
       </c>
-      <c r="AR17" t="n">
+      <c r="AR17" s="10" t="n">
         <v>338002.289777888</v>
       </c>
-      <c r="AS17" t="n">
+      <c r="AS17" s="10" t="n">
         <v>-20390.9010440048</v>
       </c>
-      <c r="AT17"/>
-      <c r="AU17"/>
-      <c r="AV17"/>
+      <c r="AT17" s="10"/>
+      <c r="AU17" s="10"/>
+      <c r="AV17" s="10"/>
+      <c r="AW17" s="10"/>
     </row>
     <row r="18">
+      <c r="A18" t="str">
+        <f>M18</f>
+      </c>
+      <c r="B18" t="str">
+        <f>N18</f>
+      </c>
       <c r="M18" t="s">
         <v>46</v>
       </c>
       <c r="N18" t="s">
         <v>46</v>
       </c>
-      <c r="O18" t="n">
+      <c r="O18" s="10" t="n">
         <v>19556684836.5411</v>
       </c>
-      <c r="P18" t="n">
+      <c r="P18" s="10" t="n">
         <v>16744539534.0472</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="Q18" s="10" t="n">
         <v>17308930895.3041</v>
       </c>
-      <c r="R18" t="n">
+      <c r="R18" s="10" t="n">
         <v>16055404967.0077</v>
       </c>
-      <c r="S18" t="n">
+      <c r="S18" s="10" t="n">
         <v>14808829381.969</v>
       </c>
-      <c r="T18" t="n">
+      <c r="T18" s="10" t="n">
         <v>14140553285.0521</v>
       </c>
-      <c r="U18" t="n">
+      <c r="U18" s="10" t="n">
         <v>13334451930.6218</v>
       </c>
-      <c r="V18" t="n">
+      <c r="V18" s="10" t="n">
         <v>12967444913.8972</v>
       </c>
-      <c r="W18" t="n">
+      <c r="W18" s="10" t="n">
         <v>14398407287.592</v>
       </c>
-      <c r="X18" t="n">
+      <c r="X18" s="10" t="n">
         <v>12148909210.0086</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="Y18" s="10" t="n">
         <v>13868770529.769</v>
       </c>
-      <c r="Z18" t="n">
+      <c r="Z18" s="10" t="n">
         <v>11996384194.7489</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AA18" s="10" t="n">
         <v>14632705441.2302</v>
       </c>
-      <c r="AB18" t="n">
+      <c r="AB18" s="10" t="n">
         <v>21343060589.1675</v>
       </c>
-      <c r="AC18" t="n">
+      <c r="AC18" s="10" t="n">
         <v>20633670824.3721</v>
       </c>
-      <c r="AD18" t="n">
+      <c r="AD18" s="10" t="n">
         <v>23258701431.9458</v>
       </c>
-      <c r="AE18" t="n">
+      <c r="AE18" s="10" t="n">
         <v>24344038508.6482</v>
       </c>
-      <c r="AF18" t="n">
+      <c r="AF18" s="10" t="n">
         <v>25400418735.3403</v>
       </c>
-      <c r="AG18" t="n">
+      <c r="AG18" s="10" t="n">
         <v>27654002904.1741</v>
       </c>
-      <c r="AH18" t="n">
+      <c r="AH18" s="10" t="n">
         <v>27454984651.6936</v>
       </c>
-      <c r="AI18" t="n">
+      <c r="AI18" s="10" t="n">
         <v>24728145320.4226</v>
       </c>
-      <c r="AJ18" t="n">
+      <c r="AJ18" s="10" t="n">
         <v>25757176323.5337</v>
       </c>
-      <c r="AK18" t="n">
+      <c r="AK18" s="10" t="n">
         <v>26877717280.6309</v>
       </c>
-      <c r="AL18" t="n">
+      <c r="AL18" s="10" t="n">
         <v>25148058839.0656</v>
       </c>
-      <c r="AM18" t="n">
+      <c r="AM18" s="10" t="n">
         <v>21062591632.4484</v>
       </c>
-      <c r="AN18" t="n">
+      <c r="AN18" s="10" t="n">
         <v>17755158831.9242</v>
       </c>
-      <c r="AO18" t="n">
+      <c r="AO18" s="10" t="n">
         <v>22704748425.5903</v>
       </c>
-      <c r="AP18" t="n">
+      <c r="AP18" s="10" t="n">
         <v>21773747607.9702</v>
       </c>
-      <c r="AQ18" t="n">
+      <c r="AQ18" s="10" t="n">
         <v>22012170827.1937</v>
       </c>
-      <c r="AR18" t="n">
+      <c r="AR18" s="10" t="n">
         <v>26945118132.3854</v>
       </c>
-      <c r="AS18" t="n">
+      <c r="AS18" s="10" t="n">
         <v>22846909773.4482</v>
       </c>
-      <c r="AT18" t="n">
+      <c r="AT18" s="10" t="n">
         <v>21281444946.7128</v>
       </c>
-      <c r="AU18" t="n">
+      <c r="AU18" s="10" t="n">
         <v>16116608567.0774</v>
       </c>
-      <c r="AV18" t="n">
+      <c r="AV18" s="10" t="n">
         <v>7403671862.21329</v>
       </c>
+      <c r="AW18" s="10"/>
     </row>
     <row r="19">
+      <c r="A19" t="str">
+        <f>M19</f>
+      </c>
+      <c r="B19" t="str">
+        <f>N19</f>
+      </c>
       <c r="M19" t="s">
         <v>44</v>
       </c>
       <c r="N19" t="s">
         <v>44</v>
       </c>
-      <c r="O19" t="n">
+      <c r="O19" s="10" t="n">
         <v>2663292.29917399</v>
       </c>
-      <c r="P19" t="n">
+      <c r="P19" s="10" t="n">
         <v>11481852.9506024</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="Q19" s="10" t="n">
         <v>12978264.1562423</v>
       </c>
-      <c r="R19" t="n">
+      <c r="R19" s="10" t="n">
         <v>16991346.732117</v>
       </c>
-      <c r="S19" t="n">
+      <c r="S19" s="10" t="n">
         <v>95806621.9493784</v>
       </c>
-      <c r="T19" t="n">
+      <c r="T19" s="10" t="n">
         <v>57218154.7223771</v>
       </c>
-      <c r="U19" t="n">
+      <c r="U19" s="10" t="n">
         <v>82901796.0775723</v>
       </c>
-      <c r="V19" t="n">
+      <c r="V19" s="10" t="n">
         <v>128724685.569757</v>
       </c>
-      <c r="W19" t="n">
+      <c r="W19" s="10" t="n">
         <v>237607011.777055</v>
       </c>
-      <c r="X19" t="n">
+      <c r="X19" s="10" t="n">
         <v>260287700.849196</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="Y19" s="10" t="n">
         <v>257261443.880679</v>
       </c>
-      <c r="Z19" t="n">
+      <c r="Z19" s="10" t="n">
         <v>247642586.612739</v>
       </c>
-      <c r="AA19" t="n">
+      <c r="AA19" s="10" t="n">
         <v>378919554.361481</v>
       </c>
-      <c r="AB19" t="n">
+      <c r="AB19" s="10" t="n">
         <v>454956236.763864</v>
       </c>
-      <c r="AC19" t="n">
+      <c r="AC19" s="10" t="n">
         <v>664253983.260503</v>
       </c>
-      <c r="AD19" t="n">
+      <c r="AD19" s="10" t="n">
         <v>630598109.342156</v>
       </c>
-      <c r="AE19" t="n">
+      <c r="AE19" s="10" t="n">
         <v>614410739.555907</v>
       </c>
-      <c r="AF19" t="n">
+      <c r="AF19" s="10" t="n">
         <v>745830981.976693</v>
       </c>
-      <c r="AG19" t="n">
+      <c r="AG19" s="10" t="n">
         <v>1045073768.23407</v>
       </c>
-      <c r="AH19" t="n">
+      <c r="AH19" s="10" t="n">
         <v>1156951167.75121</v>
       </c>
-      <c r="AI19" t="n">
+      <c r="AI19" s="10" t="n">
         <v>915200213.834922</v>
       </c>
-      <c r="AJ19" t="n">
+      <c r="AJ19" s="10" t="n">
         <v>1267382445.56139</v>
       </c>
-      <c r="AK19" t="n">
+      <c r="AK19" s="10" t="n">
         <v>904131616.150888</v>
       </c>
-      <c r="AL19" t="n">
+      <c r="AL19" s="10" t="n">
         <v>651794195.454087</v>
       </c>
-      <c r="AM19" t="n">
+      <c r="AM19" s="10" t="n">
         <v>552165536.950658</v>
       </c>
-      <c r="AN19" t="n">
+      <c r="AN19" s="10" t="n">
         <v>571338799.781236</v>
       </c>
-      <c r="AO19" t="n">
+      <c r="AO19" s="10" t="n">
         <v>670230153.612807</v>
       </c>
-      <c r="AP19" t="n">
+      <c r="AP19" s="10" t="n">
         <v>583567479.917776</v>
       </c>
-      <c r="AQ19" t="n">
+      <c r="AQ19" s="10" t="n">
         <v>1181488154.36486</v>
       </c>
-      <c r="AR19" t="n">
+      <c r="AR19" s="10" t="n">
         <v>1082643307.63388</v>
       </c>
-      <c r="AS19" t="n">
+      <c r="AS19" s="10" t="n">
         <v>1102917102.67256</v>
       </c>
-      <c r="AT19" t="n">
+      <c r="AT19" s="10" t="n">
         <v>1739489047.1828</v>
       </c>
-      <c r="AU19" t="n">
+      <c r="AU19" s="10" t="n">
         <v>1134739642.0035</v>
       </c>
-      <c r="AV19" t="n">
+      <c r="AV19" s="10" t="n">
         <v>779386619.152138</v>
       </c>
+      <c r="AW19" s="10"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <f>M20</f>
+      </c>
+      <c r="B20" t="str">
+        <f>N20</f>
+      </c>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="10"/>
+      <c r="AJ20" s="10"/>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="10"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="10"/>
+      <c r="AO20" s="10"/>
+      <c r="AP20" s="10"/>
+      <c r="AQ20" s="10"/>
+      <c r="AR20" s="10"/>
+      <c r="AS20" s="10"/>
+      <c r="AT20" s="10"/>
+      <c r="AU20" s="10"/>
+      <c r="AV20" s="10"/>
+      <c r="AW20" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4626,89 +4897,89 @@
       <c r="O2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10" t="n">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2" t="n">
         <v>18435016803.53</v>
       </c>
-      <c r="AA2" s="10" t="n">
+      <c r="AA2" s="2" t="n">
         <v>20134411773.9394</v>
       </c>
-      <c r="AB2" s="10" t="n">
+      <c r="AB2" s="2" t="n">
         <v>23443985015.1086</v>
       </c>
-      <c r="AC2" s="10" t="n">
+      <c r="AC2" s="2" t="n">
         <v>26676816872.291</v>
       </c>
-      <c r="AD2" s="10" t="n">
+      <c r="AD2" s="2" t="n">
         <v>24470273562.3805</v>
       </c>
-      <c r="AE2" s="10" t="n">
+      <c r="AE2" s="2" t="n">
         <v>20123779793.9688</v>
       </c>
-      <c r="AF2" s="10" t="n">
+      <c r="AF2" s="2" t="n">
         <v>26830244851.705</v>
       </c>
-      <c r="AG2" s="10" t="n">
+      <c r="AG2" s="2" t="n">
         <v>29080544499.0824</v>
       </c>
-      <c r="AH2" s="10" t="n">
+      <c r="AH2" s="2" t="n">
         <v>29161554168.2414</v>
       </c>
-      <c r="AI2" s="10" t="n">
+      <c r="AI2" s="2" t="n">
         <v>30233862099.7959</v>
       </c>
-      <c r="AJ2" s="10" t="n">
+      <c r="AJ2" s="2" t="n">
         <v>31789053337.2932</v>
       </c>
-      <c r="AK2" s="10" t="n">
+      <c r="AK2" s="2" t="n">
         <v>34378699278.0285</v>
       </c>
-      <c r="AL2" s="10" t="n">
+      <c r="AL2" s="2" t="n">
         <v>34050154491.8631</v>
       </c>
-      <c r="AM2" s="10" t="n">
+      <c r="AM2" s="2" t="n">
         <v>31952800826.7103</v>
       </c>
-      <c r="AN2" s="10" t="n">
+      <c r="AN2" s="2" t="n">
         <v>27283316572.8348</v>
       </c>
-      <c r="AO2" s="10" t="n">
+      <c r="AO2" s="2" t="n">
         <v>29146173982.292</v>
       </c>
-      <c r="AP2" s="10" t="n">
+      <c r="AP2" s="2" t="n">
         <v>31958272804.3431</v>
       </c>
-      <c r="AQ2" s="10" t="n">
+      <c r="AQ2" s="2" t="n">
         <v>32431531049.45</v>
       </c>
-      <c r="AR2" s="10" t="n">
+      <c r="AR2" s="2" t="n">
         <v>34027991669.7538</v>
       </c>
-      <c r="AS2" s="10" t="n">
+      <c r="AS2" s="2" t="n">
         <v>40923873119.6225</v>
       </c>
-      <c r="AT2" s="10" t="n">
+      <c r="AT2" s="2" t="n">
         <v>42320519111.1772</v>
       </c>
-      <c r="AU2" s="10" t="n">
+      <c r="AU2" s="2" t="n">
         <v>33673550260.8871</v>
       </c>
-      <c r="AV2" s="10" t="n">
+      <c r="AV2" s="2" t="n">
         <v>31510444831.3847</v>
       </c>
-      <c r="AW2" s="10" t="n">
+      <c r="AW2" s="2" t="n">
         <v>18023200566.2224</v>
       </c>
-      <c r="AX2" s="10"/>
+      <c r="AX2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -4726,89 +4997,89 @@
       <c r="O3" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10" t="n">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2" t="n">
         <v>817220948</v>
       </c>
-      <c r="AA3" s="10" t="n">
+      <c r="AA3" s="2" t="n">
         <v>1692568679</v>
       </c>
-      <c r="AB3" s="10" t="n">
+      <c r="AB3" s="2" t="n">
         <v>1864446757</v>
       </c>
-      <c r="AC3" s="10" t="n">
+      <c r="AC3" s="2" t="n">
         <v>1769819283.5</v>
       </c>
-      <c r="AD3" s="10" t="n">
+      <c r="AD3" s="2" t="n">
         <v>2469419338</v>
       </c>
-      <c r="AE3" s="10" t="n">
+      <c r="AE3" s="2" t="n">
         <v>7650069458</v>
       </c>
-      <c r="AF3" s="10" t="n">
+      <c r="AF3" s="2" t="n">
         <v>3801083671</v>
       </c>
-      <c r="AG3" s="10" t="n">
+      <c r="AG3" s="2" t="n">
         <v>3742823814.9947</v>
       </c>
-      <c r="AH3" s="10" t="n">
+      <c r="AH3" s="2" t="n">
         <v>7641439156.5834</v>
       </c>
-      <c r="AI3" s="10" t="n">
+      <c r="AI3" s="2" t="n">
         <v>4033642041.002</v>
       </c>
-      <c r="AJ3" s="10" t="n">
+      <c r="AJ3" s="2" t="n">
         <v>2173595141.6711</v>
       </c>
-      <c r="AK3" s="10" t="n">
+      <c r="AK3" s="2" t="n">
         <v>1205987932.4714</v>
       </c>
-      <c r="AL3" s="10" t="n">
+      <c r="AL3" s="2" t="n">
         <v>537654417.984</v>
       </c>
-      <c r="AM3" s="10" t="n">
+      <c r="AM3" s="2" t="n">
         <v>442105135.5651</v>
       </c>
-      <c r="AN3" s="10" t="n">
+      <c r="AN3" s="2" t="n">
         <v>326964605.8477</v>
       </c>
-      <c r="AO3" s="10" t="n">
+      <c r="AO3" s="2" t="n">
         <v>145025613.9339</v>
       </c>
-      <c r="AP3" s="10" t="n">
+      <c r="AP3" s="2" t="n">
         <v>145026013.4623</v>
       </c>
-      <c r="AQ3" s="10" t="n">
+      <c r="AQ3" s="2" t="n">
         <v>206504418.651</v>
       </c>
-      <c r="AR3" s="10" t="n">
+      <c r="AR3" s="2" t="n">
         <v>154494781.4638</v>
       </c>
-      <c r="AS3" s="10" t="n">
+      <c r="AS3" s="2" t="n">
         <v>201570450.952</v>
       </c>
-      <c r="AT3" s="10" t="n">
+      <c r="AT3" s="2" t="n">
         <v>504777241.0911</v>
       </c>
-      <c r="AU3" s="10" t="n">
+      <c r="AU3" s="2" t="n">
         <v>448119560.1044</v>
       </c>
-      <c r="AV3" s="10" t="n">
+      <c r="AV3" s="2" t="n">
         <v>382801102.4745</v>
       </c>
-      <c r="AW3" s="10" t="n">
+      <c r="AW3" s="2" t="n">
         <v>173029219.3685</v>
       </c>
-      <c r="AX3" s="10"/>
+      <c r="AX3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -4826,89 +5097,89 @@
       <c r="O4" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10" t="n">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2" t="n">
         <v>1384690540</v>
       </c>
-      <c r="AA4" s="10" t="n">
+      <c r="AA4" s="2" t="n">
         <v>1203331975</v>
       </c>
-      <c r="AB4" s="10" t="n">
+      <c r="AB4" s="2" t="n">
         <v>1348497701.4375</v>
       </c>
-      <c r="AC4" s="10" t="n">
+      <c r="AC4" s="2" t="n">
         <v>1606996362.8125</v>
       </c>
-      <c r="AD4" s="10" t="n">
+      <c r="AD4" s="2" t="n">
         <v>1865394105.1017</v>
       </c>
-      <c r="AE4" s="10" t="n">
+      <c r="AE4" s="2" t="n">
         <v>1557963564.7113</v>
       </c>
-      <c r="AF4" s="10" t="n">
+      <c r="AF4" s="2" t="n">
         <v>2323071129.2168</v>
       </c>
-      <c r="AG4" s="10" t="n">
+      <c r="AG4" s="2" t="n">
         <v>2256608267.8543</v>
       </c>
-      <c r="AH4" s="10" t="n">
+      <c r="AH4" s="2" t="n">
         <v>2431291922.565</v>
       </c>
-      <c r="AI4" s="10" t="n">
+      <c r="AI4" s="2" t="n">
         <v>2219534615.0246</v>
       </c>
-      <c r="AJ4" s="10" t="n">
+      <c r="AJ4" s="2" t="n">
         <v>1693435993.3834</v>
       </c>
-      <c r="AK4" s="10" t="n">
+      <c r="AK4" s="2" t="n">
         <v>1288566219.4594</v>
       </c>
-      <c r="AL4" s="10" t="n">
+      <c r="AL4" s="2" t="n">
         <v>997461313.5025</v>
       </c>
-      <c r="AM4" s="10" t="n">
+      <c r="AM4" s="2" t="n">
         <v>327648872.4866</v>
       </c>
-      <c r="AN4" s="10" t="n">
+      <c r="AN4" s="2" t="n">
         <v>166591293.8013</v>
       </c>
-      <c r="AO4" s="10" t="n">
+      <c r="AO4" s="2" t="n">
         <v>148429033.0806</v>
       </c>
-      <c r="AP4" s="10" t="n">
+      <c r="AP4" s="2" t="n">
         <v>194209912.2386</v>
       </c>
-      <c r="AQ4" s="10" t="n">
+      <c r="AQ4" s="2" t="n">
         <v>295069664.3187</v>
       </c>
-      <c r="AR4" s="10" t="n">
+      <c r="AR4" s="2" t="n">
         <v>222823561.9301</v>
       </c>
-      <c r="AS4" s="10" t="n">
+      <c r="AS4" s="2" t="n">
         <v>247652350.2748</v>
       </c>
-      <c r="AT4" s="10" t="n">
+      <c r="AT4" s="2" t="n">
         <v>335863737.457</v>
       </c>
-      <c r="AU4" s="10" t="n">
+      <c r="AU4" s="2" t="n">
         <v>272697611.1137</v>
       </c>
-      <c r="AV4" s="10" t="n">
+      <c r="AV4" s="2" t="n">
         <v>460093866.8452</v>
       </c>
-      <c r="AW4" s="10" t="n">
+      <c r="AW4" s="2" t="n">
         <v>320525190.566</v>
       </c>
-      <c r="AX4" s="10"/>
+      <c r="AX4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -4926,89 +5197,89 @@
       <c r="O5" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10" t="n">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2" t="n">
         <v>1464130021</v>
       </c>
-      <c r="AA5" s="10" t="n">
+      <c r="AA5" s="2" t="n">
         <v>1576349336</v>
       </c>
-      <c r="AB5" s="10" t="n">
+      <c r="AB5" s="2" t="n">
         <v>1241522003</v>
       </c>
-      <c r="AC5" s="10" t="n">
+      <c r="AC5" s="2" t="n">
         <v>2225944581</v>
       </c>
-      <c r="AD5" s="10" t="n">
+      <c r="AD5" s="2" t="n">
         <v>2051699907</v>
       </c>
-      <c r="AE5" s="10" t="n">
+      <c r="AE5" s="2" t="n">
         <v>2028172125.25</v>
       </c>
-      <c r="AF5" s="10" t="n">
+      <c r="AF5" s="2" t="n">
         <v>2396926245.3267</v>
       </c>
-      <c r="AG5" s="10" t="n">
+      <c r="AG5" s="2" t="n">
         <v>3715646511.6924</v>
       </c>
-      <c r="AH5" s="10" t="n">
+      <c r="AH5" s="2" t="n">
         <v>7269212912.972</v>
       </c>
-      <c r="AI5" s="10" t="n">
+      <c r="AI5" s="2" t="n">
         <v>7310992688.6111</v>
       </c>
-      <c r="AJ5" s="10" t="n">
+      <c r="AJ5" s="2" t="n">
         <v>8537934854.7812</v>
       </c>
-      <c r="AK5" s="10" t="n">
+      <c r="AK5" s="2" t="n">
         <v>17101059147.4311</v>
       </c>
-      <c r="AL5" s="10" t="n">
+      <c r="AL5" s="2" t="n">
         <v>15524971275.5827</v>
       </c>
-      <c r="AM5" s="10" t="n">
+      <c r="AM5" s="2" t="n">
         <v>19130825933.2869</v>
       </c>
-      <c r="AN5" s="10" t="n">
+      <c r="AN5" s="2" t="n">
         <v>15849272506.0343</v>
       </c>
-      <c r="AO5" s="10" t="n">
+      <c r="AO5" s="2" t="n">
         <v>18512220879.8149</v>
       </c>
-      <c r="AP5" s="10" t="n">
+      <c r="AP5" s="2" t="n">
         <v>16561678209.8346</v>
       </c>
-      <c r="AQ5" s="10" t="n">
+      <c r="AQ5" s="2" t="n">
         <v>13923592758.2565</v>
       </c>
-      <c r="AR5" s="10" t="n">
+      <c r="AR5" s="2" t="n">
         <v>16831828314.585</v>
       </c>
-      <c r="AS5" s="10" t="n">
+      <c r="AS5" s="2" t="n">
         <v>20862956016.424</v>
       </c>
-      <c r="AT5" s="10" t="n">
+      <c r="AT5" s="2" t="n">
         <v>16353377329.7241</v>
       </c>
-      <c r="AU5" s="10" t="n">
+      <c r="AU5" s="2" t="n">
         <v>17726249512.3628</v>
       </c>
-      <c r="AV5" s="10" t="n">
+      <c r="AV5" s="2" t="n">
         <v>14287090543.2938</v>
       </c>
-      <c r="AW5" s="10" t="n">
+      <c r="AW5" s="2" t="n">
         <v>19427349347.59</v>
       </c>
-      <c r="AX5" s="10"/>
+      <c r="AX5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -5026,89 +5297,89 @@
       <c r="O6" t="s">
         <v>57</v>
       </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10" t="n">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2" t="n">
         <v>4754887357</v>
       </c>
-      <c r="AA6" s="10" t="n">
+      <c r="AA6" s="2" t="n">
         <v>5079917345</v>
       </c>
-      <c r="AB6" s="10" t="n">
+      <c r="AB6" s="2" t="n">
         <v>5896551985.5</v>
       </c>
-      <c r="AC6" s="10" t="n">
+      <c r="AC6" s="2" t="n">
         <v>10867533308.0431</v>
       </c>
-      <c r="AD6" s="10" t="n">
+      <c r="AD6" s="2" t="n">
         <v>11748237631.1209</v>
       </c>
-      <c r="AE6" s="10" t="n">
+      <c r="AE6" s="2" t="n">
         <v>11909342815.0938</v>
       </c>
-      <c r="AF6" s="10" t="n">
+      <c r="AF6" s="2" t="n">
         <v>13955054549.5041</v>
       </c>
-      <c r="AG6" s="10" t="n">
+      <c r="AG6" s="2" t="n">
         <v>13306872348.3573</v>
       </c>
-      <c r="AH6" s="10" t="n">
+      <c r="AH6" s="2" t="n">
         <v>12825711255.1507</v>
       </c>
-      <c r="AI6" s="10" t="n">
+      <c r="AI6" s="2" t="n">
         <v>11940478265.8961</v>
       </c>
-      <c r="AJ6" s="10" t="n">
+      <c r="AJ6" s="2" t="n">
         <v>12534021537.2026</v>
       </c>
-      <c r="AK6" s="10" t="n">
+      <c r="AK6" s="2" t="n">
         <v>11591985438.8239</v>
       </c>
-      <c r="AL6" s="10" t="n">
+      <c r="AL6" s="2" t="n">
         <v>12288986042.0497</v>
       </c>
-      <c r="AM6" s="10" t="n">
+      <c r="AM6" s="2" t="n">
         <v>11646909626.7398</v>
       </c>
-      <c r="AN6" s="10" t="n">
+      <c r="AN6" s="2" t="n">
         <v>11565596250.5205</v>
       </c>
-      <c r="AO6" s="10" t="n">
+      <c r="AO6" s="2" t="n">
         <v>11141586749.5001</v>
       </c>
-      <c r="AP6" s="10" t="n">
+      <c r="AP6" s="2" t="n">
         <v>11450457090.4495</v>
       </c>
-      <c r="AQ6" s="10" t="n">
+      <c r="AQ6" s="2" t="n">
         <v>12605014750.6374</v>
       </c>
-      <c r="AR6" s="10" t="n">
+      <c r="AR6" s="2" t="n">
         <v>11306299211.1611</v>
       </c>
-      <c r="AS6" s="10" t="n">
+      <c r="AS6" s="2" t="n">
         <v>12261823447.3584</v>
       </c>
-      <c r="AT6" s="10" t="n">
+      <c r="AT6" s="2" t="n">
         <v>8775269572.6885</v>
       </c>
-      <c r="AU6" s="10" t="n">
+      <c r="AU6" s="2" t="n">
         <v>9273692343.2085</v>
       </c>
-      <c r="AV6" s="10" t="n">
+      <c r="AV6" s="2" t="n">
         <v>9580549306.11</v>
       </c>
-      <c r="AW6" s="10" t="n">
+      <c r="AW6" s="2" t="n">
         <v>4190750910.5895</v>
       </c>
-      <c r="AX6" s="10"/>
+      <c r="AX6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -5126,89 +5397,89 @@
       <c r="O7" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10" t="n">
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2" t="n">
         <v>7398907757</v>
       </c>
-      <c r="AA7" s="10" t="n">
+      <c r="AA7" s="2" t="n">
         <v>6353075318</v>
       </c>
-      <c r="AB7" s="10" t="n">
+      <c r="AB7" s="2" t="n">
         <v>5093396308</v>
       </c>
-      <c r="AC7" s="10" t="n">
+      <c r="AC7" s="2" t="n">
         <v>5928596277.8101</v>
       </c>
-      <c r="AD7" s="10" t="n">
+      <c r="AD7" s="2" t="n">
         <v>5003115808.375</v>
       </c>
-      <c r="AE7" s="10" t="n">
+      <c r="AE7" s="2" t="n">
         <v>3813708765.0596</v>
       </c>
-      <c r="AF7" s="10" t="n">
+      <c r="AF7" s="2" t="n">
         <v>4546730798.9782</v>
       </c>
-      <c r="AG7" s="10" t="n">
+      <c r="AG7" s="2" t="n">
         <v>7470415372.3167</v>
       </c>
-      <c r="AH7" s="10" t="n">
+      <c r="AH7" s="2" t="n">
         <v>4537302372.7743</v>
       </c>
-      <c r="AI7" s="10" t="n">
+      <c r="AI7" s="2" t="n">
         <v>5828136823.7699</v>
       </c>
-      <c r="AJ7" s="10" t="n">
+      <c r="AJ7" s="2" t="n">
         <v>6003155036.8935</v>
       </c>
-      <c r="AK7" s="10" t="n">
+      <c r="AK7" s="2" t="n">
         <v>3322679344.7227</v>
       </c>
-      <c r="AL7" s="10" t="n">
+      <c r="AL7" s="2" t="n">
         <v>11632708635.5434</v>
       </c>
-      <c r="AM7" s="10" t="n">
+      <c r="AM7" s="2" t="n">
         <v>9615807939.0697</v>
       </c>
-      <c r="AN7" s="10" t="n">
+      <c r="AN7" s="2" t="n">
         <v>2892889203.162</v>
       </c>
-      <c r="AO7" s="10" t="n">
+      <c r="AO7" s="2" t="n">
         <v>2357317641.1424</v>
       </c>
-      <c r="AP7" s="10" t="n">
+      <c r="AP7" s="2" t="n">
         <v>14587293141.1913</v>
       </c>
-      <c r="AQ7" s="10" t="n">
+      <c r="AQ7" s="2" t="n">
         <v>26373033545.9417</v>
       </c>
-      <c r="AR7" s="10" t="n">
+      <c r="AR7" s="2" t="n">
         <v>20795343635.5401</v>
       </c>
-      <c r="AS7" s="10" t="n">
+      <c r="AS7" s="2" t="n">
         <v>15589907994.7755</v>
       </c>
-      <c r="AT7" s="10" t="n">
+      <c r="AT7" s="2" t="n">
         <v>37020630921.7999</v>
       </c>
-      <c r="AU7" s="10" t="n">
+      <c r="AU7" s="2" t="n">
         <v>11100489237.975</v>
       </c>
-      <c r="AV7" s="10" t="n">
+      <c r="AV7" s="2" t="n">
         <v>18909526156.1226</v>
       </c>
-      <c r="AW7" s="10" t="n">
+      <c r="AW7" s="2" t="n">
         <v>8114033874.1767</v>
       </c>
-      <c r="AX7" s="10"/>
+      <c r="AX7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -5226,81 +5497,81 @@
       <c r="O8" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10" t="n">
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="10" t="n">
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2" t="n">
         <v>4989000</v>
       </c>
-      <c r="AC8" s="10" t="n">
+      <c r="AC8" s="2" t="n">
         <v>649938</v>
       </c>
-      <c r="AD8" s="10" t="n">
+      <c r="AD8" s="2" t="n">
         <v>3004126</v>
       </c>
-      <c r="AE8" s="10" t="n">
+      <c r="AE8" s="2" t="n">
         <v>23379295</v>
       </c>
-      <c r="AF8" s="10" t="n">
+      <c r="AF8" s="2" t="n">
         <v>53203268</v>
       </c>
-      <c r="AG8" s="10" t="n">
+      <c r="AG8" s="2" t="n">
         <v>897160922.3025</v>
       </c>
-      <c r="AH8" s="10" t="n">
+      <c r="AH8" s="2" t="n">
         <v>1766320288.9257</v>
       </c>
-      <c r="AI8" s="10" t="n">
+      <c r="AI8" s="2" t="n">
         <v>2561032400.5561</v>
       </c>
-      <c r="AJ8" s="10" t="n">
+      <c r="AJ8" s="2" t="n">
         <v>10524681.1805</v>
       </c>
-      <c r="AK8" s="10" t="n">
+      <c r="AK8" s="2" t="n">
         <v>227016.0541</v>
       </c>
-      <c r="AL8" s="10" t="n">
+      <c r="AL8" s="2" t="n">
         <v>-6018055.4866</v>
       </c>
-      <c r="AM8" s="10" t="n">
+      <c r="AM8" s="2" t="n">
         <v>-3983829.0098</v>
       </c>
-      <c r="AN8" s="10" t="n">
+      <c r="AN8" s="2" t="n">
         <v>-1767022.54</v>
       </c>
-      <c r="AO8" s="10" t="n">
+      <c r="AO8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AP8" s="10" t="n">
+      <c r="AP8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ8" s="10" t="n">
+      <c r="AQ8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AR8" s="10" t="n">
+      <c r="AR8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS8" s="10" t="n">
+      <c r="AS8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AT8" s="10" t="n">
+      <c r="AT8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU8" s="10"/>
-      <c r="AV8" s="10"/>
-      <c r="AW8" s="10"/>
-      <c r="AX8" s="10"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -5316,109 +5587,109 @@
         <v>60</v>
       </c>
       <c r="O9"/>
-      <c r="P9" s="10" t="n">
+      <c r="P9" s="2" t="n">
         <v>30980247148</v>
       </c>
-      <c r="Q9" s="10" t="n">
+      <c r="Q9" s="2" t="n">
         <v>30513099255</v>
       </c>
-      <c r="R9" s="10" t="n">
+      <c r="R9" s="2" t="n">
         <v>30337971567</v>
       </c>
-      <c r="S9" s="10" t="n">
+      <c r="S9" s="2" t="n">
         <v>29918044865</v>
       </c>
-      <c r="T9" s="10" t="n">
+      <c r="T9" s="2" t="n">
         <v>30546960405</v>
       </c>
-      <c r="U9" s="10" t="n">
+      <c r="U9" s="2" t="n">
         <v>26815505318</v>
       </c>
-      <c r="V9" s="10" t="n">
+      <c r="V9" s="2" t="n">
         <v>28856006190</v>
       </c>
-      <c r="W9" s="10" t="n">
+      <c r="W9" s="2" t="n">
         <v>24930833919</v>
       </c>
-      <c r="X9" s="10" t="n">
+      <c r="X9" s="2" t="n">
         <v>26529770069</v>
       </c>
-      <c r="Y9" s="10" t="n">
+      <c r="Y9" s="2" t="n">
         <v>27545374131</v>
       </c>
-      <c r="Z9" s="10" t="n">
+      <c r="Z9" s="2" t="n">
         <v>1165484638</v>
       </c>
-      <c r="AA9" s="10" t="n">
+      <c r="AA9" s="2" t="n">
         <v>82191621</v>
       </c>
-      <c r="AB9" s="10" t="n">
+      <c r="AB9" s="2" t="n">
         <v>132500791.1201</v>
       </c>
-      <c r="AC9" s="10" t="n">
+      <c r="AC9" s="2" t="n">
         <v>168663563</v>
       </c>
-      <c r="AD9" s="10" t="n">
+      <c r="AD9" s="2" t="n">
         <v>190982087</v>
       </c>
-      <c r="AE9" s="10" t="n">
+      <c r="AE9" s="2" t="n">
         <v>176182910</v>
       </c>
-      <c r="AF9" s="10" t="n">
+      <c r="AF9" s="2" t="n">
         <v>66663467.55</v>
       </c>
-      <c r="AG9" s="10" t="n">
+      <c r="AG9" s="2" t="n">
         <v>11859106.1357</v>
       </c>
-      <c r="AH9" s="10" t="n">
+      <c r="AH9" s="2" t="n">
         <v>1093903392.6831</v>
       </c>
-      <c r="AI9" s="10" t="n">
+      <c r="AI9" s="2" t="n">
         <v>1721970881.9347</v>
       </c>
-      <c r="AJ9" s="10" t="n">
+      <c r="AJ9" s="2" t="n">
         <v>860870356.5886</v>
       </c>
-      <c r="AK9" s="10" t="n">
+      <c r="AK9" s="2" t="n">
         <v>1413589516.2339</v>
       </c>
-      <c r="AL9" s="10" t="n">
+      <c r="AL9" s="2" t="n">
         <v>3138190520.6504</v>
       </c>
-      <c r="AM9" s="10" t="n">
+      <c r="AM9" s="2" t="n">
         <v>146593784.5212</v>
       </c>
-      <c r="AN9" s="10" t="n">
+      <c r="AN9" s="2" t="n">
         <v>139579867.4808</v>
       </c>
-      <c r="AO9" s="10" t="n">
+      <c r="AO9" s="2" t="n">
         <v>242406172.4482</v>
       </c>
-      <c r="AP9" s="10" t="n">
+      <c r="AP9" s="2" t="n">
         <v>449203451.2652</v>
       </c>
-      <c r="AQ9" s="10" t="n">
+      <c r="AQ9" s="2" t="n">
         <v>-12199817.5281</v>
       </c>
-      <c r="AR9" s="10" t="n">
+      <c r="AR9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS9" s="10" t="n">
+      <c r="AS9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AT9" s="10" t="n">
+      <c r="AT9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU9" s="10" t="n">
+      <c r="AU9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AV9" s="10" t="n">
+      <c r="AV9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW9" s="10" t="n">
+      <c r="AW9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AX9" s="10"/>
+      <c r="AX9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -5433,107 +5704,107 @@
       <c r="O10" t="s">
         <v>434</v>
       </c>
-      <c r="P10" s="10" t="str">
+      <c r="P10" s="2" t="str">
         <f>Sum(P2:P9)</f>
       </c>
-      <c r="Q10" s="10" t="str">
+      <c r="Q10" s="2" t="str">
         <f>Sum(Q2:Q9)</f>
       </c>
-      <c r="R10" s="10" t="str">
+      <c r="R10" s="2" t="str">
         <f>Sum(R2:R9)</f>
       </c>
-      <c r="S10" s="10" t="str">
+      <c r="S10" s="2" t="str">
         <f>Sum(S2:S9)</f>
       </c>
-      <c r="T10" s="10" t="str">
+      <c r="T10" s="2" t="str">
         <f>Sum(T2:T9)</f>
       </c>
-      <c r="U10" s="10" t="str">
+      <c r="U10" s="2" t="str">
         <f>Sum(U2:U9)</f>
       </c>
-      <c r="V10" s="10" t="str">
+      <c r="V10" s="2" t="str">
         <f>Sum(V2:V9)</f>
       </c>
-      <c r="W10" s="10" t="str">
+      <c r="W10" s="2" t="str">
         <f>Sum(W2:W9)</f>
       </c>
-      <c r="X10" s="10" t="str">
+      <c r="X10" s="2" t="str">
         <f>Sum(X2:X9)</f>
       </c>
-      <c r="Y10" s="10" t="str">
+      <c r="Y10" s="2" t="str">
         <f>Sum(Y2:Y9)</f>
       </c>
-      <c r="Z10" s="10" t="str">
+      <c r="Z10" s="2" t="str">
         <f>Sum(Z2:Z9)</f>
       </c>
-      <c r="AA10" s="10" t="str">
+      <c r="AA10" s="2" t="str">
         <f>Sum(AA2:AA9)</f>
       </c>
-      <c r="AB10" s="10" t="str">
+      <c r="AB10" s="2" t="str">
         <f>Sum(AB2:AB9)</f>
       </c>
-      <c r="AC10" s="10" t="str">
+      <c r="AC10" s="2" t="str">
         <f>Sum(AC2:AC9)</f>
       </c>
-      <c r="AD10" s="10" t="str">
+      <c r="AD10" s="2" t="str">
         <f>Sum(AD2:AD9)</f>
       </c>
-      <c r="AE10" s="10" t="str">
+      <c r="AE10" s="2" t="str">
         <f>Sum(AE2:AE9)</f>
       </c>
-      <c r="AF10" s="10" t="str">
+      <c r="AF10" s="2" t="str">
         <f>Sum(AF2:AF9)</f>
       </c>
-      <c r="AG10" s="10" t="str">
+      <c r="AG10" s="2" t="str">
         <f>Sum(AG2:AG9)</f>
       </c>
-      <c r="AH10" s="10" t="str">
+      <c r="AH10" s="2" t="str">
         <f>Sum(AH2:AH9)</f>
       </c>
-      <c r="AI10" s="10" t="str">
+      <c r="AI10" s="2" t="str">
         <f>Sum(AI2:AI9)</f>
       </c>
-      <c r="AJ10" s="10" t="str">
+      <c r="AJ10" s="2" t="str">
         <f>Sum(AJ2:AJ9)</f>
       </c>
-      <c r="AK10" s="10" t="str">
+      <c r="AK10" s="2" t="str">
         <f>Sum(AK2:AK9)</f>
       </c>
-      <c r="AL10" s="10" t="str">
+      <c r="AL10" s="2" t="str">
         <f>Sum(AL2:AL9)</f>
       </c>
-      <c r="AM10" s="10" t="str">
+      <c r="AM10" s="2" t="str">
         <f>Sum(AM2:AM9)</f>
       </c>
-      <c r="AN10" s="10" t="str">
+      <c r="AN10" s="2" t="str">
         <f>Sum(AN2:AN9)</f>
       </c>
-      <c r="AO10" s="10" t="str">
+      <c r="AO10" s="2" t="str">
         <f>Sum(AO2:AO9)</f>
       </c>
-      <c r="AP10" s="10" t="str">
+      <c r="AP10" s="2" t="str">
         <f>Sum(AP2:AP9)</f>
       </c>
-      <c r="AQ10" s="10" t="str">
+      <c r="AQ10" s="2" t="str">
         <f>Sum(AQ2:AQ9)</f>
       </c>
-      <c r="AR10" s="10" t="str">
+      <c r="AR10" s="2" t="str">
         <f>Sum(AR2:AR9)</f>
       </c>
-      <c r="AS10" s="10" t="str">
+      <c r="AS10" s="2" t="str">
         <f>Sum(AS2:AS9)</f>
       </c>
-      <c r="AT10" s="10" t="str">
+      <c r="AT10" s="2" t="str">
         <f>Sum(AT2:AT9)</f>
       </c>
-      <c r="AU10" s="10" t="str">
+      <c r="AU10" s="2" t="str">
         <f>Sum(AU2:AU9)</f>
       </c>
-      <c r="AV10" s="10" t="str">
+      <c r="AV10" s="2" t="str">
         <f>Sum(AV2:AV9)</f>
       </c>
-      <c r="AW10" s="10"/>
-      <c r="AX10" s="10"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -5670,89 +5941,89 @@
       <c r="O14" t="s">
         <v>51</v>
       </c>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10" t="n">
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2" t="n">
         <v>29786010617.463</v>
       </c>
-      <c r="AA14" s="10" t="n">
+      <c r="AA14" s="2" t="n">
         <v>31761574296.7241</v>
       </c>
-      <c r="AB14" s="10" t="n">
+      <c r="AB14" s="2" t="n">
         <v>36407707891.7418</v>
       </c>
-      <c r="AC14" s="10" t="n">
+      <c r="AC14" s="2" t="n">
         <v>40651156223.7523</v>
       </c>
-      <c r="AD14" s="10" t="n">
+      <c r="AD14" s="2" t="n">
         <v>36399026091.3253</v>
       </c>
-      <c r="AE14" s="10" t="n">
+      <c r="AE14" s="2" t="n">
         <v>29051789404.6939</v>
       </c>
-      <c r="AF14" s="10" t="n">
+      <c r="AF14" s="2" t="n">
         <v>37512298572.6687</v>
       </c>
-      <c r="AG14" s="10" t="n">
+      <c r="AG14" s="2" t="n">
         <v>39573297692.6881</v>
       </c>
-      <c r="AH14" s="10" t="n">
+      <c r="AH14" s="2" t="n">
         <v>38872811632.1524</v>
       </c>
-      <c r="AI14" s="10" t="n">
+      <c r="AI14" s="2" t="n">
         <v>39896785670.8544</v>
       </c>
-      <c r="AJ14" s="10" t="n">
+      <c r="AJ14" s="2" t="n">
         <v>41587320644.0153</v>
       </c>
-      <c r="AK14" s="10" t="n">
+      <c r="AK14" s="2" t="n">
         <v>44086655785.1458</v>
       </c>
-      <c r="AL14" s="10" t="n">
+      <c r="AL14" s="2" t="n">
         <v>42879359543.4218</v>
       </c>
-      <c r="AM14" s="10" t="n">
+      <c r="AM14" s="2" t="n">
         <v>39515036888.135</v>
       </c>
-      <c r="AN14" s="10" t="n">
+      <c r="AN14" s="2" t="n">
         <v>33100077617.8106</v>
       </c>
-      <c r="AO14" s="10" t="n">
+      <c r="AO14" s="2" t="n">
         <v>34959307472.6217</v>
       </c>
-      <c r="AP14" s="10" t="n">
+      <c r="AP14" s="2" t="n">
         <v>38017242551.0955</v>
       </c>
-      <c r="AQ14" s="10" t="n">
+      <c r="AQ14" s="2" t="n">
         <v>37903505402.2661</v>
       </c>
-      <c r="AR14" s="10" t="n">
+      <c r="AR14" s="2" t="n">
         <v>38856954937.7067</v>
       </c>
-      <c r="AS14" s="10" t="n">
+      <c r="AS14" s="2" t="n">
         <v>45833718808.7397</v>
       </c>
-      <c r="AT14" s="10" t="n">
+      <c r="AT14" s="2" t="n">
         <v>46773942202.7291</v>
       </c>
-      <c r="AU14" s="10" t="n">
+      <c r="AU14" s="2" t="n">
         <v>36006709571.0263</v>
       </c>
-      <c r="AV14" s="10" t="n">
+      <c r="AV14" s="2" t="n">
         <v>31510444831.3847</v>
       </c>
-      <c r="AW14" s="10" t="n">
+      <c r="AW14" s="2" t="n">
         <v>17190499492.3007</v>
       </c>
-      <c r="AX14" s="10"/>
+      <c r="AX14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -5770,89 +6041,89 @@
       <c r="O15" t="s">
         <v>53</v>
       </c>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10" t="n">
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2" t="n">
         <v>1320408442.98445</v>
       </c>
-      <c r="AA15" s="10" t="n">
+      <c r="AA15" s="2" t="n">
         <v>2669988398.66522</v>
       </c>
-      <c r="AB15" s="10" t="n">
+      <c r="AB15" s="2" t="n">
         <v>2895422124.89965</v>
       </c>
-      <c r="AC15" s="10" t="n">
+      <c r="AC15" s="2" t="n">
         <v>2696918471.41241</v>
       </c>
-      <c r="AD15" s="10" t="n">
+      <c r="AD15" s="2" t="n">
         <v>3673210219.13174</v>
       </c>
-      <c r="AE15" s="10" t="n">
+      <c r="AE15" s="2" t="n">
         <v>11044058775.2657</v>
       </c>
-      <c r="AF15" s="10" t="n">
+      <c r="AF15" s="2" t="n">
         <v>5314427294.80668</v>
       </c>
-      <c r="AG15" s="10" t="n">
+      <c r="AG15" s="2" t="n">
         <v>5093298065.54142</v>
       </c>
-      <c r="AH15" s="10" t="n">
+      <c r="AH15" s="2" t="n">
         <v>10186158913.8455</v>
       </c>
-      <c r="AI15" s="10" t="n">
+      <c r="AI15" s="2" t="n">
         <v>5322818217.91768</v>
       </c>
-      <c r="AJ15" s="10" t="n">
+      <c r="AJ15" s="2" t="n">
         <v>2843557407.88621</v>
       </c>
-      <c r="AK15" s="10" t="n">
+      <c r="AK15" s="2" t="n">
         <v>1546538291.92095</v>
       </c>
-      <c r="AL15" s="10" t="n">
+      <c r="AL15" s="2" t="n">
         <v>677068208.438066</v>
       </c>
-      <c r="AM15" s="10" t="n">
+      <c r="AM15" s="2" t="n">
         <v>546737697.112464</v>
       </c>
-      <c r="AN15" s="10" t="n">
+      <c r="AN15" s="2" t="n">
         <v>396672955.904907</v>
       </c>
-      <c r="AO15" s="10" t="n">
+      <c r="AO15" s="2" t="n">
         <v>173950619.796659</v>
       </c>
-      <c r="AP15" s="10" t="n">
+      <c r="AP15" s="2" t="n">
         <v>172521499.011218</v>
       </c>
-      <c r="AQ15" s="10" t="n">
+      <c r="AQ15" s="2" t="n">
         <v>241346649.222185</v>
       </c>
-      <c r="AR15" s="10" t="n">
+      <c r="AR15" s="2" t="n">
         <v>176419367.317106</v>
       </c>
-      <c r="AS15" s="10" t="n">
+      <c r="AS15" s="2" t="n">
         <v>225753885.564047</v>
       </c>
-      <c r="AT15" s="10" t="n">
+      <c r="AT15" s="2" t="n">
         <v>557895366.028543</v>
       </c>
-      <c r="AU15" s="10" t="n">
+      <c r="AU15" s="2" t="n">
         <v>479168686.662567</v>
       </c>
-      <c r="AV15" s="10" t="n">
+      <c r="AV15" s="2" t="n">
         <v>382801102.4745</v>
       </c>
-      <c r="AW15" s="10" t="n">
+      <c r="AW15" s="2" t="n">
         <v>165034989.028634</v>
       </c>
-      <c r="AX15" s="10"/>
+      <c r="AX15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -5870,89 +6141,89 @@
       <c r="O16" t="s">
         <v>54</v>
       </c>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10" t="n">
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2" t="n">
         <v>2237286115.1091</v>
       </c>
-      <c r="AA16" s="10" t="n">
+      <c r="AA16" s="2" t="n">
         <v>1898228682.15376</v>
       </c>
-      <c r="AB16" s="10" t="n">
+      <c r="AB16" s="2" t="n">
         <v>2094170866.21501</v>
       </c>
-      <c r="AC16" s="10" t="n">
+      <c r="AC16" s="2" t="n">
         <v>2448802662.94239</v>
       </c>
-      <c r="AD16" s="10" t="n">
+      <c r="AD16" s="2" t="n">
         <v>2774735171.19095</v>
       </c>
-      <c r="AE16" s="10" t="n">
+      <c r="AE16" s="2" t="n">
         <v>2249161432.17508</v>
       </c>
-      <c r="AF16" s="10" t="n">
+      <c r="AF16" s="2" t="n">
         <v>3247966549.92842</v>
       </c>
-      <c r="AG16" s="10" t="n">
+      <c r="AG16" s="2" t="n">
         <v>3070830766.67967</v>
       </c>
-      <c r="AH16" s="10" t="n">
+      <c r="AH16" s="2" t="n">
         <v>3240950478.26946</v>
       </c>
-      <c r="AI16" s="10" t="n">
+      <c r="AI16" s="2" t="n">
         <v>2928911183.50628</v>
       </c>
-      <c r="AJ16" s="10" t="n">
+      <c r="AJ16" s="2" t="n">
         <v>2215399901.96351</v>
       </c>
-      <c r="AK16" s="10" t="n">
+      <c r="AK16" s="2" t="n">
         <v>1652435274.36129</v>
       </c>
-      <c r="AL16" s="10" t="n">
+      <c r="AL16" s="2" t="n">
         <v>1256103031.85403</v>
       </c>
-      <c r="AM16" s="10" t="n">
+      <c r="AM16" s="2" t="n">
         <v>405193189.569817</v>
       </c>
-      <c r="AN16" s="10" t="n">
+      <c r="AN16" s="2" t="n">
         <v>202108300.893478</v>
       </c>
-      <c r="AO16" s="10" t="n">
+      <c r="AO16" s="2" t="n">
         <v>178032842.611906</v>
       </c>
-      <c r="AP16" s="10" t="n">
+      <c r="AP16" s="2" t="n">
         <v>231030174.39661</v>
       </c>
-      <c r="AQ16" s="10" t="n">
+      <c r="AQ16" s="2" t="n">
         <v>344854968.410083</v>
       </c>
-      <c r="AR16" s="10" t="n">
+      <c r="AR16" s="2" t="n">
         <v>254444787.368194</v>
       </c>
-      <c r="AS16" s="10" t="n">
+      <c r="AS16" s="2" t="n">
         <v>277364465.275309</v>
       </c>
-      <c r="AT16" s="10" t="n">
+      <c r="AT16" s="2" t="n">
         <v>371206955.248742</v>
       </c>
-      <c r="AU16" s="10" t="n">
+      <c r="AU16" s="2" t="n">
         <v>291592172.729369</v>
       </c>
-      <c r="AV16" s="10" t="n">
+      <c r="AV16" s="2" t="n">
         <v>460093866.8452</v>
       </c>
-      <c r="AW16" s="10" t="n">
+      <c r="AW16" s="2" t="n">
         <v>305716407.330048</v>
       </c>
-      <c r="AX16" s="10"/>
+      <c r="AX16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -5970,89 +6241,89 @@
       <c r="O17" t="s">
         <v>55</v>
       </c>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10" t="n">
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2" t="n">
         <v>2365638871.69887</v>
       </c>
-      <c r="AA17" s="10" t="n">
+      <c r="AA17" s="2" t="n">
         <v>2486655041.88006</v>
       </c>
-      <c r="AB17" s="10" t="n">
+      <c r="AB17" s="2" t="n">
         <v>1928041260.78669</v>
       </c>
-      <c r="AC17" s="10" t="n">
+      <c r="AC17" s="2" t="n">
         <v>3391979685.61362</v>
       </c>
-      <c r="AD17" s="10" t="n">
+      <c r="AD17" s="2" t="n">
         <v>3051861200.32888</v>
       </c>
-      <c r="AE17" s="10" t="n">
+      <c r="AE17" s="2" t="n">
         <v>2927980233.45955</v>
       </c>
-      <c r="AF17" s="10" t="n">
+      <c r="AF17" s="2" t="n">
         <v>3351225956.68921</v>
       </c>
-      <c r="AG17" s="10" t="n">
+      <c r="AG17" s="2" t="n">
         <v>5056314730.71768</v>
       </c>
-      <c r="AH17" s="10" t="n">
+      <c r="AH17" s="2" t="n">
         <v>9689975460.48866</v>
       </c>
-      <c r="AI17" s="10" t="n">
+      <c r="AI17" s="2" t="n">
         <v>9647629779.3483</v>
       </c>
-      <c r="AJ17" s="10" t="n">
+      <c r="AJ17" s="2" t="n">
         <v>11169563015.1701</v>
       </c>
-      <c r="AK17" s="10" t="n">
+      <c r="AK17" s="2" t="n">
         <v>21930105676.6872</v>
       </c>
-      <c r="AL17" s="10" t="n">
+      <c r="AL17" s="2" t="n">
         <v>19550596323.611</v>
       </c>
-      <c r="AM17" s="10" t="n">
+      <c r="AM17" s="2" t="n">
         <v>23658498563.3684</v>
       </c>
-      <c r="AN17" s="10" t="n">
+      <c r="AN17" s="2" t="n">
         <v>19228312977.8257</v>
       </c>
-      <c r="AO17" s="10" t="n">
+      <c r="AO17" s="2" t="n">
         <v>22204438295.4597</v>
       </c>
-      <c r="AP17" s="10" t="n">
+      <c r="AP17" s="2" t="n">
         <v>19701607199.2135</v>
       </c>
-      <c r="AQ17" s="10" t="n">
+      <c r="AQ17" s="2" t="n">
         <v>16272835609.4825</v>
       </c>
-      <c r="AR17" s="10" t="n">
+      <c r="AR17" s="2" t="n">
         <v>19220458282.8904</v>
       </c>
-      <c r="AS17" s="10" t="n">
+      <c r="AS17" s="2" t="n">
         <v>23365991209.5999</v>
       </c>
-      <c r="AT17" s="10" t="n">
+      <c r="AT17" s="2" t="n">
         <v>18074256698.7538</v>
       </c>
-      <c r="AU17" s="10" t="n">
+      <c r="AU17" s="2" t="n">
         <v>18954458708.1024</v>
       </c>
-      <c r="AV17" s="10" t="n">
+      <c r="AV17" s="2" t="n">
         <v>14287090543.2938</v>
       </c>
-      <c r="AW17" s="10" t="n">
+      <c r="AW17" s="2" t="n">
         <v>18529774324.4552</v>
       </c>
-      <c r="AX17" s="10"/>
+      <c r="AX17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -6070,89 +6341,89 @@
       <c r="O18" t="s">
         <v>57</v>
       </c>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10" t="n">
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2" t="n">
         <v>7682614385.97241</v>
       </c>
-      <c r="AA18" s="10" t="n">
+      <c r="AA18" s="2" t="n">
         <v>8013453483.81472</v>
       </c>
-      <c r="AB18" s="10" t="n">
+      <c r="AB18" s="2" t="n">
         <v>9157143809.7321</v>
       </c>
-      <c r="AC18" s="10" t="n">
+      <c r="AC18" s="2" t="n">
         <v>16560363869.0103</v>
       </c>
-      <c r="AD18" s="10" t="n">
+      <c r="AD18" s="2" t="n">
         <v>17475260624.7798</v>
       </c>
-      <c r="AE18" s="10" t="n">
+      <c r="AE18" s="2" t="n">
         <v>17192978801.9298</v>
       </c>
-      <c r="AF18" s="10" t="n">
+      <c r="AF18" s="2" t="n">
         <v>19511047169.0537</v>
       </c>
-      <c r="AG18" s="10" t="n">
+      <c r="AG18" s="2" t="n">
         <v>18108217362.1872</v>
       </c>
-      <c r="AH18" s="10" t="n">
+      <c r="AH18" s="2" t="n">
         <v>17096875385.7715</v>
       </c>
-      <c r="AI18" s="10" t="n">
+      <c r="AI18" s="2" t="n">
         <v>15756726699.6686</v>
       </c>
-      <c r="AJ18" s="10" t="n">
+      <c r="AJ18" s="2" t="n">
         <v>16397354369</v>
       </c>
-      <c r="AK18" s="10" t="n">
+      <c r="AK18" s="2" t="n">
         <v>14865363804.9205</v>
       </c>
-      <c r="AL18" s="10" t="n">
+      <c r="AL18" s="2" t="n">
         <v>15475520119.8005</v>
       </c>
-      <c r="AM18" s="10" t="n">
+      <c r="AM18" s="2" t="n">
         <v>14403371586.4019</v>
       </c>
-      <c r="AN18" s="10" t="n">
+      <c r="AN18" s="2" t="n">
         <v>14031363546.5291</v>
       </c>
-      <c r="AO18" s="10" t="n">
+      <c r="AO18" s="2" t="n">
         <v>13363749120.0494</v>
       </c>
-      <c r="AP18" s="10" t="n">
+      <c r="AP18" s="2" t="n">
         <v>13621349538.9329</v>
       </c>
-      <c r="AQ18" s="10" t="n">
+      <c r="AQ18" s="2" t="n">
         <v>14731781979.9485</v>
       </c>
-      <c r="AR18" s="10" t="n">
+      <c r="AR18" s="2" t="n">
         <v>12910793067.7795</v>
       </c>
-      <c r="AS18" s="10" t="n">
+      <c r="AS18" s="2" t="n">
         <v>13732936917.4288</v>
       </c>
-      <c r="AT18" s="10" t="n">
+      <c r="AT18" s="2" t="n">
         <v>9698698419.27091</v>
       </c>
-      <c r="AU18" s="10" t="n">
+      <c r="AU18" s="2" t="n">
         <v>9916244181.73727</v>
       </c>
-      <c r="AV18" s="10" t="n">
+      <c r="AV18" s="2" t="n">
         <v>9580549306.11</v>
       </c>
-      <c r="AW18" s="10" t="n">
+      <c r="AW18" s="2" t="n">
         <v>3997131427.13735</v>
       </c>
-      <c r="AX18" s="10"/>
+      <c r="AX18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -6170,89 +6441,89 @@
       <c r="O19" t="s">
         <v>59</v>
       </c>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="10" t="n">
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2" t="n">
         <v>11954637598.4551</v>
       </c>
-      <c r="AA19" s="10" t="n">
+      <c r="AA19" s="2" t="n">
         <v>10021831081.5773</v>
       </c>
-      <c r="AB19" s="10" t="n">
+      <c r="AB19" s="2" t="n">
         <v>7909870478.0366</v>
       </c>
-      <c r="AC19" s="10" t="n">
+      <c r="AC19" s="2" t="n">
         <v>9034222284.86127</v>
       </c>
-      <c r="AD19" s="10" t="n">
+      <c r="AD19" s="2" t="n">
         <v>7442031343.97848</v>
       </c>
-      <c r="AE19" s="10" t="n">
+      <c r="AE19" s="2" t="n">
         <v>5505678606.48885</v>
       </c>
-      <c r="AF19" s="10" t="n">
+      <c r="AF19" s="2" t="n">
         <v>6356942480.52977</v>
       </c>
-      <c r="AG19" s="10" t="n">
+      <c r="AG19" s="2" t="n">
         <v>10165867816.7477</v>
       </c>
-      <c r="AH19" s="10" t="n">
+      <c r="AH19" s="2" t="n">
         <v>6048295623.66257</v>
       </c>
-      <c r="AI19" s="10" t="n">
+      <c r="AI19" s="2" t="n">
         <v>7690844290.77725</v>
       </c>
-      <c r="AJ19" s="10" t="n">
+      <c r="AJ19" s="2" t="n">
         <v>7853493803.23143</v>
       </c>
-      <c r="AK19" s="10" t="n">
+      <c r="AK19" s="2" t="n">
         <v>4260947145.51411</v>
       </c>
-      <c r="AL19" s="10" t="n">
+      <c r="AL19" s="2" t="n">
         <v>14649069981.9448</v>
       </c>
-      <c r="AM19" s="10" t="n">
+      <c r="AM19" s="2" t="n">
         <v>11891571179.6987</v>
       </c>
-      <c r="AN19" s="10" t="n">
+      <c r="AN19" s="2" t="n">
         <v>3509648722.82898</v>
       </c>
-      <c r="AO19" s="10" t="n">
+      <c r="AO19" s="2" t="n">
         <v>2827478909.49259</v>
       </c>
-      <c r="AP19" s="10" t="n">
+      <c r="AP19" s="2" t="n">
         <v>17352898415.6251</v>
       </c>
-      <c r="AQ19" s="10" t="n">
+      <c r="AQ19" s="2" t="n">
         <v>30822794580.9453</v>
       </c>
-      <c r="AR19" s="10" t="n">
+      <c r="AR19" s="2" t="n">
         <v>23746441999.9417</v>
       </c>
-      <c r="AS19" s="10" t="n">
+      <c r="AS19" s="2" t="n">
         <v>17460308734.66</v>
       </c>
-      <c r="AT19" s="10" t="n">
+      <c r="AT19" s="2" t="n">
         <v>40916342412.9054</v>
       </c>
-      <c r="AU19" s="10" t="n">
+      <c r="AU19" s="2" t="n">
         <v>11869615439.7573</v>
       </c>
-      <c r="AV19" s="10" t="n">
+      <c r="AV19" s="2" t="n">
         <v>18909526156.1226</v>
       </c>
-      <c r="AW19" s="10" t="n">
+      <c r="AW19" s="2" t="n">
         <v>7739152359.87302</v>
       </c>
-      <c r="AX19" s="10"/>
+      <c r="AX19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -6270,81 +6541,81 @@
       <c r="O20" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10" t="n">
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA20" s="10"/>
-      <c r="AB20" s="10" t="n">
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2" t="n">
         <v>7747746.57784681</v>
       </c>
-      <c r="AC20" s="10" t="n">
+      <c r="AC20" s="2" t="n">
         <v>990400.440211295</v>
       </c>
-      <c r="AD20" s="10" t="n">
+      <c r="AD20" s="2" t="n">
         <v>4468575.32576727</v>
       </c>
-      <c r="AE20" s="10" t="n">
+      <c r="AE20" s="2" t="n">
         <v>33751629.2527597</v>
       </c>
-      <c r="AF20" s="10" t="n">
+      <c r="AF20" s="2" t="n">
         <v>74385339.5781023</v>
       </c>
-      <c r="AG20" s="10" t="n">
+      <c r="AG20" s="2" t="n">
         <v>1220871784.48958</v>
       </c>
-      <c r="AH20" s="10" t="n">
+      <c r="AH20" s="2" t="n">
         <v>2354532802.92702</v>
       </c>
-      <c r="AI20" s="10" t="n">
+      <c r="AI20" s="2" t="n">
         <v>3379553708.48206</v>
       </c>
-      <c r="AJ20" s="10" t="n">
+      <c r="AJ20" s="2" t="n">
         <v>13768679.6233095</v>
       </c>
-      <c r="AK20" s="10" t="n">
+      <c r="AK20" s="2" t="n">
         <v>291121.503866934</v>
       </c>
-      <c r="AL20" s="10" t="n">
+      <c r="AL20" s="2" t="n">
         <v>-7578537.27282939</v>
       </c>
-      <c r="AM20" s="10" t="n">
+      <c r="AM20" s="2" t="n">
         <v>-4926677.66847769</v>
       </c>
-      <c r="AN20" s="10" t="n">
+      <c r="AN20" s="2" t="n">
         <v>-2143749.02223787</v>
       </c>
-      <c r="AO20" s="10" t="n">
+      <c r="AO20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AP20" s="10" t="n">
+      <c r="AP20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ20" s="10" t="n">
+      <c r="AQ20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AR20" s="10" t="n">
+      <c r="AR20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS20" s="10" t="n">
+      <c r="AS20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AT20" s="10" t="n">
+      <c r="AT20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU20" s="10"/>
-      <c r="AV20" s="10"/>
-      <c r="AW20" s="10"/>
-      <c r="AX20" s="10"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -6360,109 +6631,109 @@
         <v>60</v>
       </c>
       <c r="O21"/>
-      <c r="P21" s="10" t="n">
+      <c r="P21" s="2" t="n">
         <v>61574219146.1011</v>
       </c>
-      <c r="Q21" s="10" t="n">
+      <c r="Q21" s="2" t="n">
         <v>58557064802.4477</v>
       </c>
-      <c r="R21" s="10" t="n">
+      <c r="R21" s="2" t="n">
         <v>56801379064.5588</v>
       </c>
-      <c r="S21" s="10" t="n">
+      <c r="S21" s="2" t="n">
         <v>54729508899.5979</v>
       </c>
-      <c r="T21" s="10" t="n">
+      <c r="T21" s="2" t="n">
         <v>54688352602.1809</v>
       </c>
-      <c r="U21" s="10" t="n">
+      <c r="U21" s="2" t="n">
         <v>47012064374.5043</v>
       </c>
-      <c r="V21" s="10" t="n">
+      <c r="V21" s="2" t="n">
         <v>49656147326.0405</v>
       </c>
-      <c r="W21" s="10" t="n">
+      <c r="W21" s="2" t="n">
         <v>42152791540.17</v>
       </c>
-      <c r="X21" s="10" t="n">
+      <c r="X21" s="2" t="n">
         <v>44303062515.0653</v>
       </c>
-      <c r="Y21" s="10" t="n">
+      <c r="Y21" s="2" t="n">
         <v>45432730399.186</v>
       </c>
-      <c r="Z21" s="10" t="n">
+      <c r="Z21" s="2" t="n">
         <v>1883108552.16094</v>
       </c>
-      <c r="AA21" s="10" t="n">
+      <c r="AA21" s="2" t="n">
         <v>129655403.210666</v>
       </c>
-      <c r="AB21" s="10" t="n">
+      <c r="AB21" s="2" t="n">
         <v>205769202.437913</v>
       </c>
-      <c r="AC21" s="10" t="n">
+      <c r="AC21" s="2" t="n">
         <v>257016003.130769</v>
       </c>
-      <c r="AD21" s="10" t="n">
+      <c r="AD21" s="2" t="n">
         <v>284081906.561755</v>
       </c>
-      <c r="AE21" s="10" t="n">
+      <c r="AE21" s="2" t="n">
         <v>254347287.16124</v>
       </c>
-      <c r="AF21" s="10" t="n">
+      <c r="AF21" s="2" t="n">
         <v>93204512.7596402</v>
       </c>
-      <c r="AG21" s="10" t="n">
+      <c r="AG21" s="2" t="n">
         <v>16138072.5691724</v>
       </c>
-      <c r="AH21" s="10" t="n">
+      <c r="AH21" s="2" t="n">
         <v>1458190475.1103</v>
       </c>
-      <c r="AI21" s="10" t="n">
+      <c r="AI21" s="2" t="n">
         <v>2272323098.55858</v>
       </c>
-      <c r="AJ21" s="10" t="n">
+      <c r="AJ21" s="2" t="n">
         <v>1126214460.44692</v>
       </c>
-      <c r="AK21" s="10" t="n">
+      <c r="AK21" s="2" t="n">
         <v>1812763011.18012</v>
       </c>
-      <c r="AL21" s="10" t="n">
+      <c r="AL21" s="2" t="n">
         <v>3951923321.90102</v>
       </c>
-      <c r="AM21" s="10" t="n">
+      <c r="AM21" s="2" t="n">
         <v>181287982.68239</v>
       </c>
-      <c r="AN21" s="10" t="n">
+      <c r="AN21" s="2" t="n">
         <v>169338080.11077</v>
       </c>
-      <c r="AO21" s="10" t="n">
+      <c r="AO21" s="2" t="n">
         <v>290753493.787097</v>
       </c>
-      <c r="AP21" s="10" t="n">
+      <c r="AP21" s="2" t="n">
         <v>534367944.916519</v>
       </c>
-      <c r="AQ21" s="10" t="n">
+      <c r="AQ21" s="2" t="n">
         <v>-14258218.3023654</v>
       </c>
-      <c r="AR21" s="10" t="n">
+      <c r="AR21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS21" s="10" t="n">
+      <c r="AS21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AT21" s="10" t="n">
+      <c r="AT21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU21" s="10" t="n">
+      <c r="AU21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AV21" s="10" t="n">
+      <c r="AV21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW21" s="10" t="n">
+      <c r="AW21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AX21" s="10"/>
+      <c r="AX21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -6471,41 +6742,41 @@
       <c r="B22" t="str">
         <f>O22</f>
       </c>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="10"/>
-      <c r="Y22" s="10"/>
-      <c r="Z22" s="10"/>
-      <c r="AA22" s="10"/>
-      <c r="AB22" s="10"/>
-      <c r="AC22" s="10"/>
-      <c r="AD22" s="10"/>
-      <c r="AE22" s="10"/>
-      <c r="AF22" s="10"/>
-      <c r="AG22" s="10"/>
-      <c r="AH22" s="10"/>
-      <c r="AI22" s="10"/>
-      <c r="AJ22" s="10"/>
-      <c r="AK22" s="10"/>
-      <c r="AL22" s="10"/>
-      <c r="AM22" s="10"/>
-      <c r="AN22" s="10"/>
-      <c r="AO22" s="10"/>
-      <c r="AP22" s="10"/>
-      <c r="AQ22" s="10"/>
-      <c r="AR22" s="10"/>
-      <c r="AS22" s="10"/>
-      <c r="AT22" s="10"/>
-      <c r="AU22" s="10"/>
-      <c r="AV22" s="10"/>
-      <c r="AW22" s="10"/>
-      <c r="AX22" s="10"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="2"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+      <c r="AX22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cleaning up acq trends and updating for 2024.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/Platform/Aircraft/DoD_Aircraft_Contracts.xlsx
+++ b/Output/AcqTrends/Platform/Aircraft/DoD_Aircraft_Contracts.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="441">
   <si>
     <t xml:space="preserve">SimpleArea</t>
   </si>
@@ -1353,6 +1353,9 @@
   <si>
     <t xml:space="preserve">Small</t>
   </si>
+  <si>
+    <t xml:space="preserve">Firm Fixed-Price</t>
+  </si>
 </sst>
 </file>
 
@@ -1368,8 +1371,8 @@
     <numFmt numFmtId="191" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="180" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="192" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="199" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="200" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="201" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1417,8 +1420,8 @@
     <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="192" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="199" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="200" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="201" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3006,110 +3009,110 @@
       <c r="K2" t="s">
         <v>436</v>
       </c>
-      <c r="L2" s="12" t="n">
+      <c r="L2" s="11" t="n">
         <v>15816663707</v>
       </c>
-      <c r="M2" s="12" t="n">
+      <c r="M2" s="11" t="n">
         <v>16474737362</v>
       </c>
-      <c r="N2" s="12" t="n">
+      <c r="N2" s="11" t="n">
         <v>17584653615</v>
       </c>
-      <c r="O2" s="12" t="n">
+      <c r="O2" s="11" t="n">
         <v>16728803202</v>
       </c>
-      <c r="P2" s="12" t="n">
+      <c r="P2" s="11" t="n">
         <v>17955716132</v>
       </c>
-      <c r="Q2" s="12" t="n">
+      <c r="Q2" s="11" t="n">
         <v>15667368304</v>
       </c>
-      <c r="R2" s="12" t="n">
+      <c r="R2" s="11" t="n">
         <v>18103520038</v>
       </c>
-      <c r="S2" s="12" t="n">
+      <c r="S2" s="11" t="n">
         <v>15325262721</v>
       </c>
-      <c r="T2" s="12" t="n">
+      <c r="T2" s="11" t="n">
         <v>16093030160</v>
       </c>
-      <c r="U2" s="12" t="n">
+      <c r="U2" s="11" t="n">
         <v>16915693475</v>
       </c>
-      <c r="V2" s="12" t="n">
+      <c r="V2" s="11" t="n">
         <v>20722676885</v>
       </c>
-      <c r="W2" s="12" t="n">
+      <c r="W2" s="11" t="n">
         <v>21761336175.5937</v>
       </c>
-      <c r="X2" s="12" t="n">
+      <c r="X2" s="11" t="n">
         <v>23961181162.7736</v>
       </c>
-      <c r="Y2" s="12" t="n">
+      <c r="Y2" s="11" t="n">
         <v>31136198789.9492</v>
       </c>
-      <c r="Z2" s="12" t="n">
+      <c r="Z2" s="11" t="n">
         <v>28603329358.0938</v>
       </c>
-      <c r="AA2" s="12" t="n">
+      <c r="AA2" s="11" t="n">
         <v>26047952355.0648</v>
       </c>
-      <c r="AB2" s="12" t="n">
+      <c r="AB2" s="11" t="n">
         <v>32653119152.2924</v>
       </c>
-      <c r="AC2" s="12" t="n">
+      <c r="AC2" s="11" t="n">
         <v>37354806997.4986</v>
       </c>
-      <c r="AD2" s="12" t="n">
+      <c r="AD2" s="11" t="n">
         <v>38068635593.0428</v>
       </c>
-      <c r="AE2" s="12" t="n">
+      <c r="AE2" s="11" t="n">
         <v>38461921152.3791</v>
       </c>
-      <c r="AF2" s="12" t="n">
+      <c r="AF2" s="11" t="n">
         <v>35332699711.0399</v>
       </c>
-      <c r="AG2" s="12" t="n">
+      <c r="AG2" s="11" t="n">
         <v>40589378944.0771</v>
       </c>
-      <c r="AH2" s="12" t="n">
+      <c r="AH2" s="11" t="n">
         <v>47634560322.7732</v>
       </c>
-      <c r="AI2" s="12" t="n">
+      <c r="AI2" s="11" t="n">
         <v>46490126493.4294</v>
       </c>
-      <c r="AJ2" s="12" t="n">
+      <c r="AJ2" s="11" t="n">
         <v>33268005196.5538</v>
       </c>
-      <c r="AK2" s="12" t="n">
+      <c r="AK2" s="11" t="n">
         <v>36231080536.9384</v>
       </c>
-      <c r="AL2" s="12" t="n">
+      <c r="AL2" s="11" t="n">
         <v>51768178639.0963</v>
       </c>
-      <c r="AM2" s="12" t="n">
+      <c r="AM2" s="11" t="n">
         <v>61695117390.5634</v>
       </c>
-      <c r="AN2" s="12" t="n">
+      <c r="AN2" s="11" t="n">
         <v>53561150365.9478</v>
       </c>
-      <c r="AO2" s="12" t="n">
+      <c r="AO2" s="11" t="n">
         <v>55232460117.1769</v>
       </c>
-      <c r="AP2" s="12" t="n">
+      <c r="AP2" s="11" t="n">
         <v>74666679382.3874</v>
       </c>
-      <c r="AQ2" s="12" t="n">
+      <c r="AQ2" s="11" t="n">
         <v>50987030472.3396</v>
       </c>
-      <c r="AR2" s="12" t="n">
+      <c r="AR2" s="11" t="n">
         <v>53457678478.0773</v>
       </c>
-      <c r="AS2" s="12" t="n">
+      <c r="AS2" s="11" t="n">
         <v>39359687569.1563</v>
       </c>
-      <c r="AT2" s="12"/>
-      <c r="AU2" s="12"/>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="11"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -3118,110 +3121,110 @@
       <c r="K3" t="s">
         <v>437</v>
       </c>
-      <c r="L3" s="12" t="n">
+      <c r="L3" s="11" t="n">
         <v>10171551107</v>
       </c>
-      <c r="M3" s="12" t="n">
+      <c r="M3" s="11" t="n">
         <v>8265092207</v>
       </c>
-      <c r="N3" s="12" t="n">
+      <c r="N3" s="11" t="n">
         <v>8128244723</v>
       </c>
-      <c r="O3" s="12" t="n">
+      <c r="O3" s="11" t="n">
         <v>8469222751</v>
       </c>
-      <c r="P3" s="12" t="n">
+      <c r="P3" s="11" t="n">
         <v>8108616677</v>
       </c>
-      <c r="Q3" s="12" t="n">
+      <c r="Q3" s="11" t="n">
         <v>6967280359</v>
       </c>
-      <c r="R3" s="12" t="n">
+      <c r="R3" s="11" t="n">
         <v>7131133532</v>
       </c>
-      <c r="S3" s="12" t="n">
+      <c r="S3" s="11" t="n">
         <v>6502953802</v>
       </c>
-      <c r="T3" s="12" t="n">
+      <c r="T3" s="11" t="n">
         <v>6988516165</v>
       </c>
-      <c r="U3" s="12" t="n">
+      <c r="U3" s="11" t="n">
         <v>6982779203</v>
       </c>
-      <c r="V3" s="12" t="n">
+      <c r="V3" s="11" t="n">
         <v>9088859410.53</v>
       </c>
-      <c r="W3" s="12" t="n">
+      <c r="W3" s="11" t="n">
         <v>9201350077.4766</v>
       </c>
-      <c r="X3" s="12" t="n">
+      <c r="X3" s="11" t="n">
         <v>9553877677.0342</v>
       </c>
-      <c r="Y3" s="12" t="n">
+      <c r="Y3" s="11" t="n">
         <v>12975707919.875</v>
       </c>
-      <c r="Z3" s="12" t="n">
+      <c r="Z3" s="11" t="n">
         <v>13535861871.5376</v>
       </c>
-      <c r="AA3" s="12" t="n">
+      <c r="AA3" s="11" t="n">
         <v>14630917283.736</v>
       </c>
-      <c r="AB3" s="12" t="n">
+      <c r="AB3" s="11" t="n">
         <v>14947962849.0103</v>
       </c>
-      <c r="AC3" s="12" t="n">
+      <c r="AC3" s="11" t="n">
         <v>16734660573.0448</v>
       </c>
-      <c r="AD3" s="12" t="n">
+      <c r="AD3" s="11" t="n">
         <v>21287099718.0048</v>
       </c>
-      <c r="AE3" s="12" t="n">
+      <c r="AE3" s="11" t="n">
         <v>19769512312.7579</v>
       </c>
-      <c r="AF3" s="12" t="n">
+      <c r="AF3" s="11" t="n">
         <v>19668575054.5295</v>
       </c>
-      <c r="AG3" s="12" t="n">
+      <c r="AG3" s="11" t="n">
         <v>20708903822.3218</v>
       </c>
-      <c r="AH3" s="12" t="n">
+      <c r="AH3" s="11" t="n">
         <v>20414673841.8096</v>
       </c>
-      <c r="AI3" s="12" t="n">
+      <c r="AI3" s="11" t="n">
         <v>17452048725.1215</v>
       </c>
-      <c r="AJ3" s="12" t="n">
+      <c r="AJ3" s="11" t="n">
         <v>16682825690.0802</v>
       </c>
-      <c r="AK3" s="12" t="n">
+      <c r="AK3" s="11" t="n">
         <v>16597128985.5856</v>
       </c>
-      <c r="AL3" s="12" t="n">
+      <c r="AL3" s="11" t="n">
         <v>14666663228.0641</v>
       </c>
-      <c r="AM3" s="12" t="n">
+      <c r="AM3" s="11" t="n">
         <v>13441942817.624</v>
       </c>
-      <c r="AN3" s="12" t="n">
+      <c r="AN3" s="11" t="n">
         <v>17412773232.5515</v>
       </c>
-      <c r="AO3" s="12" t="n">
+      <c r="AO3" s="11" t="n">
         <v>20705787814.5047</v>
       </c>
-      <c r="AP3" s="12" t="n">
+      <c r="AP3" s="11" t="n">
         <v>17975190893.2119</v>
       </c>
-      <c r="AQ3" s="12" t="n">
+      <c r="AQ3" s="11" t="n">
         <v>10292828767.8784</v>
       </c>
-      <c r="AR3" s="12" t="n">
+      <c r="AR3" s="11" t="n">
         <v>9796794669.8747</v>
       </c>
-      <c r="AS3" s="12" t="n">
+      <c r="AS3" s="11" t="n">
         <v>5256777391.4184</v>
       </c>
-      <c r="AT3" s="12"/>
-      <c r="AU3" s="12"/>
+      <c r="AT3" s="11"/>
+      <c r="AU3" s="11"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -3230,110 +3233,110 @@
       <c r="K4" t="s">
         <v>438</v>
       </c>
-      <c r="L4" s="12" t="n">
+      <c r="L4" s="11" t="n">
         <v>2843791610</v>
       </c>
-      <c r="M4" s="12" t="n">
+      <c r="M4" s="11" t="n">
         <v>4106016003</v>
       </c>
-      <c r="N4" s="12" t="n">
+      <c r="N4" s="11" t="n">
         <v>3292005381</v>
       </c>
-      <c r="O4" s="12" t="n">
+      <c r="O4" s="11" t="n">
         <v>3271657960</v>
       </c>
-      <c r="P4" s="12" t="n">
+      <c r="P4" s="11" t="n">
         <v>2882674802</v>
       </c>
-      <c r="Q4" s="12" t="n">
+      <c r="Q4" s="11" t="n">
         <v>2738404977</v>
       </c>
-      <c r="R4" s="12" t="n">
+      <c r="R4" s="11" t="n">
         <v>2037110094</v>
       </c>
-      <c r="S4" s="12" t="n">
+      <c r="S4" s="11" t="n">
         <v>1900576876</v>
       </c>
-      <c r="T4" s="12" t="n">
+      <c r="T4" s="11" t="n">
         <v>2145818346</v>
       </c>
-      <c r="U4" s="12" t="n">
+      <c r="U4" s="11" t="n">
         <v>2130794274</v>
       </c>
-      <c r="V4" s="12" t="n">
+      <c r="V4" s="11" t="n">
         <v>3372551686</v>
       </c>
-      <c r="W4" s="12" t="n">
+      <c r="W4" s="11" t="n">
         <v>3154776159.6191</v>
       </c>
-      <c r="X4" s="12" t="n">
+      <c r="X4" s="11" t="n">
         <v>3055742922.54</v>
       </c>
-      <c r="Y4" s="12" t="n">
+      <c r="Y4" s="11" t="n">
         <v>2569363809.8101</v>
       </c>
-      <c r="Z4" s="12" t="n">
+      <c r="Z4" s="11" t="n">
         <v>3085304479.3316</v>
       </c>
-      <c r="AA4" s="12" t="n">
+      <c r="AA4" s="11" t="n">
         <v>3610218000.0183</v>
       </c>
-      <c r="AB4" s="12" t="n">
+      <c r="AB4" s="11" t="n">
         <v>3522183905.5044</v>
       </c>
-      <c r="AC4" s="12" t="n">
+      <c r="AC4" s="11" t="n">
         <v>3397820321.6894</v>
       </c>
-      <c r="AD4" s="12" t="n">
+      <c r="AD4" s="11" t="n">
         <v>3921180186.4921</v>
       </c>
-      <c r="AE4" s="12" t="n">
+      <c r="AE4" s="11" t="n">
         <v>4278416438.8401</v>
       </c>
-      <c r="AF4" s="12" t="n">
+      <c r="AF4" s="11" t="n">
         <v>5054428458.7845</v>
       </c>
-      <c r="AG4" s="12" t="n">
+      <c r="AG4" s="11" t="n">
         <v>5592081696.1289</v>
       </c>
-      <c r="AH4" s="12" t="n">
+      <c r="AH4" s="11" t="n">
         <v>6635887450.6113</v>
       </c>
-      <c r="AI4" s="12" t="n">
+      <c r="AI4" s="11" t="n">
         <v>5918208574.5945</v>
       </c>
-      <c r="AJ4" s="12" t="n">
+      <c r="AJ4" s="11" t="n">
         <v>4814056127.2545</v>
       </c>
-      <c r="AK4" s="12" t="n">
+      <c r="AK4" s="11" t="n">
         <v>5377599072.9</v>
       </c>
-      <c r="AL4" s="12" t="n">
+      <c r="AL4" s="11" t="n">
         <v>5189260122.595</v>
       </c>
-      <c r="AM4" s="12" t="n">
+      <c r="AM4" s="11" t="n">
         <v>6739988065.9482</v>
       </c>
-      <c r="AN4" s="12" t="n">
+      <c r="AN4" s="11" t="n">
         <v>7524576939.9021</v>
       </c>
-      <c r="AO4" s="12" t="n">
+      <c r="AO4" s="11" t="n">
         <v>9152103661.3746</v>
       </c>
-      <c r="AP4" s="12" t="n">
+      <c r="AP4" s="11" t="n">
         <v>8603978722.3014</v>
       </c>
-      <c r="AQ4" s="12" t="n">
+      <c r="AQ4" s="11" t="n">
         <v>7550202408.2141</v>
       </c>
-      <c r="AR4" s="12" t="n">
+      <c r="AR4" s="11" t="n">
         <v>8137614778.7914</v>
       </c>
-      <c r="AS4" s="12" t="n">
+      <c r="AS4" s="11" t="n">
         <v>4373708938.9382</v>
       </c>
-      <c r="AT4" s="12"/>
-      <c r="AU4" s="12"/>
+      <c r="AT4" s="11"/>
+      <c r="AU4" s="11"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -3342,110 +3345,110 @@
       <c r="K5" t="s">
         <v>439</v>
       </c>
-      <c r="L5" s="12" t="n">
+      <c r="L5" s="11" t="n">
         <v>865758724</v>
       </c>
-      <c r="M5" s="12" t="n">
+      <c r="M5" s="11" t="n">
         <v>1375587135</v>
       </c>
-      <c r="N5" s="12" t="n">
+      <c r="N5" s="11" t="n">
         <v>985713445</v>
       </c>
-      <c r="O5" s="12" t="n">
+      <c r="O5" s="11" t="n">
         <v>1074041350</v>
       </c>
-      <c r="P5" s="12" t="n">
+      <c r="P5" s="11" t="n">
         <v>1067354203</v>
       </c>
-      <c r="Q5" s="12" t="n">
+      <c r="Q5" s="11" t="n">
         <v>1120586850</v>
       </c>
-      <c r="R5" s="12" t="n">
+      <c r="R5" s="11" t="n">
         <v>1219219467</v>
       </c>
-      <c r="S5" s="12" t="n">
+      <c r="S5" s="11" t="n">
         <v>1194879229</v>
       </c>
-      <c r="T5" s="12" t="n">
+      <c r="T5" s="11" t="n">
         <v>1270277857</v>
       </c>
-      <c r="U5" s="12" t="n">
+      <c r="U5" s="11" t="n">
         <v>1514108183</v>
       </c>
-      <c r="V5" s="12" t="n">
+      <c r="V5" s="11" t="n">
         <v>2218426809</v>
       </c>
-      <c r="W5" s="12" t="n">
+      <c r="W5" s="11" t="n">
         <v>2004263635.25</v>
       </c>
-      <c r="X5" s="12" t="n">
+      <c r="X5" s="11" t="n">
         <v>2454557553.8184</v>
       </c>
-      <c r="Y5" s="12" t="n">
+      <c r="Y5" s="11" t="n">
         <v>2559124261.8224</v>
       </c>
-      <c r="Z5" s="12" t="n">
+      <c r="Z5" s="11" t="n">
         <v>2566791213.0151</v>
       </c>
-      <c r="AA5" s="12" t="n">
+      <c r="AA5" s="11" t="n">
         <v>2983996530.2644</v>
       </c>
-      <c r="AB5" s="12" t="n">
+      <c r="AB5" s="11" t="n">
         <v>2841422561.5128</v>
       </c>
-      <c r="AC5" s="12" t="n">
+      <c r="AC5" s="11" t="n">
         <v>2992214148.6039</v>
       </c>
-      <c r="AD5" s="12" t="n">
+      <c r="AD5" s="11" t="n">
         <v>3436820597.7773</v>
       </c>
-      <c r="AE5" s="12" t="n">
+      <c r="AE5" s="11" t="n">
         <v>3332443432.9409</v>
       </c>
-      <c r="AF5" s="12" t="n">
+      <c r="AF5" s="11" t="n">
         <v>3503812205.5045</v>
       </c>
-      <c r="AG5" s="12" t="n">
+      <c r="AG5" s="11" t="n">
         <v>3325236934.5515</v>
       </c>
-      <c r="AH5" s="12" t="n">
+      <c r="AH5" s="11" t="n">
         <v>3466048377.0804</v>
       </c>
-      <c r="AI5" s="12" t="n">
+      <c r="AI5" s="11" t="n">
         <v>3392920923.5844</v>
       </c>
-      <c r="AJ5" s="12" t="n">
+      <c r="AJ5" s="11" t="n">
         <v>3451559036.4829</v>
       </c>
-      <c r="AK5" s="12" t="n">
+      <c r="AK5" s="11" t="n">
         <v>3488123938.7881</v>
       </c>
-      <c r="AL5" s="12" t="n">
+      <c r="AL5" s="11" t="n">
         <v>3721780510.6998</v>
       </c>
-      <c r="AM5" s="12" t="n">
+      <c r="AM5" s="11" t="n">
         <v>3945304481.9703</v>
       </c>
-      <c r="AN5" s="12" t="n">
+      <c r="AN5" s="11" t="n">
         <v>4839532796.3896</v>
       </c>
-      <c r="AO5" s="12" t="n">
+      <c r="AO5" s="11" t="n">
         <v>4997409450.861</v>
       </c>
-      <c r="AP5" s="12" t="n">
+      <c r="AP5" s="11" t="n">
         <v>4026004833.4548</v>
       </c>
-      <c r="AQ5" s="12" t="n">
+      <c r="AQ5" s="11" t="n">
         <v>3625227535.7022</v>
       </c>
-      <c r="AR5" s="12" t="n">
+      <c r="AR5" s="11" t="n">
         <v>3755209682.6872</v>
       </c>
-      <c r="AS5" s="12" t="n">
+      <c r="AS5" s="11" t="n">
         <v>1262329499.3766</v>
       </c>
-      <c r="AT5" s="12"/>
-      <c r="AU5" s="12"/>
+      <c r="AT5" s="11"/>
+      <c r="AU5" s="11"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -3454,110 +3457,110 @@
       <c r="K6" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="12" t="n">
+      <c r="L6" s="11" t="n">
         <v>1282482000</v>
       </c>
-      <c r="M6" s="12" t="n">
+      <c r="M6" s="11" t="n">
         <v>291666548</v>
       </c>
-      <c r="N6" s="12" t="n">
+      <c r="N6" s="11" t="n">
         <v>347354403</v>
       </c>
-      <c r="O6" s="12" t="n">
+      <c r="O6" s="11" t="n">
         <v>374319602</v>
       </c>
-      <c r="P6" s="12" t="n">
+      <c r="P6" s="11" t="n">
         <v>532598591</v>
       </c>
-      <c r="Q6" s="12" t="n">
+      <c r="Q6" s="11" t="n">
         <v>321864828</v>
       </c>
-      <c r="R6" s="12" t="n">
+      <c r="R6" s="11" t="n">
         <v>365023059</v>
       </c>
-      <c r="S6" s="12" t="n">
+      <c r="S6" s="11" t="n">
         <v>7161291</v>
       </c>
-      <c r="T6" s="12" t="n">
+      <c r="T6" s="11" t="n">
         <v>32127541</v>
       </c>
-      <c r="U6" s="12" t="n">
+      <c r="U6" s="11" t="n">
         <v>1998996</v>
       </c>
-      <c r="V6" s="12" t="n">
+      <c r="V6" s="11" t="n">
         <v>17823274</v>
       </c>
-      <c r="W6" s="12" t="n">
+      <c r="W6" s="11" t="n">
         <v>120000</v>
       </c>
-      <c r="X6" s="12" t="n">
+      <c r="X6" s="11" t="n">
         <v>530245</v>
       </c>
-      <c r="Y6" s="12" t="n">
+      <c r="Y6" s="11" t="n">
         <v>4625405</v>
       </c>
-      <c r="Z6" s="12" t="n">
+      <c r="Z6" s="11" t="n">
         <v>10839643</v>
       </c>
-      <c r="AA6" s="12" t="n">
+      <c r="AA6" s="11" t="n">
         <v>9514558</v>
       </c>
-      <c r="AB6" s="12" t="n">
+      <c r="AB6" s="11" t="n">
         <v>8289512.9609</v>
       </c>
-      <c r="AC6" s="12" t="n">
+      <c r="AC6" s="11" t="n">
         <v>2428801.8993</v>
       </c>
-      <c r="AD6" s="12" t="n">
+      <c r="AD6" s="11" t="n">
         <v>12999374.5786</v>
       </c>
-      <c r="AE6" s="12" t="n">
+      <c r="AE6" s="11" t="n">
         <v>7356479.6724</v>
       </c>
-      <c r="AF6" s="12" t="n">
+      <c r="AF6" s="11" t="n">
         <v>43075509.1357</v>
       </c>
-      <c r="AG6" s="12" t="n">
+      <c r="AG6" s="11" t="n">
         <v>87192496.1457</v>
       </c>
-      <c r="AH6" s="12" t="n">
+      <c r="AH6" s="11" t="n">
         <v>12938649.4147</v>
       </c>
-      <c r="AI6" s="12" t="n">
+      <c r="AI6" s="11" t="n">
         <v>5403572.64</v>
       </c>
-      <c r="AJ6" s="12" t="n">
+      <c r="AJ6" s="11" t="n">
         <v>5997226.77</v>
       </c>
-      <c r="AK6" s="12" t="n">
+      <c r="AK6" s="11" t="n">
         <v>-772462</v>
       </c>
-      <c r="AL6" s="12" t="n">
+      <c r="AL6" s="11" t="n">
         <v>258122.3294</v>
       </c>
-      <c r="AM6" s="12" t="n">
+      <c r="AM6" s="11" t="n">
         <v>193613.6213</v>
       </c>
-      <c r="AN6" s="12" t="n">
+      <c r="AN6" s="11" t="n">
         <v>747839.6429</v>
       </c>
-      <c r="AO6" s="12" t="n">
+      <c r="AO6" s="11" t="n">
         <v>22335.49</v>
       </c>
-      <c r="AP6" s="12" t="n">
+      <c r="AP6" s="11" t="n">
         <v>38584082.5823</v>
       </c>
-      <c r="AQ6" s="12" t="n">
+      <c r="AQ6" s="11" t="n">
         <v>39509341.5172</v>
       </c>
-      <c r="AR6" s="12" t="n">
+      <c r="AR6" s="11" t="n">
         <v>-16791803.1998</v>
       </c>
-      <c r="AS6" s="12" t="n">
+      <c r="AS6" s="11" t="n">
         <v>-3614290.3764</v>
       </c>
-      <c r="AT6" s="12"/>
-      <c r="AU6" s="12"/>
+      <c r="AT6" s="11"/>
+      <c r="AU6" s="11"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -3566,110 +3569,110 @@
       <c r="K7" t="s">
         <v>433</v>
       </c>
-      <c r="L7" s="12" t="str">
+      <c r="L7" s="11" t="str">
         <f>Sum(L2:L6)</f>
       </c>
-      <c r="M7" s="12" t="str">
+      <c r="M7" s="11" t="str">
         <f>Sum(M2:M6)</f>
       </c>
-      <c r="N7" s="12" t="str">
+      <c r="N7" s="11" t="str">
         <f>Sum(N2:N6)</f>
       </c>
-      <c r="O7" s="12" t="str">
+      <c r="O7" s="11" t="str">
         <f>Sum(O2:O6)</f>
       </c>
-      <c r="P7" s="12" t="str">
+      <c r="P7" s="11" t="str">
         <f>Sum(P2:P6)</f>
       </c>
-      <c r="Q7" s="12" t="str">
+      <c r="Q7" s="11" t="str">
         <f>Sum(Q2:Q6)</f>
       </c>
-      <c r="R7" s="12" t="str">
+      <c r="R7" s="11" t="str">
         <f>Sum(R2:R6)</f>
       </c>
-      <c r="S7" s="12" t="str">
+      <c r="S7" s="11" t="str">
         <f>Sum(S2:S6)</f>
       </c>
-      <c r="T7" s="12" t="str">
+      <c r="T7" s="11" t="str">
         <f>Sum(T2:T6)</f>
       </c>
-      <c r="U7" s="12" t="str">
+      <c r="U7" s="11" t="str">
         <f>Sum(U2:U6)</f>
       </c>
-      <c r="V7" s="12" t="str">
+      <c r="V7" s="11" t="str">
         <f>Sum(V2:V6)</f>
       </c>
-      <c r="W7" s="12" t="str">
+      <c r="W7" s="11" t="str">
         <f>Sum(W2:W6)</f>
       </c>
-      <c r="X7" s="12" t="str">
+      <c r="X7" s="11" t="str">
         <f>Sum(X2:X6)</f>
       </c>
-      <c r="Y7" s="12" t="str">
+      <c r="Y7" s="11" t="str">
         <f>Sum(Y2:Y6)</f>
       </c>
-      <c r="Z7" s="12" t="str">
+      <c r="Z7" s="11" t="str">
         <f>Sum(Z2:Z6)</f>
       </c>
-      <c r="AA7" s="12" t="str">
+      <c r="AA7" s="11" t="str">
         <f>Sum(AA2:AA6)</f>
       </c>
-      <c r="AB7" s="12" t="str">
+      <c r="AB7" s="11" t="str">
         <f>Sum(AB2:AB6)</f>
       </c>
-      <c r="AC7" s="12" t="str">
+      <c r="AC7" s="11" t="str">
         <f>Sum(AC2:AC6)</f>
       </c>
-      <c r="AD7" s="12" t="str">
+      <c r="AD7" s="11" t="str">
         <f>Sum(AD2:AD6)</f>
       </c>
-      <c r="AE7" s="12" t="str">
+      <c r="AE7" s="11" t="str">
         <f>Sum(AE2:AE6)</f>
       </c>
-      <c r="AF7" s="12" t="str">
+      <c r="AF7" s="11" t="str">
         <f>Sum(AF2:AF6)</f>
       </c>
-      <c r="AG7" s="12" t="str">
+      <c r="AG7" s="11" t="str">
         <f>Sum(AG2:AG6)</f>
       </c>
-      <c r="AH7" s="12" t="str">
+      <c r="AH7" s="11" t="str">
         <f>Sum(AH2:AH6)</f>
       </c>
-      <c r="AI7" s="12" t="str">
+      <c r="AI7" s="11" t="str">
         <f>Sum(AI2:AI6)</f>
       </c>
-      <c r="AJ7" s="12" t="str">
+      <c r="AJ7" s="11" t="str">
         <f>Sum(AJ2:AJ6)</f>
       </c>
-      <c r="AK7" s="12" t="str">
+      <c r="AK7" s="11" t="str">
         <f>Sum(AK2:AK6)</f>
       </c>
-      <c r="AL7" s="12" t="str">
+      <c r="AL7" s="11" t="str">
         <f>Sum(AL2:AL6)</f>
       </c>
-      <c r="AM7" s="12" t="str">
+      <c r="AM7" s="11" t="str">
         <f>Sum(AM2:AM6)</f>
       </c>
-      <c r="AN7" s="12" t="str">
+      <c r="AN7" s="11" t="str">
         <f>Sum(AN2:AN6)</f>
       </c>
-      <c r="AO7" s="12" t="str">
+      <c r="AO7" s="11" t="str">
         <f>Sum(AO2:AO6)</f>
       </c>
-      <c r="AP7" s="12" t="str">
+      <c r="AP7" s="11" t="str">
         <f>Sum(AP2:AP6)</f>
       </c>
-      <c r="AQ7" s="12" t="str">
+      <c r="AQ7" s="11" t="str">
         <f>Sum(AQ2:AQ6)</f>
       </c>
-      <c r="AR7" s="12" t="str">
+      <c r="AR7" s="11" t="str">
         <f>Sum(AR2:AR6)</f>
       </c>
-      <c r="AS7" s="12" t="str">
+      <c r="AS7" s="11" t="str">
         <f>Sum(AS2:AS6)</f>
       </c>
-      <c r="AT7" s="12"/>
-      <c r="AU7" s="12"/>
+      <c r="AT7" s="11"/>
+      <c r="AU7" s="11"/>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -3788,110 +3791,110 @@
       <c r="K11" t="s">
         <v>436</v>
       </c>
-      <c r="L11" s="12" t="n">
+      <c r="L11" s="11" t="n">
         <v>31436118395.1327</v>
       </c>
-      <c r="M11" s="12" t="n">
+      <c r="M11" s="11" t="n">
         <v>31616331571.1648</v>
       </c>
-      <c r="N11" s="12" t="n">
+      <c r="N11" s="11" t="n">
         <v>32923512156.9912</v>
       </c>
-      <c r="O11" s="12" t="n">
+      <c r="O11" s="11" t="n">
         <v>30602239813.9578</v>
       </c>
-      <c r="P11" s="12" t="n">
+      <c r="P11" s="11" t="n">
         <v>32146194646.9395</v>
       </c>
-      <c r="Q11" s="12" t="n">
+      <c r="Q11" s="11" t="n">
         <v>27467516220.636</v>
       </c>
-      <c r="R11" s="12" t="n">
+      <c r="R11" s="11" t="n">
         <v>31152996440.5949</v>
       </c>
-      <c r="S11" s="12" t="n">
+      <c r="S11" s="11" t="n">
         <v>25911792877.6674</v>
       </c>
-      <c r="T11" s="12" t="n">
+      <c r="T11" s="11" t="n">
         <v>26874357349.5353</v>
       </c>
-      <c r="U11" s="12" t="n">
+      <c r="U11" s="11" t="n">
         <v>27900370403.7562</v>
       </c>
-      <c r="V11" s="12" t="n">
+      <c r="V11" s="11" t="n">
         <v>33482251754.7515</v>
       </c>
-      <c r="W11" s="12" t="n">
+      <c r="W11" s="11" t="n">
         <v>34328010348.5177</v>
       </c>
-      <c r="X11" s="12" t="n">
+      <c r="X11" s="11" t="n">
         <v>37210895841.8614</v>
       </c>
-      <c r="Y11" s="12" t="n">
+      <c r="Y11" s="11" t="n">
         <v>47446533343.2913</v>
       </c>
-      <c r="Z11" s="12" t="n">
+      <c r="Z11" s="11" t="n">
         <v>42546861151.7535</v>
       </c>
-      <c r="AA11" s="12" t="n">
+      <c r="AA11" s="11" t="n">
         <v>37604249002.4484</v>
       </c>
-      <c r="AB11" s="12" t="n">
+      <c r="AB11" s="11" t="n">
         <v>45653461671.3302</v>
       </c>
-      <c r="AC11" s="12" t="n">
+      <c r="AC11" s="11" t="n">
         <v>50833054298.9511</v>
       </c>
-      <c r="AD11" s="12" t="n">
+      <c r="AD11" s="11" t="n">
         <v>50746091650.8019</v>
       </c>
-      <c r="AE11" s="12" t="n">
+      <c r="AE11" s="11" t="n">
         <v>50754581721.6693</v>
       </c>
-      <c r="AF11" s="12" t="n">
+      <c r="AF11" s="11" t="n">
         <v>46223217046.162</v>
       </c>
-      <c r="AG11" s="12" t="n">
+      <c r="AG11" s="11" t="n">
         <v>52051125133.2889</v>
       </c>
-      <c r="AH11" s="12" t="n">
+      <c r="AH11" s="11" t="n">
         <v>59986201803.0229</v>
       </c>
-      <c r="AI11" s="12" t="n">
+      <c r="AI11" s="11" t="n">
         <v>57492896265.4901</v>
       </c>
-      <c r="AJ11" s="12" t="n">
+      <c r="AJ11" s="11" t="n">
         <v>40360692632.6568</v>
       </c>
-      <c r="AK11" s="12" t="n">
+      <c r="AK11" s="11" t="n">
         <v>43457281402.5501</v>
       </c>
-      <c r="AL11" s="12" t="n">
+      <c r="AL11" s="11" t="n">
         <v>61582908932.5348</v>
       </c>
-      <c r="AM11" s="12" t="n">
+      <c r="AM11" s="11" t="n">
         <v>72104558114.7893</v>
       </c>
-      <c r="AN11" s="12" t="n">
+      <c r="AN11" s="11" t="n">
         <v>61162093442.9488</v>
       </c>
-      <c r="AO11" s="12" t="n">
+      <c r="AO11" s="11" t="n">
         <v>61858979933.9347</v>
       </c>
-      <c r="AP11" s="12" t="n">
+      <c r="AP11" s="11" t="n">
         <v>82523915567.4511</v>
       </c>
-      <c r="AQ11" s="12" t="n">
+      <c r="AQ11" s="11" t="n">
         <v>54519799186.0998</v>
       </c>
-      <c r="AR11" s="12" t="n">
+      <c r="AR11" s="11" t="n">
         <v>53457678478.0773</v>
       </c>
-      <c r="AS11" s="12" t="n">
+      <c r="AS11" s="11" t="n">
         <v>37541206218.5418</v>
       </c>
-      <c r="AT11" s="12"/>
-      <c r="AU11" s="12"/>
+      <c r="AT11" s="11"/>
+      <c r="AU11" s="11"/>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -3900,110 +3903,110 @@
       <c r="K12" t="s">
         <v>437</v>
       </c>
-      <c r="L12" s="12" t="n">
+      <c r="L12" s="11" t="n">
         <v>20216278905.9163</v>
       </c>
-      <c r="M12" s="12" t="n">
+      <c r="M12" s="11" t="n">
         <v>15861369437.3966</v>
       </c>
-      <c r="N12" s="12" t="n">
+      <c r="N12" s="11" t="n">
         <v>15218404059.1175</v>
       </c>
-      <c r="O12" s="12" t="n">
+      <c r="O12" s="11" t="n">
         <v>15492870741.2222</v>
       </c>
-      <c r="P12" s="12" t="n">
+      <c r="P12" s="11" t="n">
         <v>14516890782.8589</v>
       </c>
-      <c r="Q12" s="12" t="n">
+      <c r="Q12" s="11" t="n">
         <v>12214807398.489</v>
       </c>
-      <c r="R12" s="12" t="n">
+      <c r="R12" s="11" t="n">
         <v>12271435448.658</v>
       </c>
-      <c r="S12" s="12" t="n">
+      <c r="S12" s="11" t="n">
         <v>10995125830.9958</v>
       </c>
-      <c r="T12" s="12" t="n">
+      <c r="T12" s="11" t="n">
         <v>11670386427.786</v>
       </c>
-      <c r="U12" s="12" t="n">
+      <c r="U12" s="11" t="n">
         <v>11517241459.7886</v>
       </c>
-      <c r="V12" s="12" t="n">
+      <c r="V12" s="11" t="n">
         <v>14685143267.7206</v>
       </c>
-      <c r="W12" s="12" t="n">
+      <c r="W12" s="11" t="n">
         <v>14514919402.523</v>
       </c>
-      <c r="X12" s="12" t="n">
+      <c r="X12" s="11" t="n">
         <v>14836845675.9689</v>
       </c>
-      <c r="Y12" s="12" t="n">
+      <c r="Y12" s="11" t="n">
         <v>19772881160.8144</v>
       </c>
-      <c r="Z12" s="12" t="n">
+      <c r="Z12" s="11" t="n">
         <v>20134314729.8572</v>
       </c>
-      <c r="AA12" s="12" t="n">
+      <c r="AA12" s="11" t="n">
         <v>21121992591.6693</v>
       </c>
-      <c r="AB12" s="12" t="n">
+      <c r="AB12" s="11" t="n">
         <v>20899266799.2592</v>
       </c>
-      <c r="AC12" s="12" t="n">
+      <c r="AC12" s="11" t="n">
         <v>22772809658.5017</v>
       </c>
-      <c r="AD12" s="12" t="n">
+      <c r="AD12" s="11" t="n">
         <v>28376039656.831</v>
       </c>
-      <c r="AE12" s="12" t="n">
+      <c r="AE12" s="11" t="n">
         <v>26087966960.8847</v>
       </c>
-      <c r="AF12" s="12" t="n">
+      <c r="AF12" s="11" t="n">
         <v>25730975022.2731</v>
       </c>
-      <c r="AG12" s="12" t="n">
+      <c r="AG12" s="11" t="n">
         <v>26556743962.8492</v>
       </c>
-      <c r="AH12" s="12" t="n">
+      <c r="AH12" s="11" t="n">
         <v>25708198764.0857</v>
       </c>
-      <c r="AI12" s="12" t="n">
+      <c r="AI12" s="11" t="n">
         <v>21582406903.4422</v>
       </c>
-      <c r="AJ12" s="12" t="n">
+      <c r="AJ12" s="11" t="n">
         <v>20239578416.0593</v>
       </c>
-      <c r="AK12" s="12" t="n">
+      <c r="AK12" s="11" t="n">
         <v>19907385982.2002</v>
       </c>
-      <c r="AL12" s="12" t="n">
+      <c r="AL12" s="11" t="n">
         <v>17447316279.2693</v>
       </c>
-      <c r="AM12" s="12" t="n">
+      <c r="AM12" s="11" t="n">
         <v>15709919813.1568</v>
       </c>
-      <c r="AN12" s="12" t="n">
+      <c r="AN12" s="11" t="n">
         <v>19883845964.3556</v>
       </c>
-      <c r="AO12" s="12" t="n">
+      <c r="AO12" s="11" t="n">
         <v>23189966737.2488</v>
       </c>
-      <c r="AP12" s="12" t="n">
+      <c r="AP12" s="11" t="n">
         <v>19866735039.648</v>
       </c>
-      <c r="AQ12" s="12" t="n">
+      <c r="AQ12" s="11" t="n">
         <v>11005994118.1723</v>
       </c>
-      <c r="AR12" s="12" t="n">
+      <c r="AR12" s="11" t="n">
         <v>9796794669.8747</v>
       </c>
-      <c r="AS12" s="12" t="n">
+      <c r="AS12" s="11" t="n">
         <v>5013905756.9871</v>
       </c>
-      <c r="AT12" s="12"/>
-      <c r="AU12" s="12"/>
+      <c r="AT12" s="11"/>
+      <c r="AU12" s="11"/>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -4012,110 +4015,110 @@
       <c r="K13" t="s">
         <v>438</v>
       </c>
-      <c r="L13" s="12" t="n">
+      <c r="L13" s="11" t="n">
         <v>5652125593.55866</v>
       </c>
-      <c r="M13" s="12" t="n">
+      <c r="M13" s="11" t="n">
         <v>7879771345.35619</v>
       </c>
-      <c r="N13" s="12" t="n">
+      <c r="N13" s="11" t="n">
         <v>6163577716.98047</v>
       </c>
-      <c r="O13" s="12" t="n">
+      <c r="O13" s="11" t="n">
         <v>5984890865.90452</v>
       </c>
-      <c r="P13" s="12" t="n">
+      <c r="P13" s="11" t="n">
         <v>5160864908.29358</v>
       </c>
-      <c r="Q13" s="12" t="n">
+      <c r="Q13" s="11" t="n">
         <v>4800881785.94834</v>
       </c>
-      <c r="R13" s="12" t="n">
+      <c r="R13" s="11" t="n">
         <v>3505510716.93641</v>
       </c>
-      <c r="S13" s="12" t="n">
+      <c r="S13" s="11" t="n">
         <v>3213475374.32511</v>
       </c>
-      <c r="T13" s="12" t="n">
+      <c r="T13" s="11" t="n">
         <v>3583382897.08349</v>
       </c>
-      <c r="U13" s="12" t="n">
+      <c r="U13" s="11" t="n">
         <v>3514484912.28958</v>
       </c>
-      <c r="V13" s="12" t="n">
+      <c r="V13" s="11" t="n">
         <v>5449133103.46988</v>
       </c>
-      <c r="W13" s="12" t="n">
+      <c r="W13" s="11" t="n">
         <v>4976587272.98747</v>
       </c>
-      <c r="X13" s="12" t="n">
+      <c r="X13" s="11" t="n">
         <v>4745464375.80455</v>
       </c>
-      <c r="Y13" s="12" t="n">
+      <c r="Y13" s="11" t="n">
         <v>3915295071.68206</v>
       </c>
-      <c r="Z13" s="12" t="n">
+      <c r="Z13" s="11" t="n">
         <v>4589326635.70716</v>
       </c>
-      <c r="AA13" s="12" t="n">
+      <c r="AA13" s="11" t="n">
         <v>5211908205.88291</v>
       </c>
-      <c r="AB13" s="12" t="n">
+      <c r="AB13" s="11" t="n">
         <v>4924487831.60221</v>
       </c>
-      <c r="AC13" s="12" t="n">
+      <c r="AC13" s="11" t="n">
         <v>4623811466.14096</v>
       </c>
-      <c r="AD13" s="12" t="n">
+      <c r="AD13" s="11" t="n">
         <v>5226995032.08363</v>
       </c>
-      <c r="AE13" s="12" t="n">
+      <c r="AE13" s="11" t="n">
         <v>5645823980.66227</v>
       </c>
-      <c r="AF13" s="12" t="n">
+      <c r="AF13" s="11" t="n">
         <v>6612343398.76085</v>
       </c>
-      <c r="AG13" s="12" t="n">
+      <c r="AG13" s="11" t="n">
         <v>7171189894.81987</v>
       </c>
-      <c r="AH13" s="12" t="n">
+      <c r="AH13" s="11" t="n">
         <v>8356573064.96038</v>
       </c>
-      <c r="AI13" s="12" t="n">
+      <c r="AI13" s="11" t="n">
         <v>7318864828.31543</v>
       </c>
-      <c r="AJ13" s="12" t="n">
+      <c r="AJ13" s="11" t="n">
         <v>5840405474.28447</v>
       </c>
-      <c r="AK13" s="12" t="n">
+      <c r="AK13" s="11" t="n">
         <v>6450148124.69779</v>
       </c>
-      <c r="AL13" s="12" t="n">
+      <c r="AL13" s="11" t="n">
         <v>6173092080.07672</v>
       </c>
-      <c r="AM13" s="12" t="n">
+      <c r="AM13" s="11" t="n">
         <v>7877185128.24294</v>
       </c>
-      <c r="AN13" s="12" t="n">
+      <c r="AN13" s="11" t="n">
         <v>8592400924.41219</v>
       </c>
-      <c r="AO13" s="12" t="n">
+      <c r="AO13" s="11" t="n">
         <v>10250128195.2892</v>
       </c>
-      <c r="AP13" s="12" t="n">
+      <c r="AP13" s="11" t="n">
         <v>9509382491.58073</v>
       </c>
-      <c r="AQ13" s="12" t="n">
+      <c r="AQ13" s="11" t="n">
         <v>8073337774.27088</v>
       </c>
-      <c r="AR13" s="12" t="n">
+      <c r="AR13" s="11" t="n">
         <v>8137614778.7914</v>
       </c>
-      <c r="AS13" s="12" t="n">
+      <c r="AS13" s="11" t="n">
         <v>4171636498.08103</v>
       </c>
-      <c r="AT13" s="12"/>
-      <c r="AU13" s="12"/>
+      <c r="AT13" s="11"/>
+      <c r="AU13" s="11"/>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -4124,110 +4127,110 @@
       <c r="K14" t="s">
         <v>439</v>
       </c>
-      <c r="L14" s="12" t="n">
+      <c r="L14" s="11" t="n">
         <v>1720722792.96411</v>
       </c>
-      <c r="M14" s="12" t="n">
+      <c r="M14" s="11" t="n">
         <v>2639861140.70039</v>
       </c>
-      <c r="N14" s="12" t="n">
+      <c r="N14" s="11" t="n">
         <v>1845538120.92631</v>
       </c>
-      <c r="O14" s="12" t="n">
+      <c r="O14" s="11" t="n">
         <v>1964759257.78585</v>
       </c>
-      <c r="P14" s="12" t="n">
+      <c r="P14" s="11" t="n">
         <v>1910888750.67024</v>
       </c>
-      <c r="Q14" s="12" t="n">
+      <c r="Q14" s="11" t="n">
         <v>1964576110.15298</v>
       </c>
-      <c r="R14" s="12" t="n">
+      <c r="R14" s="11" t="n">
         <v>2098063781.85174</v>
       </c>
-      <c r="S14" s="12" t="n">
+      <c r="S14" s="11" t="n">
         <v>2020289221.74683</v>
       </c>
-      <c r="T14" s="12" t="n">
+      <c r="T14" s="11" t="n">
         <v>2121284849.57863</v>
       </c>
-      <c r="U14" s="12" t="n">
+      <c r="U14" s="11" t="n">
         <v>2497336523.59519</v>
       </c>
-      <c r="V14" s="12" t="n">
+      <c r="V14" s="11" t="n">
         <v>3584378858.51483</v>
       </c>
-      <c r="W14" s="12" t="n">
+      <c r="W14" s="11" t="n">
         <v>3161680066.74079</v>
       </c>
-      <c r="X14" s="12" t="n">
+      <c r="X14" s="11" t="n">
         <v>3811844034.42064</v>
       </c>
-      <c r="Y14" s="12" t="n">
+      <c r="Y14" s="11" t="n">
         <v>3899691655.91843</v>
       </c>
-      <c r="Z14" s="12" t="n">
+      <c r="Z14" s="11" t="n">
         <v>3818048870.41207</v>
       </c>
-      <c r="AA14" s="12" t="n">
+      <c r="AA14" s="11" t="n">
         <v>4307860633.99283</v>
       </c>
-      <c r="AB14" s="12" t="n">
+      <c r="AB14" s="11" t="n">
         <v>3972691717.41501</v>
       </c>
-      <c r="AC14" s="12" t="n">
+      <c r="AC14" s="11" t="n">
         <v>4071855713.24882</v>
       </c>
-      <c r="AD14" s="12" t="n">
+      <c r="AD14" s="11" t="n">
         <v>4581336061.17589</v>
       </c>
-      <c r="AE14" s="12" t="n">
+      <c r="AE14" s="11" t="n">
         <v>4397512331.22106</v>
       </c>
-      <c r="AF14" s="12" t="n">
+      <c r="AF14" s="11" t="n">
         <v>4583784239.20495</v>
       </c>
-      <c r="AG14" s="12" t="n">
+      <c r="AG14" s="11" t="n">
         <v>4264226954.95396</v>
       </c>
-      <c r="AH14" s="12" t="n">
+      <c r="AH14" s="11" t="n">
         <v>4364794720.42454</v>
       </c>
-      <c r="AI14" s="12" t="n">
+      <c r="AI14" s="11" t="n">
         <v>4195919981.50873</v>
       </c>
-      <c r="AJ14" s="12" t="n">
+      <c r="AJ14" s="11" t="n">
         <v>4187426103.60618</v>
       </c>
-      <c r="AK14" s="12" t="n">
+      <c r="AK14" s="11" t="n">
         <v>4183821772.03747</v>
       </c>
-      <c r="AL14" s="12" t="n">
+      <c r="AL14" s="11" t="n">
         <v>4427392971.56215</v>
       </c>
-      <c r="AM14" s="12" t="n">
+      <c r="AM14" s="11" t="n">
         <v>4610971634.91706</v>
       </c>
-      <c r="AN14" s="12" t="n">
+      <c r="AN14" s="11" t="n">
         <v>5526318144.60018</v>
       </c>
-      <c r="AO14" s="12" t="n">
+      <c r="AO14" s="11" t="n">
         <v>5596974139.60251</v>
       </c>
-      <c r="AP14" s="12" t="n">
+      <c r="AP14" s="11" t="n">
         <v>4449664638.87698</v>
       </c>
-      <c r="AQ14" s="12" t="n">
+      <c r="AQ14" s="11" t="n">
         <v>3876410832.70434</v>
       </c>
-      <c r="AR14" s="12" t="n">
+      <c r="AR14" s="11" t="n">
         <v>3755209682.6872</v>
       </c>
-      <c r="AS14" s="12" t="n">
+      <c r="AS14" s="11" t="n">
         <v>1204007830.8188</v>
       </c>
-      <c r="AT14" s="12"/>
-      <c r="AU14" s="12"/>
+      <c r="AT14" s="11"/>
+      <c r="AU14" s="11"/>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -4236,151 +4239,151 @@
       <c r="K15" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="12" t="n">
+      <c r="L15" s="11" t="n">
         <v>2548973458.5293</v>
       </c>
-      <c r="M15" s="12" t="n">
+      <c r="M15" s="11" t="n">
         <v>559731307.829819</v>
       </c>
-      <c r="N15" s="12" t="n">
+      <c r="N15" s="11" t="n">
         <v>650347010.543314</v>
       </c>
-      <c r="O15" s="12" t="n">
+      <c r="O15" s="11" t="n">
         <v>684748220.727455</v>
       </c>
-      <c r="P15" s="12" t="n">
+      <c r="P15" s="11" t="n">
         <v>953513513.418676</v>
       </c>
-      <c r="Q15" s="12" t="n">
+      <c r="Q15" s="11" t="n">
         <v>564282859.277974</v>
       </c>
-      <c r="R15" s="12" t="n">
+      <c r="R15" s="11" t="n">
         <v>628140937.9995</v>
       </c>
-      <c r="S15" s="12" t="n">
+      <c r="S15" s="11" t="n">
         <v>12108235.4349743</v>
       </c>
-      <c r="T15" s="12" t="n">
+      <c r="T15" s="11" t="n">
         <v>53650991.0819584</v>
       </c>
-      <c r="U15" s="12" t="n">
+      <c r="U15" s="11" t="n">
         <v>3297099.75639217</v>
       </c>
-      <c r="V15" s="12" t="n">
+      <c r="V15" s="11" t="n">
         <v>28797599.3870696</v>
       </c>
-      <c r="W15" s="12" t="n">
+      <c r="W15" s="11" t="n">
         <v>189297.256776088</v>
       </c>
-      <c r="X15" s="12" t="n">
+      <c r="X15" s="11" t="n">
         <v>823452.372052593</v>
       </c>
-      <c r="Y15" s="12" t="n">
+      <c r="Y15" s="11" t="n">
         <v>7048369.45701824</v>
       </c>
-      <c r="Z15" s="12" t="n">
+      <c r="Z15" s="11" t="n">
         <v>16123744.8928327</v>
       </c>
-      <c r="AA15" s="12" t="n">
+      <c r="AA15" s="11" t="n">
         <v>13735736.4334502</v>
       </c>
-      <c r="AB15" s="12" t="n">
+      <c r="AB15" s="11" t="n">
         <v>11589856.4075731</v>
       </c>
-      <c r="AC15" s="12" t="n">
+      <c r="AC15" s="11" t="n">
         <v>3305154.7779856</v>
       </c>
-      <c r="AD15" s="12" t="n">
+      <c r="AD15" s="11" t="n">
         <v>17328371.334887</v>
       </c>
-      <c r="AE15" s="12" t="n">
+      <c r="AE15" s="11" t="n">
         <v>9707654.6758385</v>
       </c>
-      <c r="AF15" s="12" t="n">
+      <c r="AF15" s="11" t="n">
         <v>56352574.9358821</v>
       </c>
-      <c r="AG15" s="12" t="n">
+      <c r="AG15" s="11" t="n">
         <v>111814165.321835</v>
       </c>
-      <c r="AH15" s="12" t="n">
+      <c r="AH15" s="11" t="n">
         <v>16293641.2048229</v>
       </c>
-      <c r="AI15" s="12" t="n">
+      <c r="AI15" s="11" t="n">
         <v>6682430.54357936</v>
       </c>
-      <c r="AJ15" s="12" t="n">
+      <c r="AJ15" s="11" t="n">
         <v>7275826.27459085</v>
       </c>
-      <c r="AK15" s="12" t="n">
+      <c r="AK15" s="11" t="n">
         <v>-926527.666558336</v>
       </c>
-      <c r="AL15" s="12" t="n">
+      <c r="AL15" s="11" t="n">
         <v>307059.74833909</v>
       </c>
-      <c r="AM15" s="12" t="n">
+      <c r="AM15" s="11" t="n">
         <v>226280.866287418</v>
       </c>
-      <c r="AN15" s="12" t="n">
+      <c r="AN15" s="11" t="n">
         <v>853966.686803477</v>
       </c>
-      <c r="AO15" s="12" t="n">
+      <c r="AO15" s="11" t="n">
         <v>25015.1926022016</v>
       </c>
-      <c r="AP15" s="12" t="n">
+      <c r="AP15" s="11" t="n">
         <v>42644317.3796793</v>
       </c>
-      <c r="AQ15" s="12" t="n">
+      <c r="AQ15" s="11" t="n">
         <v>42246848.7679694</v>
       </c>
-      <c r="AR15" s="12" t="n">
+      <c r="AR15" s="11" t="n">
         <v>-16791803.1998</v>
       </c>
-      <c r="AS15" s="12" t="n">
+      <c r="AS15" s="11" t="n">
         <v>-3447304.30381899</v>
       </c>
-      <c r="AT15" s="12"/>
-      <c r="AU15" s="12"/>
+      <c r="AT15" s="11"/>
+      <c r="AU15" s="11"/>
     </row>
     <row r="16">
       <c r="A16" t="str">
         <f>K16</f>
       </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="12"/>
-      <c r="AD16" s="12"/>
-      <c r="AE16" s="12"/>
-      <c r="AF16" s="12"/>
-      <c r="AG16" s="12"/>
-      <c r="AH16" s="12"/>
-      <c r="AI16" s="12"/>
-      <c r="AJ16" s="12"/>
-      <c r="AK16" s="12"/>
-      <c r="AL16" s="12"/>
-      <c r="AM16" s="12"/>
-      <c r="AN16" s="12"/>
-      <c r="AO16" s="12"/>
-      <c r="AP16" s="12"/>
-      <c r="AQ16" s="12"/>
-      <c r="AR16" s="12"/>
-      <c r="AS16" s="12"/>
-      <c r="AT16" s="12"/>
-      <c r="AU16" s="12"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="11"/>
+      <c r="AM16" s="11"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="11"/>
+      <c r="AP16" s="11"/>
+      <c r="AQ16" s="11"/>
+      <c r="AR16" s="11"/>
+      <c r="AS16" s="11"/>
+      <c r="AT16" s="11"/>
+      <c r="AU16" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6422,94 +6425,94 @@
         <v>50</v>
       </c>
       <c r="N2" t="s">
-        <v>50</v>
+        <v>440</v>
       </c>
       <c r="O2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3" t="n">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12" t="n">
         <v>18435016803.53</v>
       </c>
-      <c r="AA2" s="3" t="n">
-        <v>20134411773.9394</v>
-      </c>
-      <c r="AB2" s="3" t="n">
-        <v>23443985015.1086</v>
-      </c>
-      <c r="AC2" s="3" t="n">
-        <v>26676816872.291</v>
-      </c>
-      <c r="AD2" s="3" t="n">
-        <v>24470273562.3805</v>
-      </c>
-      <c r="AE2" s="3" t="n">
-        <v>20123779793.9688</v>
-      </c>
-      <c r="AF2" s="3" t="n">
-        <v>26830244851.705</v>
-      </c>
-      <c r="AG2" s="3" t="n">
-        <v>29080544499.0824</v>
-      </c>
-      <c r="AH2" s="3" t="n">
-        <v>29161554168.2414</v>
-      </c>
-      <c r="AI2" s="3" t="n">
-        <v>30233862099.7959</v>
-      </c>
-      <c r="AJ2" s="3" t="n">
+      <c r="AA2" s="12" t="n">
+        <v>20134164854.9257</v>
+      </c>
+      <c r="AB2" s="12" t="n">
+        <v>23443925260.1051</v>
+      </c>
+      <c r="AC2" s="12" t="n">
+        <v>26676816790.2912</v>
+      </c>
+      <c r="AD2" s="12" t="n">
+        <v>24470273590.4286</v>
+      </c>
+      <c r="AE2" s="12" t="n">
+        <v>20123779781.3259</v>
+      </c>
+      <c r="AF2" s="12" t="n">
+        <v>26830244884.6484</v>
+      </c>
+      <c r="AG2" s="12" t="n">
+        <v>29080544537.5695</v>
+      </c>
+      <c r="AH2" s="12" t="n">
+        <v>29161554123.4792</v>
+      </c>
+      <c r="AI2" s="12" t="n">
+        <v>30233862074.6934</v>
+      </c>
+      <c r="AJ2" s="12" t="n">
         <v>31789053337.2932</v>
       </c>
-      <c r="AK2" s="3" t="n">
+      <c r="AK2" s="12" t="n">
         <v>34378699278.0285</v>
       </c>
-      <c r="AL2" s="3" t="n">
+      <c r="AL2" s="12" t="n">
         <v>34050154491.8631</v>
       </c>
-      <c r="AM2" s="3" t="n">
+      <c r="AM2" s="12" t="n">
         <v>31952800826.7103</v>
       </c>
-      <c r="AN2" s="3" t="n">
+      <c r="AN2" s="12" t="n">
         <v>27283316572.8348</v>
       </c>
-      <c r="AO2" s="3" t="n">
+      <c r="AO2" s="12" t="n">
         <v>29146173982.292</v>
       </c>
-      <c r="AP2" s="3" t="n">
+      <c r="AP2" s="12" t="n">
         <v>31958272804.3431</v>
       </c>
-      <c r="AQ2" s="3" t="n">
+      <c r="AQ2" s="12" t="n">
         <v>32431531049.45</v>
       </c>
-      <c r="AR2" s="3" t="n">
-        <v>34027991669.7538</v>
-      </c>
-      <c r="AS2" s="3" t="n">
-        <v>40923873119.6225</v>
-      </c>
-      <c r="AT2" s="3" t="n">
-        <v>42320519111.1772</v>
-      </c>
-      <c r="AU2" s="3" t="n">
-        <v>33673550260.8871</v>
-      </c>
-      <c r="AV2" s="3" t="n">
-        <v>31510444831.3847</v>
-      </c>
-      <c r="AW2" s="3" t="n">
-        <v>18023200566.2224</v>
-      </c>
-      <c r="AX2" s="3"/>
+      <c r="AR2" s="12" t="n">
+        <v>34132562684.0882</v>
+      </c>
+      <c r="AS2" s="12" t="n">
+        <v>40901341510.525</v>
+      </c>
+      <c r="AT2" s="12" t="n">
+        <v>42329966729.5582</v>
+      </c>
+      <c r="AU2" s="12" t="n">
+        <v>33705424896.8231</v>
+      </c>
+      <c r="AV2" s="12" t="n">
+        <v>31429996545.6082</v>
+      </c>
+      <c r="AW2" s="12" t="n">
+        <v>38731758499.3037</v>
+      </c>
+      <c r="AX2" s="12"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -6527,89 +6530,89 @@
       <c r="O3" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3" t="n">
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12" t="n">
         <v>817220948</v>
       </c>
-      <c r="AA3" s="3" t="n">
-        <v>1692568679</v>
-      </c>
-      <c r="AB3" s="3" t="n">
-        <v>1864446757</v>
-      </c>
-      <c r="AC3" s="3" t="n">
+      <c r="AA3" s="12" t="n">
+        <v>1692568712</v>
+      </c>
+      <c r="AB3" s="12" t="n">
+        <v>1864446769</v>
+      </c>
+      <c r="AC3" s="12" t="n">
         <v>1769819283.5</v>
       </c>
-      <c r="AD3" s="3" t="n">
-        <v>2469419338</v>
-      </c>
-      <c r="AE3" s="3" t="n">
-        <v>7650069458</v>
-      </c>
-      <c r="AF3" s="3" t="n">
-        <v>3801083671</v>
-      </c>
-      <c r="AG3" s="3" t="n">
-        <v>3742823814.9947</v>
-      </c>
-      <c r="AH3" s="3" t="n">
-        <v>7641439156.5834</v>
-      </c>
-      <c r="AI3" s="3" t="n">
-        <v>4033642041.002</v>
-      </c>
-      <c r="AJ3" s="3" t="n">
+      <c r="AD3" s="12" t="n">
+        <v>2469419357</v>
+      </c>
+      <c r="AE3" s="12" t="n">
+        <v>7650069363</v>
+      </c>
+      <c r="AF3" s="12" t="n">
+        <v>3801083704</v>
+      </c>
+      <c r="AG3" s="12" t="n">
+        <v>3742823764.8051</v>
+      </c>
+      <c r="AH3" s="12" t="n">
+        <v>7641439227.027</v>
+      </c>
+      <c r="AI3" s="12" t="n">
+        <v>4033642124.2937</v>
+      </c>
+      <c r="AJ3" s="12" t="n">
         <v>2173595141.6711</v>
       </c>
-      <c r="AK3" s="3" t="n">
+      <c r="AK3" s="12" t="n">
         <v>1205987932.4714</v>
       </c>
-      <c r="AL3" s="3" t="n">
+      <c r="AL3" s="12" t="n">
         <v>537654417.984</v>
       </c>
-      <c r="AM3" s="3" t="n">
+      <c r="AM3" s="12" t="n">
         <v>442105135.5651</v>
       </c>
-      <c r="AN3" s="3" t="n">
+      <c r="AN3" s="12" t="n">
         <v>326964605.8477</v>
       </c>
-      <c r="AO3" s="3" t="n">
+      <c r="AO3" s="12" t="n">
         <v>145025613.9339</v>
       </c>
-      <c r="AP3" s="3" t="n">
+      <c r="AP3" s="12" t="n">
         <v>145026013.4623</v>
       </c>
-      <c r="AQ3" s="3" t="n">
+      <c r="AQ3" s="12" t="n">
         <v>206504418.651</v>
       </c>
-      <c r="AR3" s="3" t="n">
-        <v>154494781.4638</v>
-      </c>
-      <c r="AS3" s="3" t="n">
-        <v>201570450.952</v>
-      </c>
-      <c r="AT3" s="3" t="n">
-        <v>504777241.0911</v>
-      </c>
-      <c r="AU3" s="3" t="n">
-        <v>448119560.1044</v>
-      </c>
-      <c r="AV3" s="3" t="n">
-        <v>382801102.4745</v>
-      </c>
-      <c r="AW3" s="3" t="n">
-        <v>173029219.3685</v>
-      </c>
-      <c r="AX3" s="3"/>
+      <c r="AR3" s="12" t="n">
+        <v>154494781.3622</v>
+      </c>
+      <c r="AS3" s="12" t="n">
+        <v>201570450.2269</v>
+      </c>
+      <c r="AT3" s="12" t="n">
+        <v>440717314.8573</v>
+      </c>
+      <c r="AU3" s="12" t="n">
+        <v>447944732.3863</v>
+      </c>
+      <c r="AV3" s="12" t="n">
+        <v>358397023.6191</v>
+      </c>
+      <c r="AW3" s="12" t="n">
+        <v>402382120.7333</v>
+      </c>
+      <c r="AX3" s="12"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -6627,89 +6630,89 @@
       <c r="O4" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3" t="n">
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12" t="n">
         <v>1384690540</v>
       </c>
-      <c r="AA4" s="3" t="n">
-        <v>1203331975</v>
-      </c>
-      <c r="AB4" s="3" t="n">
+      <c r="AA4" s="12" t="n">
+        <v>1203331976</v>
+      </c>
+      <c r="AB4" s="12" t="n">
         <v>1348497701.4375</v>
       </c>
-      <c r="AC4" s="3" t="n">
+      <c r="AC4" s="12" t="n">
         <v>1606996362.8125</v>
       </c>
-      <c r="AD4" s="3" t="n">
-        <v>1865394105.1017</v>
-      </c>
-      <c r="AE4" s="3" t="n">
-        <v>1557963564.7113</v>
-      </c>
-      <c r="AF4" s="3" t="n">
+      <c r="AD4" s="12" t="n">
+        <v>1865394104.0979</v>
+      </c>
+      <c r="AE4" s="12" t="n">
+        <v>1557963564.7013</v>
+      </c>
+      <c r="AF4" s="12" t="n">
         <v>2323071129.2168</v>
       </c>
-      <c r="AG4" s="3" t="n">
-        <v>2256608267.8543</v>
-      </c>
-      <c r="AH4" s="3" t="n">
-        <v>2431291922.565</v>
-      </c>
-      <c r="AI4" s="3" t="n">
-        <v>2219534615.0246</v>
-      </c>
-      <c r="AJ4" s="3" t="n">
+      <c r="AG4" s="12" t="n">
+        <v>2257268627.3812</v>
+      </c>
+      <c r="AH4" s="12" t="n">
+        <v>2431291921.894</v>
+      </c>
+      <c r="AI4" s="12" t="n">
+        <v>2219534613.7357</v>
+      </c>
+      <c r="AJ4" s="12" t="n">
         <v>1693435993.3834</v>
       </c>
-      <c r="AK4" s="3" t="n">
+      <c r="AK4" s="12" t="n">
         <v>1288566219.4594</v>
       </c>
-      <c r="AL4" s="3" t="n">
+      <c r="AL4" s="12" t="n">
         <v>997461313.5025</v>
       </c>
-      <c r="AM4" s="3" t="n">
+      <c r="AM4" s="12" t="n">
         <v>327648872.4866</v>
       </c>
-      <c r="AN4" s="3" t="n">
+      <c r="AN4" s="12" t="n">
         <v>166591293.8013</v>
       </c>
-      <c r="AO4" s="3" t="n">
+      <c r="AO4" s="12" t="n">
         <v>148429033.0806</v>
       </c>
-      <c r="AP4" s="3" t="n">
+      <c r="AP4" s="12" t="n">
         <v>194209912.2386</v>
       </c>
-      <c r="AQ4" s="3" t="n">
+      <c r="AQ4" s="12" t="n">
         <v>295069664.3187</v>
       </c>
-      <c r="AR4" s="3" t="n">
-        <v>222823561.9301</v>
-      </c>
-      <c r="AS4" s="3" t="n">
-        <v>247652350.2748</v>
-      </c>
-      <c r="AT4" s="3" t="n">
-        <v>335863737.457</v>
-      </c>
-      <c r="AU4" s="3" t="n">
-        <v>272697611.1137</v>
-      </c>
-      <c r="AV4" s="3" t="n">
-        <v>460093866.8452</v>
-      </c>
-      <c r="AW4" s="3" t="n">
-        <v>320525190.566</v>
-      </c>
-      <c r="AX4" s="3"/>
+      <c r="AR4" s="12" t="n">
+        <v>222823561.9128</v>
+      </c>
+      <c r="AS4" s="12" t="n">
+        <v>247652350.2745</v>
+      </c>
+      <c r="AT4" s="12" t="n">
+        <v>337371358.5994</v>
+      </c>
+      <c r="AU4" s="12" t="n">
+        <v>274197611.1081</v>
+      </c>
+      <c r="AV4" s="12" t="n">
+        <v>460093867.2378</v>
+      </c>
+      <c r="AW4" s="12" t="n">
+        <v>622231249.3476</v>
+      </c>
+      <c r="AX4" s="12"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -6727,89 +6730,89 @@
       <c r="O5" t="s">
         <v>55</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3" t="n">
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12" t="n">
         <v>1464130021</v>
       </c>
-      <c r="AA5" s="3" t="n">
-        <v>1576349336</v>
-      </c>
-      <c r="AB5" s="3" t="n">
-        <v>1241522003</v>
-      </c>
-      <c r="AC5" s="3" t="n">
+      <c r="AA5" s="12" t="n">
+        <v>1576349340</v>
+      </c>
+      <c r="AB5" s="12" t="n">
+        <v>1241522004</v>
+      </c>
+      <c r="AC5" s="12" t="n">
         <v>2225944581</v>
       </c>
-      <c r="AD5" s="3" t="n">
-        <v>2051699907</v>
-      </c>
-      <c r="AE5" s="3" t="n">
-        <v>2028172125.25</v>
-      </c>
-      <c r="AF5" s="3" t="n">
-        <v>2396926245.3267</v>
-      </c>
-      <c r="AG5" s="3" t="n">
-        <v>3715646511.6924</v>
-      </c>
-      <c r="AH5" s="3" t="n">
-        <v>7269212912.972</v>
-      </c>
-      <c r="AI5" s="3" t="n">
-        <v>7310992688.6111</v>
-      </c>
-      <c r="AJ5" s="3" t="n">
+      <c r="AD5" s="12" t="n">
+        <v>2051699918</v>
+      </c>
+      <c r="AE5" s="12" t="n">
+        <v>2028172126.25</v>
+      </c>
+      <c r="AF5" s="12" t="n">
+        <v>2396926252.3037</v>
+      </c>
+      <c r="AG5" s="12" t="n">
+        <v>3715646535.7098</v>
+      </c>
+      <c r="AH5" s="12" t="n">
+        <v>7269212899.239</v>
+      </c>
+      <c r="AI5" s="12" t="n">
+        <v>7310992725.8812</v>
+      </c>
+      <c r="AJ5" s="12" t="n">
         <v>8537934854.7812</v>
       </c>
-      <c r="AK5" s="3" t="n">
+      <c r="AK5" s="12" t="n">
         <v>17101059147.4311</v>
       </c>
-      <c r="AL5" s="3" t="n">
+      <c r="AL5" s="12" t="n">
         <v>15524971275.5827</v>
       </c>
-      <c r="AM5" s="3" t="n">
+      <c r="AM5" s="12" t="n">
         <v>19130825933.2869</v>
       </c>
-      <c r="AN5" s="3" t="n">
+      <c r="AN5" s="12" t="n">
         <v>15849272506.0343</v>
       </c>
-      <c r="AO5" s="3" t="n">
+      <c r="AO5" s="12" t="n">
         <v>18512220879.8149</v>
       </c>
-      <c r="AP5" s="3" t="n">
+      <c r="AP5" s="12" t="n">
         <v>16561678209.8346</v>
       </c>
-      <c r="AQ5" s="3" t="n">
+      <c r="AQ5" s="12" t="n">
         <v>13923592758.2565</v>
       </c>
-      <c r="AR5" s="3" t="n">
-        <v>16831828314.585</v>
-      </c>
-      <c r="AS5" s="3" t="n">
-        <v>20862956016.424</v>
-      </c>
-      <c r="AT5" s="3" t="n">
-        <v>16353377329.7241</v>
-      </c>
-      <c r="AU5" s="3" t="n">
-        <v>17726249512.3628</v>
-      </c>
-      <c r="AV5" s="3" t="n">
-        <v>14287090543.2938</v>
-      </c>
-      <c r="AW5" s="3" t="n">
-        <v>19427349347.59</v>
-      </c>
-      <c r="AX5" s="3"/>
+      <c r="AR5" s="12" t="n">
+        <v>16823330790.1993</v>
+      </c>
+      <c r="AS5" s="12" t="n">
+        <v>20862956050.8977</v>
+      </c>
+      <c r="AT5" s="12" t="n">
+        <v>16353377327.1689</v>
+      </c>
+      <c r="AU5" s="12" t="n">
+        <v>17374298546.2222</v>
+      </c>
+      <c r="AV5" s="12" t="n">
+        <v>14287090568.7343</v>
+      </c>
+      <c r="AW5" s="12" t="n">
+        <v>33328417151.5841</v>
+      </c>
+      <c r="AX5" s="12"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -6827,89 +6830,89 @@
       <c r="O6" t="s">
         <v>57</v>
       </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3" t="n">
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12" t="n">
         <v>4754887357</v>
       </c>
-      <c r="AA6" s="3" t="n">
-        <v>5079917345</v>
-      </c>
-      <c r="AB6" s="3" t="n">
-        <v>5896551985.5</v>
-      </c>
-      <c r="AC6" s="3" t="n">
-        <v>10867533308.0431</v>
-      </c>
-      <c r="AD6" s="3" t="n">
-        <v>11748237631.1209</v>
-      </c>
-      <c r="AE6" s="3" t="n">
-        <v>11909342815.0938</v>
-      </c>
-      <c r="AF6" s="3" t="n">
-        <v>13955054549.5041</v>
-      </c>
-      <c r="AG6" s="3" t="n">
-        <v>13306872348.3573</v>
-      </c>
-      <c r="AH6" s="3" t="n">
-        <v>12825711255.1507</v>
-      </c>
-      <c r="AI6" s="3" t="n">
-        <v>11940478265.8961</v>
-      </c>
-      <c r="AJ6" s="3" t="n">
+      <c r="AA6" s="12" t="n">
+        <v>5079917334</v>
+      </c>
+      <c r="AB6" s="12" t="n">
+        <v>5896551978.5</v>
+      </c>
+      <c r="AC6" s="12" t="n">
+        <v>10867533298.05</v>
+      </c>
+      <c r="AD6" s="12" t="n">
+        <v>11748237581.12</v>
+      </c>
+      <c r="AE6" s="12" t="n">
+        <v>11909342834.67</v>
+      </c>
+      <c r="AF6" s="12" t="n">
+        <v>13955054520.7164</v>
+      </c>
+      <c r="AG6" s="12" t="n">
+        <v>13306872364.9494</v>
+      </c>
+      <c r="AH6" s="12" t="n">
+        <v>12825711257.4344</v>
+      </c>
+      <c r="AI6" s="12" t="n">
+        <v>11940478232.0369</v>
+      </c>
+      <c r="AJ6" s="12" t="n">
         <v>12534021537.2026</v>
       </c>
-      <c r="AK6" s="3" t="n">
+      <c r="AK6" s="12" t="n">
         <v>11591985438.8239</v>
       </c>
-      <c r="AL6" s="3" t="n">
+      <c r="AL6" s="12" t="n">
         <v>12288986042.0497</v>
       </c>
-      <c r="AM6" s="3" t="n">
+      <c r="AM6" s="12" t="n">
         <v>11646909626.7398</v>
       </c>
-      <c r="AN6" s="3" t="n">
+      <c r="AN6" s="12" t="n">
         <v>11565596250.5205</v>
       </c>
-      <c r="AO6" s="3" t="n">
+      <c r="AO6" s="12" t="n">
         <v>11141586749.5001</v>
       </c>
-      <c r="AP6" s="3" t="n">
+      <c r="AP6" s="12" t="n">
         <v>11450457090.4495</v>
       </c>
-      <c r="AQ6" s="3" t="n">
+      <c r="AQ6" s="12" t="n">
         <v>12605014750.6374</v>
       </c>
-      <c r="AR6" s="3" t="n">
-        <v>11306299211.1611</v>
-      </c>
-      <c r="AS6" s="3" t="n">
-        <v>12261823447.3584</v>
-      </c>
-      <c r="AT6" s="3" t="n">
-        <v>8775269572.6885</v>
-      </c>
-      <c r="AU6" s="3" t="n">
-        <v>9273692343.2085</v>
-      </c>
-      <c r="AV6" s="3" t="n">
-        <v>9580549306.11</v>
-      </c>
-      <c r="AW6" s="3" t="n">
-        <v>4190750910.5895</v>
-      </c>
-      <c r="AX6" s="3"/>
+      <c r="AR6" s="12" t="n">
+        <v>11335866345.5578</v>
+      </c>
+      <c r="AS6" s="12" t="n">
+        <v>12269942976.0774</v>
+      </c>
+      <c r="AT6" s="12" t="n">
+        <v>8815954156.05</v>
+      </c>
+      <c r="AU6" s="12" t="n">
+        <v>9355260343.4745</v>
+      </c>
+      <c r="AV6" s="12" t="n">
+        <v>9648889535.2315</v>
+      </c>
+      <c r="AW6" s="12" t="n">
+        <v>8544697923.0524</v>
+      </c>
+      <c r="AX6" s="12"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -6927,89 +6930,89 @@
       <c r="O7" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3" t="n">
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12" t="n">
         <v>7398907757</v>
       </c>
-      <c r="AA7" s="3" t="n">
-        <v>6353075318</v>
-      </c>
-      <c r="AB7" s="3" t="n">
-        <v>5093396308</v>
-      </c>
-      <c r="AC7" s="3" t="n">
-        <v>5928596277.8101</v>
-      </c>
-      <c r="AD7" s="3" t="n">
-        <v>5003115808.375</v>
-      </c>
-      <c r="AE7" s="3" t="n">
-        <v>3813708765.0596</v>
-      </c>
-      <c r="AF7" s="3" t="n">
-        <v>4546730798.9782</v>
-      </c>
-      <c r="AG7" s="3" t="n">
-        <v>7470415372.3167</v>
-      </c>
-      <c r="AH7" s="3" t="n">
-        <v>4537302372.7743</v>
-      </c>
-      <c r="AI7" s="3" t="n">
-        <v>5828136823.7699</v>
-      </c>
-      <c r="AJ7" s="3" t="n">
+      <c r="AA7" s="12" t="n">
+        <v>6353322328</v>
+      </c>
+      <c r="AB7" s="12" t="n">
+        <v>5093455977</v>
+      </c>
+      <c r="AC7" s="12" t="n">
+        <v>5928596212.81</v>
+      </c>
+      <c r="AD7" s="12" t="n">
+        <v>5003115825.36</v>
+      </c>
+      <c r="AE7" s="12" t="n">
+        <v>3813708765.34</v>
+      </c>
+      <c r="AF7" s="12" t="n">
+        <v>4546730791.0395</v>
+      </c>
+      <c r="AG7" s="12" t="n">
+        <v>7470415397.404</v>
+      </c>
+      <c r="AH7" s="12" t="n">
+        <v>4537302363.0974</v>
+      </c>
+      <c r="AI7" s="12" t="n">
+        <v>5828136846.3726</v>
+      </c>
+      <c r="AJ7" s="12" t="n">
         <v>6003155036.8935</v>
       </c>
-      <c r="AK7" s="3" t="n">
+      <c r="AK7" s="12" t="n">
         <v>3322679344.7227</v>
       </c>
-      <c r="AL7" s="3" t="n">
+      <c r="AL7" s="12" t="n">
         <v>11632708635.5434</v>
       </c>
-      <c r="AM7" s="3" t="n">
+      <c r="AM7" s="12" t="n">
         <v>9615807939.0697</v>
       </c>
-      <c r="AN7" s="3" t="n">
+      <c r="AN7" s="12" t="n">
         <v>2892889203.162</v>
       </c>
-      <c r="AO7" s="3" t="n">
+      <c r="AO7" s="12" t="n">
         <v>2357317641.1424</v>
       </c>
-      <c r="AP7" s="3" t="n">
+      <c r="AP7" s="12" t="n">
         <v>14587293141.1913</v>
       </c>
-      <c r="AQ7" s="3" t="n">
+      <c r="AQ7" s="12" t="n">
         <v>26373033545.9417</v>
       </c>
-      <c r="AR7" s="3" t="n">
-        <v>20795343635.5401</v>
-      </c>
-      <c r="AS7" s="3" t="n">
-        <v>15589907994.7755</v>
-      </c>
-      <c r="AT7" s="3" t="n">
-        <v>37020630921.7999</v>
-      </c>
-      <c r="AU7" s="3" t="n">
-        <v>11100489237.975</v>
-      </c>
-      <c r="AV7" s="3" t="n">
-        <v>18909526156.1226</v>
-      </c>
-      <c r="AW7" s="3" t="n">
-        <v>8114033874.1767</v>
-      </c>
-      <c r="AX7" s="3"/>
+      <c r="AR7" s="12" t="n">
+        <v>20704226038.0419</v>
+      </c>
+      <c r="AS7" s="12" t="n">
+        <v>15369429068.7005</v>
+      </c>
+      <c r="AT7" s="12" t="n">
+        <v>37020630923.4319</v>
+      </c>
+      <c r="AU7" s="12" t="n">
+        <v>11160270195.3109</v>
+      </c>
+      <c r="AV7" s="12" t="n">
+        <v>18924117475.2411</v>
+      </c>
+      <c r="AW7" s="12" t="n">
+        <v>15366198673.9905</v>
+      </c>
+      <c r="AX7" s="12"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -7027,81 +7030,81 @@
       <c r="O8" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3" t="n">
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3" t="n">
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12" t="n">
         <v>4989000</v>
       </c>
-      <c r="AC8" s="3" t="n">
+      <c r="AC8" s="12" t="n">
         <v>649938</v>
       </c>
-      <c r="AD8" s="3" t="n">
+      <c r="AD8" s="12" t="n">
         <v>3004126</v>
       </c>
-      <c r="AE8" s="3" t="n">
+      <c r="AE8" s="12" t="n">
         <v>23379295</v>
       </c>
-      <c r="AF8" s="3" t="n">
+      <c r="AF8" s="12" t="n">
         <v>53203268</v>
       </c>
-      <c r="AG8" s="3" t="n">
-        <v>897160922.3025</v>
-      </c>
-      <c r="AH8" s="3" t="n">
-        <v>1766320288.9257</v>
-      </c>
-      <c r="AI8" s="3" t="n">
-        <v>2561032400.5561</v>
-      </c>
-      <c r="AJ8" s="3" t="n">
+      <c r="AG8" s="12" t="n">
+        <v>897160924.2524</v>
+      </c>
+      <c r="AH8" s="12" t="n">
+        <v>1766320286.594</v>
+      </c>
+      <c r="AI8" s="12" t="n">
+        <v>2561032404.8141</v>
+      </c>
+      <c r="AJ8" s="12" t="n">
         <v>10524681.1805</v>
       </c>
-      <c r="AK8" s="3" t="n">
+      <c r="AK8" s="12" t="n">
         <v>227016.0541</v>
       </c>
-      <c r="AL8" s="3" t="n">
+      <c r="AL8" s="12" t="n">
         <v>-6018055.4866</v>
       </c>
-      <c r="AM8" s="3" t="n">
+      <c r="AM8" s="12" t="n">
         <v>-3983829.0098</v>
       </c>
-      <c r="AN8" s="3" t="n">
+      <c r="AN8" s="12" t="n">
         <v>-1767022.54</v>
       </c>
-      <c r="AO8" s="3" t="n">
+      <c r="AO8" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AP8" s="3" t="n">
+      <c r="AP8" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AQ8" s="3" t="n">
+      <c r="AQ8" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AR8" s="3" t="n">
+      <c r="AR8" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AS8" s="3" t="n">
+      <c r="AS8" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AT8" s="3" t="n">
+      <c r="AT8" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AU8" s="3"/>
-      <c r="AV8" s="3"/>
-      <c r="AW8" s="3"/>
-      <c r="AX8" s="3"/>
+      <c r="AU8" s="12"/>
+      <c r="AV8" s="12"/>
+      <c r="AW8" s="12"/>
+      <c r="AX8" s="12"/>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -7117,109 +7120,109 @@
         <v>60</v>
       </c>
       <c r="O9"/>
-      <c r="P9" s="3" t="n">
+      <c r="P9" s="12" t="n">
         <v>30980247148</v>
       </c>
-      <c r="Q9" s="3" t="n">
+      <c r="Q9" s="12" t="n">
         <v>30513099255</v>
       </c>
-      <c r="R9" s="3" t="n">
+      <c r="R9" s="12" t="n">
         <v>30337971567</v>
       </c>
-      <c r="S9" s="3" t="n">
+      <c r="S9" s="12" t="n">
         <v>29918044865</v>
       </c>
-      <c r="T9" s="3" t="n">
+      <c r="T9" s="12" t="n">
         <v>30546960405</v>
       </c>
-      <c r="U9" s="3" t="n">
+      <c r="U9" s="12" t="n">
         <v>26815505318</v>
       </c>
-      <c r="V9" s="3" t="n">
+      <c r="V9" s="12" t="n">
         <v>28856006190</v>
       </c>
-      <c r="W9" s="3" t="n">
+      <c r="W9" s="12" t="n">
         <v>24930833919</v>
       </c>
-      <c r="X9" s="3" t="n">
+      <c r="X9" s="12" t="n">
         <v>26529770069</v>
       </c>
-      <c r="Y9" s="3" t="n">
+      <c r="Y9" s="12" t="n">
         <v>27545374131</v>
       </c>
-      <c r="Z9" s="3" t="n">
+      <c r="Z9" s="12" t="n">
         <v>1165484638</v>
       </c>
-      <c r="AA9" s="3" t="n">
+      <c r="AA9" s="12" t="n">
         <v>82191621</v>
       </c>
-      <c r="AB9" s="3" t="n">
-        <v>132500791.1201</v>
-      </c>
-      <c r="AC9" s="3" t="n">
+      <c r="AB9" s="12" t="n">
+        <v>132500791.12</v>
+      </c>
+      <c r="AC9" s="12" t="n">
         <v>168663563</v>
       </c>
-      <c r="AD9" s="3" t="n">
+      <c r="AD9" s="12" t="n">
         <v>190982087</v>
       </c>
-      <c r="AE9" s="3" t="n">
+      <c r="AE9" s="12" t="n">
         <v>176182910</v>
       </c>
-      <c r="AF9" s="3" t="n">
+      <c r="AF9" s="12" t="n">
         <v>66663467.55</v>
       </c>
-      <c r="AG9" s="3" t="n">
-        <v>11859106.1357</v>
-      </c>
-      <c r="AH9" s="3" t="n">
-        <v>1093903392.6831</v>
-      </c>
-      <c r="AI9" s="3" t="n">
-        <v>1721970881.9347</v>
-      </c>
-      <c r="AJ9" s="3" t="n">
+      <c r="AG9" s="12" t="n">
+        <v>11859106.1266</v>
+      </c>
+      <c r="AH9" s="12" t="n">
+        <v>1093903388.3803</v>
+      </c>
+      <c r="AI9" s="12" t="n">
+        <v>1721970874.3112</v>
+      </c>
+      <c r="AJ9" s="12" t="n">
         <v>860870356.5886</v>
       </c>
-      <c r="AK9" s="3" t="n">
+      <c r="AK9" s="12" t="n">
         <v>1413589516.2339</v>
       </c>
-      <c r="AL9" s="3" t="n">
+      <c r="AL9" s="12" t="n">
         <v>3138190520.6504</v>
       </c>
-      <c r="AM9" s="3" t="n">
+      <c r="AM9" s="12" t="n">
         <v>146593784.5212</v>
       </c>
-      <c r="AN9" s="3" t="n">
+      <c r="AN9" s="12" t="n">
         <v>139579867.4808</v>
       </c>
-      <c r="AO9" s="3" t="n">
+      <c r="AO9" s="12" t="n">
         <v>242406172.4482</v>
       </c>
-      <c r="AP9" s="3" t="n">
+      <c r="AP9" s="12" t="n">
         <v>449203451.2652</v>
       </c>
-      <c r="AQ9" s="3" t="n">
+      <c r="AQ9" s="12" t="n">
         <v>-12199817.5281</v>
       </c>
-      <c r="AR9" s="3" t="n">
+      <c r="AR9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AS9" s="3" t="n">
+      <c r="AS9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AT9" s="3" t="n">
+      <c r="AT9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AU9" s="3" t="n">
+      <c r="AU9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AV9" s="3" t="n">
+      <c r="AV9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AW9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="3"/>
+      <c r="AW9" s="12" t="n">
+        <v>-39324.9492</v>
+      </c>
+      <c r="AX9" s="12"/>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -7234,107 +7237,107 @@
       <c r="O10" t="s">
         <v>434</v>
       </c>
-      <c r="P10" s="3" t="str">
+      <c r="P10" s="12" t="str">
         <f>Sum(P2:P9)</f>
       </c>
-      <c r="Q10" s="3" t="str">
+      <c r="Q10" s="12" t="str">
         <f>Sum(Q2:Q9)</f>
       </c>
-      <c r="R10" s="3" t="str">
+      <c r="R10" s="12" t="str">
         <f>Sum(R2:R9)</f>
       </c>
-      <c r="S10" s="3" t="str">
+      <c r="S10" s="12" t="str">
         <f>Sum(S2:S9)</f>
       </c>
-      <c r="T10" s="3" t="str">
+      <c r="T10" s="12" t="str">
         <f>Sum(T2:T9)</f>
       </c>
-      <c r="U10" s="3" t="str">
+      <c r="U10" s="12" t="str">
         <f>Sum(U2:U9)</f>
       </c>
-      <c r="V10" s="3" t="str">
+      <c r="V10" s="12" t="str">
         <f>Sum(V2:V9)</f>
       </c>
-      <c r="W10" s="3" t="str">
+      <c r="W10" s="12" t="str">
         <f>Sum(W2:W9)</f>
       </c>
-      <c r="X10" s="3" t="str">
+      <c r="X10" s="12" t="str">
         <f>Sum(X2:X9)</f>
       </c>
-      <c r="Y10" s="3" t="str">
+      <c r="Y10" s="12" t="str">
         <f>Sum(Y2:Y9)</f>
       </c>
-      <c r="Z10" s="3" t="str">
+      <c r="Z10" s="12" t="str">
         <f>Sum(Z2:Z9)</f>
       </c>
-      <c r="AA10" s="3" t="str">
+      <c r="AA10" s="12" t="str">
         <f>Sum(AA2:AA9)</f>
       </c>
-      <c r="AB10" s="3" t="str">
+      <c r="AB10" s="12" t="str">
         <f>Sum(AB2:AB9)</f>
       </c>
-      <c r="AC10" s="3" t="str">
+      <c r="AC10" s="12" t="str">
         <f>Sum(AC2:AC9)</f>
       </c>
-      <c r="AD10" s="3" t="str">
+      <c r="AD10" s="12" t="str">
         <f>Sum(AD2:AD9)</f>
       </c>
-      <c r="AE10" s="3" t="str">
+      <c r="AE10" s="12" t="str">
         <f>Sum(AE2:AE9)</f>
       </c>
-      <c r="AF10" s="3" t="str">
+      <c r="AF10" s="12" t="str">
         <f>Sum(AF2:AF9)</f>
       </c>
-      <c r="AG10" s="3" t="str">
+      <c r="AG10" s="12" t="str">
         <f>Sum(AG2:AG9)</f>
       </c>
-      <c r="AH10" s="3" t="str">
+      <c r="AH10" s="12" t="str">
         <f>Sum(AH2:AH9)</f>
       </c>
-      <c r="AI10" s="3" t="str">
+      <c r="AI10" s="12" t="str">
         <f>Sum(AI2:AI9)</f>
       </c>
-      <c r="AJ10" s="3" t="str">
+      <c r="AJ10" s="12" t="str">
         <f>Sum(AJ2:AJ9)</f>
       </c>
-      <c r="AK10" s="3" t="str">
+      <c r="AK10" s="12" t="str">
         <f>Sum(AK2:AK9)</f>
       </c>
-      <c r="AL10" s="3" t="str">
+      <c r="AL10" s="12" t="str">
         <f>Sum(AL2:AL9)</f>
       </c>
-      <c r="AM10" s="3" t="str">
+      <c r="AM10" s="12" t="str">
         <f>Sum(AM2:AM9)</f>
       </c>
-      <c r="AN10" s="3" t="str">
+      <c r="AN10" s="12" t="str">
         <f>Sum(AN2:AN9)</f>
       </c>
-      <c r="AO10" s="3" t="str">
+      <c r="AO10" s="12" t="str">
         <f>Sum(AO2:AO9)</f>
       </c>
-      <c r="AP10" s="3" t="str">
+      <c r="AP10" s="12" t="str">
         <f>Sum(AP2:AP9)</f>
       </c>
-      <c r="AQ10" s="3" t="str">
+      <c r="AQ10" s="12" t="str">
         <f>Sum(AQ2:AQ9)</f>
       </c>
-      <c r="AR10" s="3" t="str">
+      <c r="AR10" s="12" t="str">
         <f>Sum(AR2:AR9)</f>
       </c>
-      <c r="AS10" s="3" t="str">
+      <c r="AS10" s="12" t="str">
         <f>Sum(AS2:AS9)</f>
       </c>
-      <c r="AT10" s="3" t="str">
+      <c r="AT10" s="12" t="str">
         <f>Sum(AT2:AT9)</f>
       </c>
-      <c r="AU10" s="3" t="str">
+      <c r="AU10" s="12" t="str">
         <f>Sum(AU2:AU9)</f>
       </c>
-      <c r="AV10" s="3" t="str">
+      <c r="AV10" s="12" t="str">
         <f>Sum(AV2:AV9)</f>
       </c>
-      <c r="AW10" s="3"/>
-      <c r="AX10" s="3"/>
+      <c r="AW10" s="12"/>
+      <c r="AX10" s="12"/>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -7466,94 +7469,94 @@
         <v>50</v>
       </c>
       <c r="N14" t="s">
-        <v>50</v>
+        <v>440</v>
       </c>
       <c r="O14" t="s">
         <v>51</v>
       </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3" t="n">
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12" t="n">
         <v>29786010617.463</v>
       </c>
-      <c r="AA14" s="3" t="n">
-        <v>31761574296.7241</v>
-      </c>
-      <c r="AB14" s="3" t="n">
-        <v>36407707891.7418</v>
-      </c>
-      <c r="AC14" s="3" t="n">
-        <v>40651156223.7523</v>
-      </c>
-      <c r="AD14" s="3" t="n">
-        <v>36399026091.3253</v>
-      </c>
-      <c r="AE14" s="3" t="n">
-        <v>29051789404.6939</v>
-      </c>
-      <c r="AF14" s="3" t="n">
-        <v>37512298572.6687</v>
-      </c>
-      <c r="AG14" s="3" t="n">
-        <v>39573297692.6881</v>
-      </c>
-      <c r="AH14" s="3" t="n">
-        <v>38872811632.1524</v>
-      </c>
-      <c r="AI14" s="3" t="n">
-        <v>39896785670.8544</v>
-      </c>
-      <c r="AJ14" s="3" t="n">
+      <c r="AA14" s="12" t="n">
+        <v>31761184787.6246</v>
+      </c>
+      <c r="AB14" s="12" t="n">
+        <v>36407615094.2625</v>
+      </c>
+      <c r="AC14" s="12" t="n">
+        <v>40651156098.7978</v>
+      </c>
+      <c r="AD14" s="12" t="n">
+        <v>36399026133.0462</v>
+      </c>
+      <c r="AE14" s="12" t="n">
+        <v>29051789386.4419</v>
+      </c>
+      <c r="AF14" s="12" t="n">
+        <v>37512298618.728</v>
+      </c>
+      <c r="AG14" s="12" t="n">
+        <v>39573297745.062</v>
+      </c>
+      <c r="AH14" s="12" t="n">
+        <v>38872811572.4836</v>
+      </c>
+      <c r="AI14" s="12" t="n">
+        <v>39896785637.729</v>
+      </c>
+      <c r="AJ14" s="12" t="n">
         <v>41587320644.0153</v>
       </c>
-      <c r="AK14" s="3" t="n">
+      <c r="AK14" s="12" t="n">
         <v>44086655785.1458</v>
       </c>
-      <c r="AL14" s="3" t="n">
+      <c r="AL14" s="12" t="n">
         <v>42879359543.4218</v>
       </c>
-      <c r="AM14" s="3" t="n">
+      <c r="AM14" s="12" t="n">
         <v>39515036888.135</v>
       </c>
-      <c r="AN14" s="3" t="n">
+      <c r="AN14" s="12" t="n">
         <v>33100077617.8106</v>
       </c>
-      <c r="AO14" s="3" t="n">
+      <c r="AO14" s="12" t="n">
         <v>34959307472.6217</v>
       </c>
-      <c r="AP14" s="3" t="n">
+      <c r="AP14" s="12" t="n">
         <v>38017242551.0955</v>
       </c>
-      <c r="AQ14" s="3" t="n">
+      <c r="AQ14" s="12" t="n">
         <v>37903505402.2661</v>
       </c>
-      <c r="AR14" s="3" t="n">
-        <v>38856954937.7067</v>
-      </c>
-      <c r="AS14" s="3" t="n">
-        <v>45833718808.7397</v>
-      </c>
-      <c r="AT14" s="3" t="n">
-        <v>46773942202.7291</v>
-      </c>
-      <c r="AU14" s="3" t="n">
-        <v>36006709571.0263</v>
-      </c>
-      <c r="AV14" s="3" t="n">
-        <v>31510444831.3847</v>
-      </c>
-      <c r="AW14" s="3" t="n">
-        <v>17190499492.3007</v>
-      </c>
-      <c r="AX14" s="3"/>
+      <c r="AR14" s="12" t="n">
+        <v>38976365781.3209</v>
+      </c>
+      <c r="AS14" s="12" t="n">
+        <v>45808483967.6321</v>
+      </c>
+      <c r="AT14" s="12" t="n">
+        <v>46784384001.7756</v>
+      </c>
+      <c r="AU14" s="12" t="n">
+        <v>36040792723.8254</v>
+      </c>
+      <c r="AV14" s="12" t="n">
+        <v>31429996545.6082</v>
+      </c>
+      <c r="AW14" s="12" t="n">
+        <v>36942288489.316</v>
+      </c>
+      <c r="AX14" s="12"/>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -7571,89 +7574,89 @@
       <c r="O15" t="s">
         <v>53</v>
       </c>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3" t="n">
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12" t="n">
         <v>1320408442.98445</v>
       </c>
-      <c r="AA15" s="3" t="n">
-        <v>2669988398.66522</v>
-      </c>
-      <c r="AB15" s="3" t="n">
-        <v>2895422124.89965</v>
-      </c>
-      <c r="AC15" s="3" t="n">
+      <c r="AA15" s="12" t="n">
+        <v>2669988450.72197</v>
+      </c>
+      <c r="AB15" s="12" t="n">
+        <v>2895422143.53524</v>
+      </c>
+      <c r="AC15" s="12" t="n">
         <v>2696918471.41241</v>
       </c>
-      <c r="AD15" s="3" t="n">
-        <v>3673210219.13174</v>
-      </c>
-      <c r="AE15" s="3" t="n">
-        <v>11044058775.2657</v>
-      </c>
-      <c r="AF15" s="3" t="n">
-        <v>5314427294.80668</v>
-      </c>
-      <c r="AG15" s="3" t="n">
-        <v>5093298065.54142</v>
-      </c>
-      <c r="AH15" s="3" t="n">
-        <v>10186158913.8455</v>
-      </c>
-      <c r="AI15" s="3" t="n">
-        <v>5322818217.91768</v>
-      </c>
-      <c r="AJ15" s="3" t="n">
+      <c r="AD15" s="12" t="n">
+        <v>3673210247.39384</v>
+      </c>
+      <c r="AE15" s="12" t="n">
+        <v>11044058638.1185</v>
+      </c>
+      <c r="AF15" s="12" t="n">
+        <v>5314427340.94513</v>
+      </c>
+      <c r="AG15" s="12" t="n">
+        <v>5093297997.24257</v>
+      </c>
+      <c r="AH15" s="12" t="n">
+        <v>10186159007.7479</v>
+      </c>
+      <c r="AI15" s="12" t="n">
+        <v>5322818327.82991</v>
+      </c>
+      <c r="AJ15" s="12" t="n">
         <v>2843557407.88621</v>
       </c>
-      <c r="AK15" s="3" t="n">
+      <c r="AK15" s="12" t="n">
         <v>1546538291.92095</v>
       </c>
-      <c r="AL15" s="3" t="n">
+      <c r="AL15" s="12" t="n">
         <v>677068208.438066</v>
       </c>
-      <c r="AM15" s="3" t="n">
+      <c r="AM15" s="12" t="n">
         <v>546737697.112464</v>
       </c>
-      <c r="AN15" s="3" t="n">
+      <c r="AN15" s="12" t="n">
         <v>396672955.904907</v>
       </c>
-      <c r="AO15" s="3" t="n">
+      <c r="AO15" s="12" t="n">
         <v>173950619.796659</v>
       </c>
-      <c r="AP15" s="3" t="n">
+      <c r="AP15" s="12" t="n">
         <v>172521499.011218</v>
       </c>
-      <c r="AQ15" s="3" t="n">
+      <c r="AQ15" s="12" t="n">
         <v>241346649.222185</v>
       </c>
-      <c r="AR15" s="3" t="n">
-        <v>176419367.317106</v>
-      </c>
-      <c r="AS15" s="3" t="n">
-        <v>225753885.564047</v>
-      </c>
-      <c r="AT15" s="3" t="n">
-        <v>557895366.028543</v>
-      </c>
-      <c r="AU15" s="3" t="n">
-        <v>479168686.662567</v>
-      </c>
-      <c r="AV15" s="3" t="n">
-        <v>382801102.4745</v>
-      </c>
-      <c r="AW15" s="3" t="n">
-        <v>165034989.028634</v>
-      </c>
-      <c r="AX15" s="3"/>
+      <c r="AR15" s="12" t="n">
+        <v>176419367.201088</v>
+      </c>
+      <c r="AS15" s="12" t="n">
+        <v>225753884.751953</v>
+      </c>
+      <c r="AT15" s="12" t="n">
+        <v>487094360.981809</v>
+      </c>
+      <c r="AU15" s="12" t="n">
+        <v>478981745.552354</v>
+      </c>
+      <c r="AV15" s="12" t="n">
+        <v>358397023.6191</v>
+      </c>
+      <c r="AW15" s="12" t="n">
+        <v>383791414.669169</v>
+      </c>
+      <c r="AX15" s="12"/>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -7671,89 +7674,89 @@
       <c r="O16" t="s">
         <v>54</v>
       </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3" t="n">
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12" t="n">
         <v>2237286115.1091</v>
       </c>
-      <c r="AA16" s="3" t="n">
-        <v>1898228682.15376</v>
-      </c>
-      <c r="AB16" s="3" t="n">
+      <c r="AA16" s="12" t="n">
+        <v>1898228683.73124</v>
+      </c>
+      <c r="AB16" s="12" t="n">
         <v>2094170866.21501</v>
       </c>
-      <c r="AC16" s="3" t="n">
+      <c r="AC16" s="12" t="n">
         <v>2448802662.94239</v>
       </c>
-      <c r="AD16" s="3" t="n">
-        <v>2774735171.19095</v>
-      </c>
-      <c r="AE16" s="3" t="n">
-        <v>2249161432.17508</v>
-      </c>
-      <c r="AF16" s="3" t="n">
+      <c r="AD16" s="12" t="n">
+        <v>2774735169.69781</v>
+      </c>
+      <c r="AE16" s="12" t="n">
+        <v>2249161432.16065</v>
+      </c>
+      <c r="AF16" s="12" t="n">
         <v>3247966549.92842</v>
       </c>
-      <c r="AG16" s="3" t="n">
-        <v>3070830766.67967</v>
-      </c>
-      <c r="AH16" s="3" t="n">
-        <v>3240950478.26946</v>
-      </c>
-      <c r="AI16" s="3" t="n">
-        <v>2928911183.50628</v>
-      </c>
-      <c r="AJ16" s="3" t="n">
+      <c r="AG16" s="12" t="n">
+        <v>3071729395.11295</v>
+      </c>
+      <c r="AH16" s="12" t="n">
+        <v>3240950477.37501</v>
+      </c>
+      <c r="AI16" s="12" t="n">
+        <v>2928911181.80544</v>
+      </c>
+      <c r="AJ16" s="12" t="n">
         <v>2215399901.96351</v>
       </c>
-      <c r="AK16" s="3" t="n">
+      <c r="AK16" s="12" t="n">
         <v>1652435274.36129</v>
       </c>
-      <c r="AL16" s="3" t="n">
+      <c r="AL16" s="12" t="n">
         <v>1256103031.85403</v>
       </c>
-      <c r="AM16" s="3" t="n">
+      <c r="AM16" s="12" t="n">
         <v>405193189.569817</v>
       </c>
-      <c r="AN16" s="3" t="n">
+      <c r="AN16" s="12" t="n">
         <v>202108300.893478</v>
       </c>
-      <c r="AO16" s="3" t="n">
+      <c r="AO16" s="12" t="n">
         <v>178032842.611906</v>
       </c>
-      <c r="AP16" s="3" t="n">
+      <c r="AP16" s="12" t="n">
         <v>231030174.39661</v>
       </c>
-      <c r="AQ16" s="3" t="n">
+      <c r="AQ16" s="12" t="n">
         <v>344854968.410083</v>
       </c>
-      <c r="AR16" s="3" t="n">
-        <v>254444787.368194</v>
-      </c>
-      <c r="AS16" s="3" t="n">
-        <v>277364465.275309</v>
-      </c>
-      <c r="AT16" s="3" t="n">
-        <v>371206955.248742</v>
-      </c>
-      <c r="AU16" s="3" t="n">
-        <v>291592172.729369</v>
-      </c>
-      <c r="AV16" s="3" t="n">
-        <v>460093866.8452</v>
-      </c>
-      <c r="AW16" s="3" t="n">
-        <v>305716407.330048</v>
-      </c>
-      <c r="AX16" s="3"/>
+      <c r="AR16" s="12" t="n">
+        <v>254444787.348439</v>
+      </c>
+      <c r="AS16" s="12" t="n">
+        <v>277364465.274973</v>
+      </c>
+      <c r="AT16" s="12" t="n">
+        <v>372873224.606</v>
+      </c>
+      <c r="AU16" s="12" t="n">
+        <v>293196104.115767</v>
+      </c>
+      <c r="AV16" s="12" t="n">
+        <v>460093867.2378</v>
+      </c>
+      <c r="AW16" s="12" t="n">
+        <v>593483157.261755</v>
+      </c>
+      <c r="AX16" s="12"/>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -7771,89 +7774,89 @@
       <c r="O17" t="s">
         <v>55</v>
       </c>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3" t="n">
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12" t="n">
         <v>2365638871.69887</v>
       </c>
-      <c r="AA17" s="3" t="n">
-        <v>2486655041.88006</v>
-      </c>
-      <c r="AB17" s="3" t="n">
-        <v>1928041260.78669</v>
-      </c>
-      <c r="AC17" s="3" t="n">
+      <c r="AA17" s="12" t="n">
+        <v>2486655048.18997</v>
+      </c>
+      <c r="AB17" s="12" t="n">
+        <v>1928041262.33965</v>
+      </c>
+      <c r="AC17" s="12" t="n">
         <v>3391979685.61362</v>
       </c>
-      <c r="AD17" s="3" t="n">
-        <v>3051861200.32888</v>
-      </c>
-      <c r="AE17" s="3" t="n">
-        <v>2927980233.45955</v>
-      </c>
-      <c r="AF17" s="3" t="n">
-        <v>3351225956.68921</v>
-      </c>
-      <c r="AG17" s="3" t="n">
-        <v>5056314730.71768</v>
-      </c>
-      <c r="AH17" s="3" t="n">
-        <v>9689975460.48866</v>
-      </c>
-      <c r="AI17" s="3" t="n">
-        <v>9647629779.3483</v>
-      </c>
-      <c r="AJ17" s="3" t="n">
+      <c r="AD17" s="12" t="n">
+        <v>3051861216.69115</v>
+      </c>
+      <c r="AE17" s="12" t="n">
+        <v>2927980234.90321</v>
+      </c>
+      <c r="AF17" s="12" t="n">
+        <v>3351225966.444</v>
+      </c>
+      <c r="AG17" s="12" t="n">
+        <v>5056314763.40096</v>
+      </c>
+      <c r="AH17" s="12" t="n">
+        <v>9689975442.18236</v>
+      </c>
+      <c r="AI17" s="12" t="n">
+        <v>9647629828.53015</v>
+      </c>
+      <c r="AJ17" s="12" t="n">
         <v>11169563015.1701</v>
       </c>
-      <c r="AK17" s="3" t="n">
+      <c r="AK17" s="12" t="n">
         <v>21930105676.6872</v>
       </c>
-      <c r="AL17" s="3" t="n">
+      <c r="AL17" s="12" t="n">
         <v>19550596323.611</v>
       </c>
-      <c r="AM17" s="3" t="n">
+      <c r="AM17" s="12" t="n">
         <v>23658498563.3684</v>
       </c>
-      <c r="AN17" s="3" t="n">
+      <c r="AN17" s="12" t="n">
         <v>19228312977.8257</v>
       </c>
-      <c r="AO17" s="3" t="n">
+      <c r="AO17" s="12" t="n">
         <v>22204438295.4597</v>
       </c>
-      <c r="AP17" s="3" t="n">
+      <c r="AP17" s="12" t="n">
         <v>19701607199.2135</v>
       </c>
-      <c r="AQ17" s="3" t="n">
+      <c r="AQ17" s="12" t="n">
         <v>16272835609.4825</v>
       </c>
-      <c r="AR17" s="3" t="n">
-        <v>19220458282.8904</v>
-      </c>
-      <c r="AS17" s="3" t="n">
-        <v>23365991209.5999</v>
-      </c>
-      <c r="AT17" s="3" t="n">
-        <v>18074256698.7538</v>
-      </c>
-      <c r="AU17" s="3" t="n">
-        <v>18954458708.1024</v>
-      </c>
-      <c r="AV17" s="3" t="n">
-        <v>14287090543.2938</v>
-      </c>
-      <c r="AW17" s="3" t="n">
-        <v>18529774324.4552</v>
-      </c>
-      <c r="AX17" s="3"/>
+      <c r="AR17" s="12" t="n">
+        <v>19210754862.0908</v>
+      </c>
+      <c r="AS17" s="12" t="n">
+        <v>23365991248.2096</v>
+      </c>
+      <c r="AT17" s="12" t="n">
+        <v>18074256695.9298</v>
+      </c>
+      <c r="AU17" s="12" t="n">
+        <v>18578121905.9866</v>
+      </c>
+      <c r="AV17" s="12" t="n">
+        <v>14287090568.7343</v>
+      </c>
+      <c r="AW17" s="12" t="n">
+        <v>31788590268.3252</v>
+      </c>
+      <c r="AX17" s="12"/>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -7871,89 +7874,89 @@
       <c r="O18" t="s">
         <v>57</v>
       </c>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3" t="n">
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12" t="n">
         <v>7682614385.97241</v>
       </c>
-      <c r="AA18" s="3" t="n">
-        <v>8013453483.81472</v>
-      </c>
-      <c r="AB18" s="3" t="n">
-        <v>9157143809.7321</v>
-      </c>
-      <c r="AC18" s="3" t="n">
-        <v>16560363869.0103</v>
-      </c>
-      <c r="AD18" s="3" t="n">
-        <v>17475260624.7798</v>
-      </c>
-      <c r="AE18" s="3" t="n">
-        <v>17192978801.9298</v>
-      </c>
-      <c r="AF18" s="3" t="n">
-        <v>19511047169.0537</v>
-      </c>
-      <c r="AG18" s="3" t="n">
-        <v>18108217362.1872</v>
-      </c>
-      <c r="AH18" s="3" t="n">
-        <v>17096875385.7715</v>
-      </c>
-      <c r="AI18" s="3" t="n">
-        <v>15756726699.6686</v>
-      </c>
-      <c r="AJ18" s="3" t="n">
+      <c r="AA18" s="12" t="n">
+        <v>8013453466.46248</v>
+      </c>
+      <c r="AB18" s="12" t="n">
+        <v>9157143798.86134</v>
+      </c>
+      <c r="AC18" s="12" t="n">
+        <v>16560363853.7824</v>
+      </c>
+      <c r="AD18" s="12" t="n">
+        <v>17475260550.4045</v>
+      </c>
+      <c r="AE18" s="12" t="n">
+        <v>17192978830.1911</v>
+      </c>
+      <c r="AF18" s="12" t="n">
+        <v>19511047128.8046</v>
+      </c>
+      <c r="AG18" s="12" t="n">
+        <v>18108217384.766</v>
+      </c>
+      <c r="AH18" s="12" t="n">
+        <v>17096875388.8157</v>
+      </c>
+      <c r="AI18" s="12" t="n">
+        <v>15756726654.9878</v>
+      </c>
+      <c r="AJ18" s="12" t="n">
         <v>16397354369</v>
       </c>
-      <c r="AK18" s="3" t="n">
+      <c r="AK18" s="12" t="n">
         <v>14865363804.9205</v>
       </c>
-      <c r="AL18" s="3" t="n">
+      <c r="AL18" s="12" t="n">
         <v>15475520119.8005</v>
       </c>
-      <c r="AM18" s="3" t="n">
+      <c r="AM18" s="12" t="n">
         <v>14403371586.4019</v>
       </c>
-      <c r="AN18" s="3" t="n">
+      <c r="AN18" s="12" t="n">
         <v>14031363546.5291</v>
       </c>
-      <c r="AO18" s="3" t="n">
+      <c r="AO18" s="12" t="n">
         <v>13363749120.0494</v>
       </c>
-      <c r="AP18" s="3" t="n">
+      <c r="AP18" s="12" t="n">
         <v>13621349538.9329</v>
       </c>
-      <c r="AQ18" s="3" t="n">
+      <c r="AQ18" s="12" t="n">
         <v>14731781979.9485</v>
       </c>
-      <c r="AR18" s="3" t="n">
-        <v>12910793067.7795</v>
-      </c>
-      <c r="AS18" s="3" t="n">
-        <v>13732936917.4288</v>
-      </c>
-      <c r="AT18" s="3" t="n">
-        <v>9698698419.27091</v>
-      </c>
-      <c r="AU18" s="3" t="n">
-        <v>9916244181.73727</v>
-      </c>
-      <c r="AV18" s="3" t="n">
-        <v>9580549306.11</v>
-      </c>
-      <c r="AW18" s="3" t="n">
-        <v>3997131427.13735</v>
-      </c>
-      <c r="AX18" s="3"/>
+      <c r="AR18" s="12" t="n">
+        <v>12944556118.5067</v>
+      </c>
+      <c r="AS18" s="12" t="n">
+        <v>13742030587.4018</v>
+      </c>
+      <c r="AT18" s="12" t="n">
+        <v>9743664274.85727</v>
+      </c>
+      <c r="AU18" s="12" t="n">
+        <v>10003463832.5645</v>
+      </c>
+      <c r="AV18" s="12" t="n">
+        <v>9648889535.2315</v>
+      </c>
+      <c r="AW18" s="12" t="n">
+        <v>8149919031.77172</v>
+      </c>
+      <c r="AX18" s="12"/>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -7971,89 +7974,89 @@
       <c r="O19" t="s">
         <v>59</v>
       </c>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3" t="n">
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12" t="n">
         <v>11954637598.4551</v>
       </c>
-      <c r="AA19" s="3" t="n">
-        <v>10021831081.5773</v>
-      </c>
-      <c r="AB19" s="3" t="n">
-        <v>7909870478.0366</v>
-      </c>
-      <c r="AC19" s="3" t="n">
-        <v>9034222284.86127</v>
-      </c>
-      <c r="AD19" s="3" t="n">
-        <v>7442031343.97848</v>
-      </c>
-      <c r="AE19" s="3" t="n">
-        <v>5505678606.48885</v>
-      </c>
-      <c r="AF19" s="3" t="n">
-        <v>6356942480.52977</v>
-      </c>
-      <c r="AG19" s="3" t="n">
-        <v>10165867816.7477</v>
-      </c>
-      <c r="AH19" s="3" t="n">
-        <v>6048295623.66257</v>
-      </c>
-      <c r="AI19" s="3" t="n">
-        <v>7690844290.77725</v>
-      </c>
-      <c r="AJ19" s="3" t="n">
+      <c r="AA19" s="12" t="n">
+        <v>10022220734.2056</v>
+      </c>
+      <c r="AB19" s="12" t="n">
+        <v>7909963141.95533</v>
+      </c>
+      <c r="AC19" s="12" t="n">
+        <v>9034222185.81163</v>
+      </c>
+      <c r="AD19" s="12" t="n">
+        <v>7442031369.24332</v>
+      </c>
+      <c r="AE19" s="12" t="n">
+        <v>5505678606.89365</v>
+      </c>
+      <c r="AF19" s="12" t="n">
+        <v>6356942469.43039</v>
+      </c>
+      <c r="AG19" s="12" t="n">
+        <v>10165867850.8869</v>
+      </c>
+      <c r="AH19" s="12" t="n">
+        <v>6048295610.76311</v>
+      </c>
+      <c r="AI19" s="12" t="n">
+        <v>7690844320.60391</v>
+      </c>
+      <c r="AJ19" s="12" t="n">
         <v>7853493803.23143</v>
       </c>
-      <c r="AK19" s="3" t="n">
+      <c r="AK19" s="12" t="n">
         <v>4260947145.51411</v>
       </c>
-      <c r="AL19" s="3" t="n">
+      <c r="AL19" s="12" t="n">
         <v>14649069981.9448</v>
       </c>
-      <c r="AM19" s="3" t="n">
+      <c r="AM19" s="12" t="n">
         <v>11891571179.6987</v>
       </c>
-      <c r="AN19" s="3" t="n">
+      <c r="AN19" s="12" t="n">
         <v>3509648722.82898</v>
       </c>
-      <c r="AO19" s="3" t="n">
+      <c r="AO19" s="12" t="n">
         <v>2827478909.49259</v>
       </c>
-      <c r="AP19" s="3" t="n">
+      <c r="AP19" s="12" t="n">
         <v>17352898415.6251</v>
       </c>
-      <c r="AQ19" s="3" t="n">
+      <c r="AQ19" s="12" t="n">
         <v>30822794580.9453</v>
       </c>
-      <c r="AR19" s="3" t="n">
-        <v>23746441999.9417</v>
-      </c>
-      <c r="AS19" s="3" t="n">
-        <v>17460308734.66</v>
-      </c>
-      <c r="AT19" s="3" t="n">
-        <v>40916342412.9054</v>
-      </c>
-      <c r="AU19" s="3" t="n">
-        <v>11869615439.7573</v>
-      </c>
-      <c r="AV19" s="3" t="n">
-        <v>18909526156.1226</v>
-      </c>
-      <c r="AW19" s="3" t="n">
-        <v>7739152359.87302</v>
-      </c>
-      <c r="AX19" s="3"/>
+      <c r="AR19" s="12" t="n">
+        <v>23642393767.6986</v>
+      </c>
+      <c r="AS19" s="12" t="n">
+        <v>17213377827.8166</v>
+      </c>
+      <c r="AT19" s="12" t="n">
+        <v>40916342414.7091</v>
+      </c>
+      <c r="AU19" s="12" t="n">
+        <v>11933538475.8493</v>
+      </c>
+      <c r="AV19" s="12" t="n">
+        <v>18924117475.2411</v>
+      </c>
+      <c r="AW19" s="12" t="n">
+        <v>14656255393.3333</v>
+      </c>
+      <c r="AX19" s="12"/>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -8071,81 +8074,81 @@
       <c r="O20" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3" t="n">
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3" t="n">
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="12" t="n">
         <v>7747746.57784681</v>
       </c>
-      <c r="AC20" s="3" t="n">
+      <c r="AC20" s="12" t="n">
         <v>990400.440211295</v>
       </c>
-      <c r="AD20" s="3" t="n">
+      <c r="AD20" s="12" t="n">
         <v>4468575.32576727</v>
       </c>
-      <c r="AE20" s="3" t="n">
+      <c r="AE20" s="12" t="n">
         <v>33751629.2527597</v>
       </c>
-      <c r="AF20" s="3" t="n">
+      <c r="AF20" s="12" t="n">
         <v>74385339.5781023</v>
       </c>
-      <c r="AG20" s="3" t="n">
-        <v>1220871784.48958</v>
-      </c>
-      <c r="AH20" s="3" t="n">
-        <v>2354532802.92702</v>
-      </c>
-      <c r="AI20" s="3" t="n">
-        <v>3379553708.48206</v>
-      </c>
-      <c r="AJ20" s="3" t="n">
+      <c r="AG20" s="12" t="n">
+        <v>1220871787.14304</v>
+      </c>
+      <c r="AH20" s="12" t="n">
+        <v>2354532799.81883</v>
+      </c>
+      <c r="AI20" s="12" t="n">
+        <v>3379553714.10095</v>
+      </c>
+      <c r="AJ20" s="12" t="n">
         <v>13768679.6233095</v>
       </c>
-      <c r="AK20" s="3" t="n">
+      <c r="AK20" s="12" t="n">
         <v>291121.503866934</v>
       </c>
-      <c r="AL20" s="3" t="n">
+      <c r="AL20" s="12" t="n">
         <v>-7578537.27282939</v>
       </c>
-      <c r="AM20" s="3" t="n">
+      <c r="AM20" s="12" t="n">
         <v>-4926677.66847769</v>
       </c>
-      <c r="AN20" s="3" t="n">
+      <c r="AN20" s="12" t="n">
         <v>-2143749.02223787</v>
       </c>
-      <c r="AO20" s="3" t="n">
+      <c r="AO20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AP20" s="3" t="n">
+      <c r="AP20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AQ20" s="3" t="n">
+      <c r="AQ20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AR20" s="3" t="n">
+      <c r="AR20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AS20" s="3" t="n">
+      <c r="AS20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AT20" s="3" t="n">
+      <c r="AT20" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AU20" s="3"/>
-      <c r="AV20" s="3"/>
-      <c r="AW20" s="3"/>
-      <c r="AX20" s="3"/>
+      <c r="AU20" s="12"/>
+      <c r="AV20" s="12"/>
+      <c r="AW20" s="12"/>
+      <c r="AX20" s="12"/>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -8161,109 +8164,109 @@
         <v>60</v>
       </c>
       <c r="O21"/>
-      <c r="P21" s="3" t="n">
+      <c r="P21" s="12" t="n">
         <v>61574219146.1011</v>
       </c>
-      <c r="Q21" s="3" t="n">
+      <c r="Q21" s="12" t="n">
         <v>58557064802.4477</v>
       </c>
-      <c r="R21" s="3" t="n">
+      <c r="R21" s="12" t="n">
         <v>56801379064.5588</v>
       </c>
-      <c r="S21" s="3" t="n">
+      <c r="S21" s="12" t="n">
         <v>54729508899.5979</v>
       </c>
-      <c r="T21" s="3" t="n">
+      <c r="T21" s="12" t="n">
         <v>54688352602.1809</v>
       </c>
-      <c r="U21" s="3" t="n">
+      <c r="U21" s="12" t="n">
         <v>47012064374.5043</v>
       </c>
-      <c r="V21" s="3" t="n">
+      <c r="V21" s="12" t="n">
         <v>49656147326.0405</v>
       </c>
-      <c r="W21" s="3" t="n">
+      <c r="W21" s="12" t="n">
         <v>42152791540.17</v>
       </c>
-      <c r="X21" s="3" t="n">
+      <c r="X21" s="12" t="n">
         <v>44303062515.0653</v>
       </c>
-      <c r="Y21" s="3" t="n">
+      <c r="Y21" s="12" t="n">
         <v>45432730399.186</v>
       </c>
-      <c r="Z21" s="3" t="n">
+      <c r="Z21" s="12" t="n">
         <v>1883108552.16094</v>
       </c>
-      <c r="AA21" s="3" t="n">
+      <c r="AA21" s="12" t="n">
         <v>129655403.210666</v>
       </c>
-      <c r="AB21" s="3" t="n">
-        <v>205769202.437913</v>
-      </c>
-      <c r="AC21" s="3" t="n">
+      <c r="AB21" s="12" t="n">
+        <v>205769202.437758</v>
+      </c>
+      <c r="AC21" s="12" t="n">
         <v>257016003.130769</v>
       </c>
-      <c r="AD21" s="3" t="n">
+      <c r="AD21" s="12" t="n">
         <v>284081906.561755</v>
       </c>
-      <c r="AE21" s="3" t="n">
+      <c r="AE21" s="12" t="n">
         <v>254347287.16124</v>
       </c>
-      <c r="AF21" s="3" t="n">
+      <c r="AF21" s="12" t="n">
         <v>93204512.7596402</v>
       </c>
-      <c r="AG21" s="3" t="n">
-        <v>16138072.5691724</v>
-      </c>
-      <c r="AH21" s="3" t="n">
-        <v>1458190475.1103</v>
-      </c>
-      <c r="AI21" s="3" t="n">
-        <v>2272323098.55858</v>
-      </c>
-      <c r="AJ21" s="3" t="n">
+      <c r="AG21" s="12" t="n">
+        <v>16138072.556789</v>
+      </c>
+      <c r="AH21" s="12" t="n">
+        <v>1458190469.3746</v>
+      </c>
+      <c r="AI21" s="12" t="n">
+        <v>2272323088.49856</v>
+      </c>
+      <c r="AJ21" s="12" t="n">
         <v>1126214460.44692</v>
       </c>
-      <c r="AK21" s="3" t="n">
+      <c r="AK21" s="12" t="n">
         <v>1812763011.18012</v>
       </c>
-      <c r="AL21" s="3" t="n">
+      <c r="AL21" s="12" t="n">
         <v>3951923321.90102</v>
       </c>
-      <c r="AM21" s="3" t="n">
+      <c r="AM21" s="12" t="n">
         <v>181287982.68239</v>
       </c>
-      <c r="AN21" s="3" t="n">
+      <c r="AN21" s="12" t="n">
         <v>169338080.11077</v>
       </c>
-      <c r="AO21" s="3" t="n">
+      <c r="AO21" s="12" t="n">
         <v>290753493.787097</v>
       </c>
-      <c r="AP21" s="3" t="n">
+      <c r="AP21" s="12" t="n">
         <v>534367944.916519</v>
       </c>
-      <c r="AQ21" s="3" t="n">
+      <c r="AQ21" s="12" t="n">
         <v>-14258218.3023654</v>
       </c>
-      <c r="AR21" s="3" t="n">
+      <c r="AR21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AS21" s="3" t="n">
+      <c r="AS21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AT21" s="3" t="n">
+      <c r="AT21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AU21" s="3" t="n">
+      <c r="AU21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AV21" s="3" t="n">
+      <c r="AV21" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AW21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX21" s="3"/>
+      <c r="AW21" s="12" t="n">
+        <v>-37508.0728183363</v>
+      </c>
+      <c r="AX21" s="12"/>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -8272,41 +8275,41 @@
       <c r="B22" t="str">
         <f>O22</f>
       </c>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
-      <c r="AG22" s="3"/>
-      <c r="AH22" s="3"/>
-      <c r="AI22" s="3"/>
-      <c r="AJ22" s="3"/>
-      <c r="AK22" s="3"/>
-      <c r="AL22" s="3"/>
-      <c r="AM22" s="3"/>
-      <c r="AN22" s="3"/>
-      <c r="AO22" s="3"/>
-      <c r="AP22" s="3"/>
-      <c r="AQ22" s="3"/>
-      <c r="AR22" s="3"/>
-      <c r="AS22" s="3"/>
-      <c r="AT22" s="3"/>
-      <c r="AU22" s="3"/>
-      <c r="AV22" s="3"/>
-      <c r="AW22" s="3"/>
-      <c r="AX22" s="3"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="12"/>
+      <c r="AD22" s="12"/>
+      <c r="AE22" s="12"/>
+      <c r="AF22" s="12"/>
+      <c r="AG22" s="12"/>
+      <c r="AH22" s="12"/>
+      <c r="AI22" s="12"/>
+      <c r="AJ22" s="12"/>
+      <c r="AK22" s="12"/>
+      <c r="AL22" s="12"/>
+      <c r="AM22" s="12"/>
+      <c r="AN22" s="12"/>
+      <c r="AO22" s="12"/>
+      <c r="AP22" s="12"/>
+      <c r="AQ22" s="12"/>
+      <c r="AR22" s="12"/>
+      <c r="AS22" s="12"/>
+      <c r="AT22" s="12"/>
+      <c r="AU22" s="12"/>
+      <c r="AV22" s="12"/>
+      <c r="AW22" s="12"/>
+      <c r="AX22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>